<commit_message>
Google Sheet data request Optimization: 1.Limit the number of calls per project. 2.Delay the requests to reduce number of calls per second.
</commit_message>
<xml_diff>
--- a/WICR Estimator/SummaryTemplate.xlsx
+++ b/WICR Estimator/SummaryTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Freelancer Projects\Amin_WICr Estimator\WICR Estimator_08-10-18\WICR Estimator_08-10-18\WICR Estimator\WICR Estimator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A839DE8-FB88-4538-A219-CF0E4500A3BF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3160B1FF-9C45-486F-BEB2-2EE0B6D2AAE3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="347" xr2:uid="{C3BB3D69-FD31-4C45-AAE2-714CBD52CC32}"/>
   </bookViews>
@@ -281,18 +281,12 @@
     <t>Mat Pricing</t>
   </si>
   <si>
-    <t>SP Mat Pricing</t>
-  </si>
-  <si>
     <t>Manual Override</t>
   </si>
   <si>
     <t>Mat Price</t>
   </si>
   <si>
-    <t>SP Pricing</t>
-  </si>
-  <si>
     <t>Labor Hours</t>
   </si>
   <si>
@@ -396,6 +390,12 @@
   </si>
   <si>
     <t>Total Other Labor Cost</t>
+  </si>
+  <si>
+    <t>MAT EXTENSION</t>
+  </si>
+  <si>
+    <t>Urethane Slope</t>
   </si>
 </sst>
 </file>
@@ -1417,7 +1417,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyProtection="1"/>
@@ -1512,41 +1512,260 @@
     <xf numFmtId="2" fontId="3" fillId="3" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="53" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="52" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="54" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="55" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="68" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="69" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="70" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="56" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="57" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="58" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="63" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="64" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="65" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="66" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="60" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="61" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="5" fillId="5" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="5" fillId="5" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="48" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1578,212 +1797,11 @@
     <xf numFmtId="2" fontId="4" fillId="4" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="4" fillId="5" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="5" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="5" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="5" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="48" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="52" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="53" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="56" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="57" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="58" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="4" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="4" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="63" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="64" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="65" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="66" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="60" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="61" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="54" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="55" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="68" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="69" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="70" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2225,7 +2243,7 @@
   <dimension ref="A1:BD219"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:D10"/>
+      <selection activeCell="A16" sqref="A16:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2271,35 +2289,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="134" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="54"/>
-      <c r="G1" s="64" t="s">
+      <c r="B1" s="135"/>
+      <c r="C1" s="135"/>
+      <c r="D1" s="135"/>
+      <c r="E1" s="136"/>
+      <c r="G1" s="137" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="66"/>
+      <c r="H1" s="138"/>
+      <c r="I1" s="138"/>
+      <c r="J1" s="138"/>
+      <c r="K1" s="138"/>
+      <c r="L1" s="139"/>
     </row>
     <row r="2" spans="1:32" ht="12.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="140" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="69"/>
+      <c r="B2" s="141"/>
+      <c r="C2" s="141"/>
+      <c r="D2" s="141"/>
+      <c r="E2" s="142"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="70" t="s">
-        <v>86</v>
-      </c>
-      <c r="H2" s="71"/>
+      <c r="G2" s="143" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" s="144"/>
       <c r="I2" s="29" t="s">
         <v>55</v>
       </c>
@@ -2310,58 +2328,58 @@
         <v>77</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>78</v>
+        <v>115</v>
       </c>
       <c r="P2" s="5"/>
       <c r="AA2" s="5"/>
       <c r="AF2" s="5"/>
     </row>
     <row r="3" spans="1:32" s="9" customFormat="1" ht="12.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="145" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="31"/>
+      <c r="B3" s="146"/>
+      <c r="C3" s="146"/>
+      <c r="D3" s="146"/>
+      <c r="E3" s="54"/>
       <c r="F3" s="7"/>
-      <c r="G3" s="74" t="s">
+      <c r="G3" s="131" t="s">
         <v>67</v>
       </c>
-      <c r="H3" s="75"/>
+      <c r="H3" s="132"/>
       <c r="I3" s="32"/>
       <c r="J3" s="32"/>
       <c r="K3" s="32"/>
       <c r="L3" s="33"/>
     </row>
     <row r="4" spans="1:32" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="80" t="s">
+      <c r="A4" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="81"/>
-      <c r="C4" s="81"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="10"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="55"/>
       <c r="F4" s="7"/>
-      <c r="G4" s="82" t="s">
+      <c r="G4" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="83"/>
+      <c r="H4" s="75"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
       <c r="L4" s="26"/>
     </row>
     <row r="5" spans="1:32" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="76" t="s">
+      <c r="A5" s="133" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="77"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="12"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="56"/>
       <c r="F5" s="7"/>
-      <c r="G5" s="78" t="s">
+      <c r="G5" s="77" t="s">
         <v>68</v>
       </c>
       <c r="H5" s="79"/>
@@ -2371,33 +2389,33 @@
       <c r="L5" s="27"/>
     </row>
     <row r="6" spans="1:32" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="80" t="s">
+      <c r="A6" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="81"/>
-      <c r="C6" s="81"/>
-      <c r="D6" s="81"/>
-      <c r="E6" s="10"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="69"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="55"/>
       <c r="F6" s="7"/>
-      <c r="G6" s="82" t="s">
+      <c r="G6" s="74" t="s">
         <v>69</v>
       </c>
-      <c r="H6" s="83"/>
+      <c r="H6" s="75"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
       <c r="L6" s="26"/>
     </row>
     <row r="7" spans="1:32" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="61" t="s">
+      <c r="A7" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="62"/>
-      <c r="C7" s="63"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="60"/>
       <c r="D7" s="13"/>
-      <c r="E7" s="12"/>
+      <c r="E7" s="56"/>
       <c r="F7" s="7"/>
-      <c r="G7" s="78" t="s">
+      <c r="G7" s="77" t="s">
         <v>70</v>
       </c>
       <c r="H7" s="79"/>
@@ -2407,33 +2425,33 @@
       <c r="L7" s="27"/>
     </row>
     <row r="8" spans="1:32" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="80" t="s">
+      <c r="A8" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="81"/>
-      <c r="C8" s="81"/>
-      <c r="D8" s="81"/>
-      <c r="E8" s="10"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="55"/>
       <c r="F8" s="7"/>
-      <c r="G8" s="82" t="s">
+      <c r="G8" s="74" t="s">
         <v>71</v>
       </c>
-      <c r="H8" s="83"/>
+      <c r="H8" s="75"/>
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
       <c r="L8" s="26"/>
     </row>
     <row r="9" spans="1:32" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="76" t="s">
+      <c r="A9" s="133" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="77"/>
-      <c r="C9" s="77"/>
-      <c r="D9" s="77"/>
-      <c r="E9" s="12"/>
+      <c r="B9" s="70"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="56"/>
       <c r="F9" s="7"/>
-      <c r="G9" s="78" t="s">
+      <c r="G9" s="77" t="s">
         <v>72</v>
       </c>
       <c r="H9" s="79"/>
@@ -2443,33 +2461,33 @@
       <c r="L9" s="27"/>
     </row>
     <row r="10" spans="1:32" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="80" t="s">
+      <c r="A10" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="81"/>
-      <c r="C10" s="81"/>
-      <c r="D10" s="81"/>
-      <c r="E10" s="10"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="55"/>
       <c r="F10" s="7"/>
-      <c r="G10" s="82" t="s">
+      <c r="G10" s="74" t="s">
         <v>73</v>
       </c>
-      <c r="H10" s="83"/>
+      <c r="H10" s="75"/>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
       <c r="L10" s="26"/>
     </row>
     <row r="11" spans="1:32" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="76" t="s">
+      <c r="A11" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="77"/>
-      <c r="C11" s="77"/>
-      <c r="D11" s="77"/>
-      <c r="E11" s="12"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="56"/>
       <c r="F11" s="7"/>
-      <c r="G11" s="78" t="s">
+      <c r="G11" s="77" t="s">
         <v>26</v>
       </c>
       <c r="H11" s="79"/>
@@ -2479,33 +2497,33 @@
       <c r="L11" s="27"/>
     </row>
     <row r="12" spans="1:32" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="80" t="s">
+      <c r="A12" s="68" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="81"/>
-      <c r="C12" s="81"/>
-      <c r="D12" s="81"/>
-      <c r="E12" s="10"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="55"/>
       <c r="F12" s="7"/>
-      <c r="G12" s="82" t="s">
+      <c r="G12" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="83"/>
+      <c r="H12" s="75"/>
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
       <c r="L12" s="26"/>
     </row>
     <row r="13" spans="1:32" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="61" t="s">
+      <c r="A13" s="58" t="s">
         <v>65</v>
       </c>
-      <c r="B13" s="62"/>
-      <c r="C13" s="62"/>
-      <c r="D13" s="63"/>
-      <c r="E13" s="12"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="56"/>
       <c r="F13" s="7"/>
-      <c r="G13" s="78" t="s">
+      <c r="G13" s="77" t="s">
         <v>28</v>
       </c>
       <c r="H13" s="79"/>
@@ -2515,33 +2533,33 @@
       <c r="L13" s="27"/>
     </row>
     <row r="14" spans="1:32" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="84" t="s">
+      <c r="A14" s="147" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="85"/>
-      <c r="C14" s="85"/>
-      <c r="D14" s="85"/>
-      <c r="E14" s="34"/>
+      <c r="B14" s="148"/>
+      <c r="C14" s="148"/>
+      <c r="D14" s="148"/>
+      <c r="E14" s="57"/>
       <c r="F14" s="7"/>
-      <c r="G14" s="82" t="s">
+      <c r="G14" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="H14" s="83"/>
+      <c r="H14" s="75"/>
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
       <c r="K14" s="11"/>
       <c r="L14" s="26"/>
     </row>
     <row r="15" spans="1:32" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="76" t="s">
-        <v>83</v>
-      </c>
-      <c r="B15" s="77"/>
-      <c r="C15" s="77"/>
-      <c r="D15" s="77"/>
-      <c r="E15" s="12"/>
+      <c r="A15" s="133" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" s="70"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="56"/>
       <c r="F15" s="7"/>
-      <c r="G15" s="78" t="s">
+      <c r="G15" s="77" t="s">
         <v>30</v>
       </c>
       <c r="H15" s="79"/>
@@ -2551,33 +2569,33 @@
       <c r="L15" s="27"/>
     </row>
     <row r="16" spans="1:32" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="80" t="s">
-        <v>84</v>
-      </c>
-      <c r="B16" s="81"/>
-      <c r="C16" s="81"/>
-      <c r="D16" s="81"/>
-      <c r="E16" s="10"/>
+      <c r="A16" s="68" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" s="69"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="55"/>
       <c r="F16" s="7"/>
-      <c r="G16" s="82" t="s">
+      <c r="G16" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="H16" s="83"/>
+      <c r="H16" s="75"/>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
       <c r="K16" s="11"/>
       <c r="L16" s="26"/>
     </row>
     <row r="17" spans="1:12" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="76" t="s">
-        <v>85</v>
-      </c>
-      <c r="B17" s="77"/>
-      <c r="C17" s="77"/>
-      <c r="D17" s="77"/>
-      <c r="E17" s="12"/>
+      <c r="A17" s="133" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" s="70"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="56"/>
       <c r="F17" s="7"/>
-      <c r="G17" s="78" t="s">
+      <c r="G17" s="77" t="s">
         <v>32</v>
       </c>
       <c r="H17" s="79"/>
@@ -2587,29 +2605,29 @@
       <c r="L17" s="27"/>
     </row>
     <row r="18" spans="1:12" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="80"/>
-      <c r="B18" s="81"/>
-      <c r="C18" s="81"/>
-      <c r="D18" s="81"/>
-      <c r="E18" s="10"/>
+      <c r="A18" s="68"/>
+      <c r="B18" s="69"/>
+      <c r="C18" s="69"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="55"/>
       <c r="F18" s="7"/>
-      <c r="G18" s="82" t="s">
+      <c r="G18" s="74" t="s">
         <v>33</v>
       </c>
-      <c r="H18" s="83"/>
+      <c r="H18" s="75"/>
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
       <c r="K18" s="11"/>
       <c r="L18" s="26"/>
     </row>
     <row r="19" spans="1:12" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="77"/>
-      <c r="B19" s="77"/>
-      <c r="C19" s="77"/>
-      <c r="D19" s="77"/>
-      <c r="E19" s="13"/>
+      <c r="A19" s="70"/>
+      <c r="B19" s="70"/>
+      <c r="C19" s="70"/>
+      <c r="D19" s="70"/>
+      <c r="E19" s="52"/>
       <c r="F19" s="7"/>
-      <c r="G19" s="78" t="s">
+      <c r="G19" s="77" t="s">
         <v>74</v>
       </c>
       <c r="H19" s="79"/>
@@ -2619,60 +2637,60 @@
       <c r="L19" s="27"/>
     </row>
     <row r="20" spans="1:12" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="81"/>
-      <c r="B20" s="81"/>
-      <c r="C20" s="81"/>
-      <c r="D20" s="81"/>
-      <c r="E20" s="11"/>
+      <c r="A20" s="69"/>
+      <c r="B20" s="69"/>
+      <c r="C20" s="69"/>
+      <c r="D20" s="69"/>
+      <c r="E20" s="53"/>
       <c r="F20" s="7"/>
-      <c r="G20" s="82" t="s">
+      <c r="G20" s="74" t="s">
         <v>75</v>
       </c>
-      <c r="H20" s="83"/>
+      <c r="H20" s="75"/>
       <c r="I20" s="11"/>
       <c r="J20" s="11"/>
       <c r="K20" s="11"/>
       <c r="L20" s="26"/>
     </row>
     <row r="21" spans="1:12" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="77"/>
-      <c r="B21" s="77"/>
-      <c r="C21" s="77"/>
-      <c r="D21" s="77"/>
-      <c r="E21" s="13"/>
+      <c r="A21" s="70"/>
+      <c r="B21" s="70"/>
+      <c r="C21" s="70"/>
+      <c r="D21" s="70"/>
+      <c r="E21" s="52"/>
       <c r="F21" s="7"/>
-      <c r="G21" s="86" t="s">
+      <c r="G21" s="61" t="s">
         <v>76</v>
       </c>
-      <c r="H21" s="87"/>
+      <c r="H21" s="62"/>
       <c r="I21" s="13"/>
       <c r="J21" s="13"/>
       <c r="K21" s="13"/>
       <c r="L21" s="27"/>
     </row>
     <row r="22" spans="1:12" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="81"/>
-      <c r="B22" s="81"/>
-      <c r="C22" s="81"/>
-      <c r="D22" s="81"/>
-      <c r="E22" s="11"/>
-      <c r="G22" s="82" t="s">
-        <v>87</v>
-      </c>
-      <c r="H22" s="83"/>
+      <c r="A22" s="69"/>
+      <c r="B22" s="69"/>
+      <c r="C22" s="69"/>
+      <c r="D22" s="69"/>
+      <c r="E22" s="53"/>
+      <c r="G22" s="74" t="s">
+        <v>85</v>
+      </c>
+      <c r="H22" s="75"/>
       <c r="I22" s="11"/>
       <c r="J22" s="11"/>
       <c r="K22" s="11"/>
       <c r="L22" s="26"/>
     </row>
     <row r="23" spans="1:12" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="77"/>
-      <c r="B23" s="77"/>
-      <c r="C23" s="77"/>
-      <c r="D23" s="77"/>
-      <c r="E23" s="13"/>
-      <c r="G23" s="78" t="s">
-        <v>88</v>
+      <c r="A23" s="70"/>
+      <c r="B23" s="70"/>
+      <c r="C23" s="70"/>
+      <c r="D23" s="70"/>
+      <c r="E23" s="52"/>
+      <c r="G23" s="77" t="s">
+        <v>86</v>
       </c>
       <c r="H23" s="79"/>
       <c r="I23" s="13"/>
@@ -2681,23 +2699,23 @@
       <c r="L23" s="27"/>
     </row>
     <row r="24" spans="1:12" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="81"/>
-      <c r="B24" s="81"/>
-      <c r="C24" s="81"/>
-      <c r="D24" s="81"/>
-      <c r="E24" s="11"/>
-      <c r="G24" s="82" t="s">
-        <v>89</v>
-      </c>
-      <c r="H24" s="83"/>
+      <c r="A24" s="69"/>
+      <c r="B24" s="69"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="53"/>
+      <c r="G24" s="74" t="s">
+        <v>87</v>
+      </c>
+      <c r="H24" s="75"/>
       <c r="I24" s="11"/>
       <c r="J24" s="11"/>
       <c r="K24" s="11"/>
       <c r="L24" s="26"/>
     </row>
     <row r="25" spans="1:12" s="9" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G25" s="78" t="s">
-        <v>90</v>
+      <c r="G25" s="77" t="s">
+        <v>88</v>
       </c>
       <c r="H25" s="79"/>
       <c r="I25" s="13"/>
@@ -2706,27 +2724,27 @@
       <c r="L25" s="27"/>
     </row>
     <row r="26" spans="1:12" s="9" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="52" t="s">
+      <c r="A26" s="134" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="53"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="54"/>
-      <c r="G26" s="82" t="s">
-        <v>91</v>
-      </c>
-      <c r="H26" s="83"/>
+      <c r="B26" s="135"/>
+      <c r="C26" s="135"/>
+      <c r="D26" s="135"/>
+      <c r="E26" s="136"/>
+      <c r="G26" s="74" t="s">
+        <v>89</v>
+      </c>
+      <c r="H26" s="75"/>
       <c r="I26" s="11"/>
       <c r="J26" s="11"/>
       <c r="K26" s="11"/>
       <c r="L26" s="26"/>
     </row>
     <row r="27" spans="1:12" s="9" customFormat="1" ht="12.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="55" t="s">
+      <c r="A27" s="113" t="s">
         <v>56</v>
       </c>
-      <c r="B27" s="56"/>
+      <c r="B27" s="111"/>
       <c r="C27" s="29" t="s">
         <v>55</v>
       </c>
@@ -2736,8 +2754,8 @@
       <c r="E27" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G27" s="78" t="s">
-        <v>92</v>
+      <c r="G27" s="77" t="s">
+        <v>90</v>
       </c>
       <c r="H27" s="79"/>
       <c r="I27" s="13"/>
@@ -2746,36 +2764,36 @@
       <c r="L27" s="27"/>
     </row>
     <row r="28" spans="1:12" s="9" customFormat="1" ht="12.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="74" t="s">
-        <v>105</v>
-      </c>
-      <c r="B28" s="75"/>
+      <c r="A28" s="131" t="s">
+        <v>103</v>
+      </c>
+      <c r="B28" s="132"/>
       <c r="C28" s="8" t="s">
         <v>66</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="6"/>
-      <c r="G28" s="82" t="s">
-        <v>93</v>
-      </c>
-      <c r="H28" s="83"/>
+      <c r="G28" s="74" t="s">
+        <v>91</v>
+      </c>
+      <c r="H28" s="75"/>
       <c r="I28" s="11"/>
       <c r="J28" s="11"/>
       <c r="K28" s="11"/>
       <c r="L28" s="26"/>
     </row>
     <row r="29" spans="1:12" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="82" t="s">
-        <v>106</v>
-      </c>
-      <c r="B29" s="83"/>
+      <c r="A29" s="74" t="s">
+        <v>104</v>
+      </c>
+      <c r="B29" s="75"/>
       <c r="C29" s="11" t="s">
         <v>66</v>
       </c>
       <c r="D29" s="11"/>
       <c r="E29" s="10"/>
-      <c r="G29" s="78" t="s">
-        <v>94</v>
+      <c r="G29" s="77" t="s">
+        <v>92</v>
       </c>
       <c r="H29" s="79"/>
       <c r="I29" s="13"/>
@@ -2784,8 +2802,8 @@
       <c r="L29" s="27"/>
     </row>
     <row r="30" spans="1:12" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="78" t="s">
-        <v>107</v>
+      <c r="A30" s="77" t="s">
+        <v>105</v>
       </c>
       <c r="B30" s="79"/>
       <c r="C30" s="13" t="s">
@@ -2794,24 +2812,24 @@
       <c r="D30" s="13"/>
       <c r="E30" s="12"/>
       <c r="F30" s="7"/>
-      <c r="G30" s="82" t="s">
-        <v>95</v>
-      </c>
-      <c r="H30" s="83"/>
+      <c r="G30" s="74" t="s">
+        <v>93</v>
+      </c>
+      <c r="H30" s="75"/>
       <c r="I30" s="11"/>
       <c r="J30" s="11"/>
       <c r="K30" s="11"/>
       <c r="L30" s="26"/>
     </row>
     <row r="31" spans="1:12" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="82"/>
-      <c r="B31" s="83"/>
+      <c r="A31" s="74"/>
+      <c r="B31" s="75"/>
       <c r="C31" s="11"/>
       <c r="D31" s="11"/>
       <c r="E31" s="10"/>
       <c r="F31" s="7"/>
-      <c r="G31" s="78" t="s">
-        <v>96</v>
+      <c r="G31" s="77" t="s">
+        <v>94</v>
       </c>
       <c r="H31" s="79"/>
       <c r="I31" s="13"/>
@@ -2820,30 +2838,30 @@
       <c r="L31" s="27"/>
     </row>
     <row r="32" spans="1:12" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="78"/>
+      <c r="A32" s="77"/>
       <c r="B32" s="79"/>
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>
       <c r="E32" s="12"/>
       <c r="F32" s="7"/>
-      <c r="G32" s="82" t="s">
-        <v>97</v>
-      </c>
-      <c r="H32" s="83"/>
+      <c r="G32" s="74" t="s">
+        <v>95</v>
+      </c>
+      <c r="H32" s="75"/>
       <c r="I32" s="11"/>
       <c r="J32" s="11"/>
       <c r="K32" s="11"/>
       <c r="L32" s="26"/>
     </row>
     <row r="33" spans="1:56" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="82"/>
-      <c r="B33" s="83"/>
+      <c r="A33" s="74"/>
+      <c r="B33" s="75"/>
       <c r="C33" s="11"/>
       <c r="D33" s="11"/>
       <c r="E33" s="10"/>
       <c r="F33" s="7"/>
-      <c r="G33" s="78" t="s">
-        <v>98</v>
+      <c r="G33" s="77" t="s">
+        <v>96</v>
       </c>
       <c r="H33" s="79"/>
       <c r="I33" s="13"/>
@@ -2852,30 +2870,30 @@
       <c r="L33" s="27"/>
     </row>
     <row r="34" spans="1:56" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="78"/>
+      <c r="A34" s="77"/>
       <c r="B34" s="79"/>
       <c r="C34" s="13"/>
       <c r="D34" s="13"/>
       <c r="E34" s="12"/>
       <c r="F34" s="7"/>
-      <c r="G34" s="82" t="s">
-        <v>99</v>
-      </c>
-      <c r="H34" s="83"/>
+      <c r="G34" s="74" t="s">
+        <v>97</v>
+      </c>
+      <c r="H34" s="75"/>
       <c r="I34" s="11"/>
       <c r="J34" s="11"/>
       <c r="K34" s="11"/>
       <c r="L34" s="26"/>
     </row>
     <row r="35" spans="1:56" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="96"/>
-      <c r="B35" s="96"/>
+      <c r="A35" s="64"/>
+      <c r="B35" s="64"/>
       <c r="C35" s="11"/>
       <c r="D35" s="11"/>
       <c r="E35" s="12"/>
       <c r="F35" s="7"/>
-      <c r="G35" s="78" t="s">
-        <v>100</v>
+      <c r="G35" s="77" t="s">
+        <v>98</v>
       </c>
       <c r="H35" s="79"/>
       <c r="I35" s="13"/>
@@ -2884,30 +2902,30 @@
       <c r="L35" s="27"/>
     </row>
     <row r="36" spans="1:56" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="87"/>
-      <c r="B36" s="87"/>
+      <c r="A36" s="62"/>
+      <c r="B36" s="62"/>
       <c r="C36" s="13"/>
       <c r="D36" s="13"/>
       <c r="E36" s="12"/>
       <c r="F36" s="7"/>
-      <c r="G36" s="82" t="s">
-        <v>101</v>
-      </c>
-      <c r="H36" s="83"/>
+      <c r="G36" s="74" t="s">
+        <v>99</v>
+      </c>
+      <c r="H36" s="75"/>
       <c r="I36" s="11"/>
       <c r="J36" s="11"/>
       <c r="K36" s="11"/>
       <c r="L36" s="26"/>
     </row>
     <row r="37" spans="1:56" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="87"/>
-      <c r="B37" s="87"/>
+      <c r="A37" s="62"/>
+      <c r="B37" s="62"/>
       <c r="C37" s="13"/>
       <c r="D37" s="13"/>
       <c r="E37" s="12"/>
       <c r="F37" s="7"/>
-      <c r="G37" s="78" t="s">
-        <v>102</v>
+      <c r="G37" s="77" t="s">
+        <v>100</v>
       </c>
       <c r="H37" s="79"/>
       <c r="I37" s="13"/>
@@ -2925,16 +2943,16 @@
       <c r="AS37" s="5"/>
     </row>
     <row r="38" spans="1:56" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="87"/>
-      <c r="B38" s="87"/>
+      <c r="A38" s="62"/>
+      <c r="B38" s="62"/>
       <c r="C38" s="13"/>
       <c r="D38" s="13"/>
       <c r="E38" s="12"/>
       <c r="F38" s="7"/>
-      <c r="G38" s="82" t="s">
-        <v>103</v>
-      </c>
-      <c r="H38" s="83"/>
+      <c r="G38" s="74" t="s">
+        <v>101</v>
+      </c>
+      <c r="H38" s="75"/>
       <c r="I38" s="11"/>
       <c r="J38" s="11"/>
       <c r="K38" s="11"/>
@@ -2950,16 +2968,16 @@
       <c r="AS38" s="5"/>
     </row>
     <row r="39" spans="1:56" s="9" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="96"/>
-      <c r="B39" s="96"/>
+      <c r="A39" s="64"/>
+      <c r="B39" s="64"/>
       <c r="C39" s="11"/>
       <c r="D39" s="11"/>
       <c r="E39" s="12"/>
       <c r="F39" s="7"/>
-      <c r="G39" s="97" t="s">
-        <v>104</v>
-      </c>
-      <c r="H39" s="98"/>
+      <c r="G39" s="123" t="s">
+        <v>102</v>
+      </c>
+      <c r="H39" s="124"/>
       <c r="I39" s="20"/>
       <c r="J39" s="20"/>
       <c r="K39" s="20"/>
@@ -2979,7 +2997,7 @@
       <c r="AS39" s="5"/>
     </row>
     <row r="40" spans="1:56" s="9" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="78"/>
+      <c r="A40" s="77"/>
       <c r="B40" s="79"/>
       <c r="C40" s="13"/>
       <c r="D40" s="13"/>
@@ -3010,32 +3028,32 @@
       <c r="BD40" s="5"/>
     </row>
     <row r="41" spans="1:56" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="82"/>
-      <c r="B41" s="83"/>
+      <c r="A41" s="74"/>
+      <c r="B41" s="75"/>
       <c r="C41" s="11"/>
       <c r="D41" s="11"/>
       <c r="E41" s="10"/>
       <c r="F41" s="7"/>
-      <c r="G41" s="52" t="s">
+      <c r="G41" s="134" t="s">
         <v>5</v>
       </c>
-      <c r="H41" s="53"/>
-      <c r="I41" s="53"/>
-      <c r="J41" s="53"/>
-      <c r="K41" s="53"/>
-      <c r="L41" s="54"/>
+      <c r="H41" s="135"/>
+      <c r="I41" s="135"/>
+      <c r="J41" s="135"/>
+      <c r="K41" s="135"/>
+      <c r="L41" s="136"/>
     </row>
     <row r="42" spans="1:56" s="5" customFormat="1" ht="12.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="78"/>
+      <c r="A42" s="77"/>
       <c r="B42" s="79"/>
       <c r="C42" s="13"/>
       <c r="D42" s="13"/>
       <c r="E42" s="12"/>
       <c r="F42" s="7"/>
-      <c r="G42" s="55" t="s">
+      <c r="G42" s="113" t="s">
         <v>47</v>
       </c>
-      <c r="H42" s="56"/>
+      <c r="H42" s="111"/>
       <c r="I42" s="51" t="s">
         <v>43</v>
       </c>
@@ -3043,35 +3061,35 @@
         <v>34</v>
       </c>
       <c r="K42" s="51" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L42" s="4" t="s">
-        <v>81</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:56" s="5" customFormat="1" ht="12.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="106"/>
-      <c r="B43" s="107"/>
+      <c r="A43" s="129"/>
+      <c r="B43" s="130"/>
       <c r="C43" s="35"/>
       <c r="D43" s="35"/>
       <c r="E43" s="34"/>
       <c r="F43" s="7"/>
-      <c r="G43" s="99"/>
-      <c r="H43" s="100"/>
+      <c r="G43" s="125"/>
+      <c r="H43" s="126"/>
       <c r="I43" s="8"/>
       <c r="J43" s="8"/>
       <c r="K43" s="32"/>
       <c r="L43" s="25"/>
     </row>
     <row r="44" spans="1:56" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="97"/>
-      <c r="B44" s="98"/>
+      <c r="A44" s="123"/>
+      <c r="B44" s="124"/>
       <c r="C44" s="20"/>
       <c r="D44" s="20"/>
       <c r="E44" s="14"/>
       <c r="F44" s="7"/>
-      <c r="G44" s="59"/>
-      <c r="H44" s="60"/>
+      <c r="G44" s="85"/>
+      <c r="H44" s="86"/>
       <c r="I44" s="11"/>
       <c r="J44" s="11"/>
       <c r="K44" s="11"/>
@@ -3084,24 +3102,24 @@
       <c r="D45" s="9"/>
       <c r="E45" s="9"/>
       <c r="F45" s="7"/>
-      <c r="G45" s="57"/>
-      <c r="H45" s="58"/>
+      <c r="G45" s="83"/>
+      <c r="H45" s="84"/>
       <c r="I45" s="13"/>
       <c r="J45" s="13"/>
       <c r="K45" s="13"/>
       <c r="L45" s="27"/>
     </row>
     <row r="46" spans="1:56" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="103" t="s">
+      <c r="A46" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B46" s="104"/>
-      <c r="C46" s="104"/>
-      <c r="D46" s="104"/>
-      <c r="E46" s="105"/>
+      <c r="B46" s="72"/>
+      <c r="C46" s="72"/>
+      <c r="D46" s="72"/>
+      <c r="E46" s="73"/>
       <c r="F46" s="3"/>
-      <c r="G46" s="59"/>
-      <c r="H46" s="60"/>
+      <c r="G46" s="85"/>
+      <c r="H46" s="86"/>
       <c r="I46" s="11"/>
       <c r="J46" s="11"/>
       <c r="K46" s="11"/>
@@ -3124,8 +3142,8 @@
         <v>19</v>
       </c>
       <c r="F47" s="3"/>
-      <c r="G47" s="57"/>
-      <c r="H47" s="58"/>
+      <c r="G47" s="83"/>
+      <c r="H47" s="84"/>
       <c r="I47" s="13"/>
       <c r="J47" s="13"/>
       <c r="K47" s="13"/>
@@ -3140,8 +3158,8 @@
       <c r="D48" s="11"/>
       <c r="E48" s="10"/>
       <c r="F48" s="3"/>
-      <c r="G48" s="59"/>
-      <c r="H48" s="60"/>
+      <c r="G48" s="85"/>
+      <c r="H48" s="86"/>
       <c r="I48" s="11"/>
       <c r="J48" s="11"/>
       <c r="K48" s="11"/>
@@ -3156,8 +3174,8 @@
       <c r="D49" s="13"/>
       <c r="E49" s="12"/>
       <c r="F49" s="3"/>
-      <c r="G49" s="57"/>
-      <c r="H49" s="58"/>
+      <c r="G49" s="83"/>
+      <c r="H49" s="84"/>
       <c r="I49" s="13"/>
       <c r="J49" s="13"/>
       <c r="K49" s="13"/>
@@ -3172,8 +3190,8 @@
       <c r="D50" s="11"/>
       <c r="E50" s="10"/>
       <c r="F50" s="3"/>
-      <c r="G50" s="59"/>
-      <c r="H50" s="60"/>
+      <c r="G50" s="85"/>
+      <c r="H50" s="86"/>
       <c r="I50" s="11"/>
       <c r="J50" s="11"/>
       <c r="K50" s="11"/>
@@ -3188,8 +3206,8 @@
       <c r="D51" s="13"/>
       <c r="E51" s="12"/>
       <c r="F51" s="3"/>
-      <c r="G51" s="57"/>
-      <c r="H51" s="58"/>
+      <c r="G51" s="83"/>
+      <c r="H51" s="84"/>
       <c r="I51" s="13"/>
       <c r="J51" s="13"/>
       <c r="K51" s="13"/>
@@ -3204,24 +3222,24 @@
       <c r="D52" s="11"/>
       <c r="E52" s="10"/>
       <c r="F52" s="3"/>
-      <c r="G52" s="59"/>
-      <c r="H52" s="60"/>
+      <c r="G52" s="85"/>
+      <c r="H52" s="86"/>
       <c r="I52" s="11"/>
       <c r="J52" s="11"/>
       <c r="K52" s="11"/>
       <c r="L52" s="26"/>
     </row>
     <row r="53" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="93" t="s">
+      <c r="A53" s="120" t="s">
         <v>14</v>
       </c>
-      <c r="B53" s="94"/>
-      <c r="C53" s="95"/>
+      <c r="B53" s="121"/>
+      <c r="C53" s="122"/>
       <c r="D53" s="30"/>
       <c r="E53" s="17"/>
       <c r="F53" s="3"/>
-      <c r="G53" s="118"/>
-      <c r="H53" s="119"/>
+      <c r="G53" s="116"/>
+      <c r="H53" s="117"/>
       <c r="I53" s="13"/>
       <c r="J53" s="13"/>
       <c r="K53" s="13"/>
@@ -3229,19 +3247,19 @@
     </row>
     <row r="54" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="B54" s="108" t="s">
+        <v>78</v>
+      </c>
+      <c r="B54" s="110" t="s">
         <v>20</v>
       </c>
-      <c r="C54" s="56"/>
-      <c r="D54" s="108" t="s">
-        <v>108</v>
-      </c>
-      <c r="E54" s="109"/>
+      <c r="C54" s="111"/>
+      <c r="D54" s="110" t="s">
+        <v>106</v>
+      </c>
+      <c r="E54" s="112"/>
       <c r="F54" s="3"/>
-      <c r="G54" s="59"/>
-      <c r="H54" s="60"/>
+      <c r="G54" s="85"/>
+      <c r="H54" s="86"/>
       <c r="I54" s="11"/>
       <c r="J54" s="11"/>
       <c r="K54" s="11"/>
@@ -3249,13 +3267,13 @@
     </row>
     <row r="55" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="37"/>
-      <c r="B55" s="110"/>
-      <c r="C55" s="111"/>
-      <c r="D55" s="110"/>
-      <c r="E55" s="112"/>
+      <c r="B55" s="80"/>
+      <c r="C55" s="82"/>
+      <c r="D55" s="80"/>
+      <c r="E55" s="81"/>
       <c r="F55" s="3"/>
-      <c r="G55" s="57"/>
-      <c r="H55" s="58"/>
+      <c r="G55" s="83"/>
+      <c r="H55" s="84"/>
       <c r="I55" s="13"/>
       <c r="J55" s="13"/>
       <c r="K55" s="13"/>
@@ -3263,24 +3281,24 @@
     </row>
     <row r="56" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F56" s="3"/>
-      <c r="G56" s="91"/>
-      <c r="H56" s="92"/>
+      <c r="G56" s="118"/>
+      <c r="H56" s="119"/>
       <c r="I56" s="11"/>
       <c r="J56" s="11"/>
       <c r="K56" s="11"/>
       <c r="L56" s="26"/>
     </row>
     <row r="57" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="103" t="s">
-        <v>2</v>
-      </c>
-      <c r="B57" s="104"/>
-      <c r="C57" s="104"/>
-      <c r="D57" s="104"/>
-      <c r="E57" s="105"/>
+      <c r="A57" s="71" t="s">
+        <v>116</v>
+      </c>
+      <c r="B57" s="72"/>
+      <c r="C57" s="72"/>
+      <c r="D57" s="72"/>
+      <c r="E57" s="73"/>
       <c r="F57" s="3"/>
-      <c r="G57" s="57"/>
-      <c r="H57" s="58"/>
+      <c r="G57" s="83"/>
+      <c r="H57" s="84"/>
       <c r="I57" s="13"/>
       <c r="J57" s="13"/>
       <c r="K57" s="13"/>
@@ -3303,8 +3321,8 @@
         <v>19</v>
       </c>
       <c r="F58" s="3"/>
-      <c r="G58" s="59"/>
-      <c r="H58" s="60"/>
+      <c r="G58" s="85"/>
+      <c r="H58" s="86"/>
       <c r="I58" s="11"/>
       <c r="J58" s="11"/>
       <c r="K58" s="11"/>
@@ -3319,8 +3337,8 @@
       <c r="D59" s="11"/>
       <c r="E59" s="10"/>
       <c r="F59" s="3"/>
-      <c r="G59" s="57"/>
-      <c r="H59" s="58"/>
+      <c r="G59" s="83"/>
+      <c r="H59" s="84"/>
       <c r="I59" s="13"/>
       <c r="J59" s="13"/>
       <c r="K59" s="13"/>
@@ -3335,8 +3353,8 @@
       <c r="D60" s="13"/>
       <c r="E60" s="12"/>
       <c r="F60" s="3"/>
-      <c r="G60" s="59"/>
-      <c r="H60" s="60"/>
+      <c r="G60" s="85"/>
+      <c r="H60" s="86"/>
       <c r="I60" s="11"/>
       <c r="J60" s="11"/>
       <c r="K60" s="11"/>
@@ -3351,8 +3369,8 @@
       <c r="D61" s="11"/>
       <c r="E61" s="10"/>
       <c r="F61" s="3"/>
-      <c r="G61" s="57"/>
-      <c r="H61" s="58"/>
+      <c r="G61" s="83"/>
+      <c r="H61" s="84"/>
       <c r="I61" s="13"/>
       <c r="J61" s="13"/>
       <c r="K61" s="13"/>
@@ -3367,8 +3385,8 @@
       <c r="D62" s="13"/>
       <c r="E62" s="12"/>
       <c r="F62" s="3"/>
-      <c r="G62" s="59"/>
-      <c r="H62" s="60"/>
+      <c r="G62" s="85"/>
+      <c r="H62" s="86"/>
       <c r="I62" s="11"/>
       <c r="J62" s="11"/>
       <c r="K62" s="11"/>
@@ -3383,24 +3401,24 @@
       <c r="D63" s="11"/>
       <c r="E63" s="10"/>
       <c r="F63" s="3"/>
-      <c r="G63" s="57"/>
-      <c r="H63" s="58"/>
+      <c r="G63" s="83"/>
+      <c r="H63" s="84"/>
       <c r="I63" s="13"/>
       <c r="J63" s="13"/>
       <c r="K63" s="13"/>
       <c r="L63" s="27"/>
     </row>
     <row r="64" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="136" t="s">
+      <c r="A64" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="B64" s="137"/>
-      <c r="C64" s="138"/>
+      <c r="B64" s="90"/>
+      <c r="C64" s="91"/>
       <c r="D64" s="30"/>
       <c r="E64" s="17"/>
       <c r="F64" s="3"/>
-      <c r="G64" s="59"/>
-      <c r="H64" s="60"/>
+      <c r="G64" s="85"/>
+      <c r="H64" s="86"/>
       <c r="I64" s="11"/>
       <c r="J64" s="11"/>
       <c r="K64" s="11"/>
@@ -3408,19 +3426,19 @@
     </row>
     <row r="65" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="B65" s="108" t="s">
+        <v>78</v>
+      </c>
+      <c r="B65" s="110" t="s">
         <v>20</v>
       </c>
-      <c r="C65" s="56"/>
-      <c r="D65" s="108" t="s">
-        <v>108</v>
-      </c>
-      <c r="E65" s="109"/>
+      <c r="C65" s="111"/>
+      <c r="D65" s="110" t="s">
+        <v>106</v>
+      </c>
+      <c r="E65" s="112"/>
       <c r="F65" s="3"/>
-      <c r="G65" s="57"/>
-      <c r="H65" s="58"/>
+      <c r="G65" s="83"/>
+      <c r="H65" s="84"/>
       <c r="I65" s="13"/>
       <c r="J65" s="13"/>
       <c r="K65" s="13"/>
@@ -3428,13 +3446,13 @@
     </row>
     <row r="66" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="37"/>
-      <c r="B66" s="110"/>
-      <c r="C66" s="111"/>
-      <c r="D66" s="110"/>
-      <c r="E66" s="112"/>
+      <c r="B66" s="80"/>
+      <c r="C66" s="82"/>
+      <c r="D66" s="80"/>
+      <c r="E66" s="81"/>
       <c r="F66" s="3"/>
-      <c r="G66" s="59"/>
-      <c r="H66" s="60"/>
+      <c r="G66" s="85"/>
+      <c r="H66" s="86"/>
       <c r="I66" s="11"/>
       <c r="J66" s="11"/>
       <c r="K66" s="11"/>
@@ -3442,104 +3460,104 @@
     </row>
     <row r="67" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F67" s="3"/>
-      <c r="G67" s="57"/>
-      <c r="H67" s="58"/>
+      <c r="G67" s="83"/>
+      <c r="H67" s="84"/>
       <c r="I67" s="13"/>
       <c r="J67" s="13"/>
       <c r="K67" s="13"/>
       <c r="L67" s="27"/>
     </row>
     <row r="68" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="88" t="s">
+      <c r="A68" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="B68" s="89"/>
-      <c r="C68" s="89"/>
-      <c r="D68" s="89"/>
-      <c r="E68" s="90"/>
+      <c r="B68" s="96"/>
+      <c r="C68" s="96"/>
+      <c r="D68" s="96"/>
+      <c r="E68" s="97"/>
       <c r="F68" s="3"/>
-      <c r="G68" s="59"/>
-      <c r="H68" s="60"/>
+      <c r="G68" s="85"/>
+      <c r="H68" s="86"/>
       <c r="I68" s="11"/>
       <c r="J68" s="11"/>
       <c r="K68" s="11"/>
       <c r="L68" s="26"/>
     </row>
     <row r="69" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="55" t="s">
+      <c r="A69" s="113" t="s">
         <v>35</v>
       </c>
-      <c r="B69" s="56"/>
+      <c r="B69" s="111"/>
       <c r="C69" s="29" t="s">
         <v>43</v>
       </c>
       <c r="D69" s="29" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E69" s="4" t="s">
         <v>44</v>
       </c>
       <c r="F69" s="3"/>
-      <c r="G69" s="57"/>
-      <c r="H69" s="58"/>
+      <c r="G69" s="83"/>
+      <c r="H69" s="84"/>
       <c r="I69" s="13"/>
       <c r="J69" s="13"/>
       <c r="K69" s="13"/>
       <c r="L69" s="27"/>
     </row>
     <row r="70" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="113"/>
-      <c r="B70" s="114"/>
+      <c r="A70" s="114"/>
+      <c r="B70" s="115"/>
       <c r="C70" s="32"/>
       <c r="D70" s="32"/>
       <c r="E70" s="31"/>
       <c r="F70" s="3"/>
-      <c r="G70" s="59"/>
-      <c r="H70" s="60"/>
+      <c r="G70" s="85"/>
+      <c r="H70" s="86"/>
       <c r="I70" s="11"/>
       <c r="J70" s="11"/>
       <c r="K70" s="11"/>
       <c r="L70" s="26"/>
     </row>
     <row r="71" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="124"/>
-      <c r="B71" s="96"/>
+      <c r="A71" s="63"/>
+      <c r="B71" s="64"/>
       <c r="C71" s="11"/>
       <c r="D71" s="11"/>
       <c r="E71" s="10"/>
       <c r="F71" s="3"/>
-      <c r="G71" s="57"/>
-      <c r="H71" s="58"/>
+      <c r="G71" s="83"/>
+      <c r="H71" s="84"/>
       <c r="I71" s="13"/>
       <c r="J71" s="13"/>
       <c r="K71" s="13"/>
       <c r="L71" s="27"/>
     </row>
     <row r="72" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="132"/>
-      <c r="B72" s="133"/>
+      <c r="A72" s="108"/>
+      <c r="B72" s="109"/>
       <c r="C72" s="39"/>
       <c r="D72" s="39"/>
       <c r="E72" s="40"/>
       <c r="F72" s="3"/>
-      <c r="G72" s="59"/>
-      <c r="H72" s="60"/>
+      <c r="G72" s="85"/>
+      <c r="H72" s="86"/>
       <c r="I72" s="11"/>
       <c r="J72" s="11"/>
       <c r="K72" s="11"/>
       <c r="L72" s="26"/>
     </row>
     <row r="73" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="115" t="s">
-        <v>110</v>
-      </c>
-      <c r="B73" s="116"/>
-      <c r="C73" s="116"/>
-      <c r="D73" s="117"/>
+      <c r="A73" s="92" t="s">
+        <v>108</v>
+      </c>
+      <c r="B73" s="93"/>
+      <c r="C73" s="93"/>
+      <c r="D73" s="94"/>
       <c r="E73" s="38"/>
       <c r="F73" s="3"/>
-      <c r="G73" s="57"/>
-      <c r="H73" s="58"/>
+      <c r="G73" s="83"/>
+      <c r="H73" s="84"/>
       <c r="I73" s="13"/>
       <c r="J73" s="13"/>
       <c r="K73" s="13"/>
@@ -3547,46 +3565,46 @@
     </row>
     <row r="74" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F74" s="3"/>
-      <c r="G74" s="59"/>
-      <c r="H74" s="60"/>
+      <c r="G74" s="85"/>
+      <c r="H74" s="86"/>
       <c r="I74" s="11"/>
       <c r="J74" s="11"/>
       <c r="K74" s="11"/>
       <c r="L74" s="26"/>
     </row>
     <row r="75" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="120" t="s">
-        <v>82</v>
-      </c>
-      <c r="B75" s="121"/>
-      <c r="C75" s="121"/>
-      <c r="D75" s="121"/>
-      <c r="E75" s="122"/>
+      <c r="A75" s="98" t="s">
+        <v>80</v>
+      </c>
+      <c r="B75" s="99"/>
+      <c r="C75" s="99"/>
+      <c r="D75" s="99"/>
+      <c r="E75" s="100"/>
       <c r="F75" s="3"/>
-      <c r="G75" s="57"/>
-      <c r="H75" s="58"/>
+      <c r="G75" s="83"/>
+      <c r="H75" s="84"/>
       <c r="I75" s="13"/>
       <c r="J75" s="13"/>
       <c r="K75" s="13"/>
       <c r="L75" s="27"/>
     </row>
     <row r="76" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="78" t="s">
+      <c r="A76" s="77" t="s">
         <v>50</v>
       </c>
-      <c r="B76" s="123"/>
-      <c r="C76" s="123"/>
+      <c r="B76" s="78"/>
+      <c r="C76" s="78"/>
       <c r="D76" s="79"/>
       <c r="E76" s="19"/>
       <c r="F76" s="3"/>
     </row>
     <row r="77" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="82" t="s">
+      <c r="A77" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="B77" s="142"/>
-      <c r="C77" s="142"/>
-      <c r="D77" s="83"/>
+      <c r="B77" s="76"/>
+      <c r="C77" s="76"/>
+      <c r="D77" s="75"/>
       <c r="E77" s="18"/>
       <c r="F77" s="3"/>
       <c r="G77" s="47" t="s">
@@ -3599,11 +3617,11 @@
       <c r="L77" s="49"/>
     </row>
     <row r="78" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="78" t="s">
+      <c r="A78" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="B78" s="123"/>
-      <c r="C78" s="123"/>
+      <c r="B78" s="78"/>
+      <c r="C78" s="78"/>
       <c r="D78" s="79"/>
       <c r="E78" s="19"/>
       <c r="F78" s="3"/>
@@ -3617,7 +3635,7 @@
         <v>3</v>
       </c>
       <c r="J78" s="23" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K78" s="23" t="s">
         <v>49</v>
@@ -3627,12 +3645,12 @@
       </c>
     </row>
     <row r="79" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="82" t="s">
+      <c r="A79" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="B79" s="142"/>
-      <c r="C79" s="142"/>
-      <c r="D79" s="83"/>
+      <c r="B79" s="76"/>
+      <c r="C79" s="76"/>
+      <c r="D79" s="75"/>
       <c r="E79" s="18"/>
       <c r="F79" s="3"/>
       <c r="G79" s="45" t="s">
@@ -3645,12 +3663,12 @@
       <c r="L79" s="13"/>
     </row>
     <row r="80" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="139" t="s">
+      <c r="A80" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="B80" s="140"/>
-      <c r="C80" s="140"/>
-      <c r="D80" s="141"/>
+      <c r="B80" s="66"/>
+      <c r="C80" s="66"/>
+      <c r="D80" s="67"/>
       <c r="E80" s="44"/>
       <c r="F80" s="3"/>
       <c r="G80" s="46" t="s">
@@ -3674,16 +3692,16 @@
       <c r="L81" s="13"/>
     </row>
     <row r="82" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="88" t="s">
+      <c r="A82" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="B82" s="89"/>
-      <c r="C82" s="89"/>
-      <c r="D82" s="89"/>
-      <c r="E82" s="90"/>
+      <c r="B82" s="96"/>
+      <c r="C82" s="96"/>
+      <c r="D82" s="96"/>
+      <c r="E82" s="97"/>
       <c r="F82" s="3"/>
       <c r="G82" s="46" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H82" s="11"/>
       <c r="I82" s="11"/>
@@ -3692,22 +3710,22 @@
       <c r="L82" s="11"/>
     </row>
     <row r="83" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="55" t="s">
+      <c r="A83" s="113" t="s">
         <v>35</v>
       </c>
-      <c r="B83" s="56"/>
+      <c r="B83" s="111"/>
       <c r="C83" s="29" t="s">
         <v>34</v>
       </c>
       <c r="D83" s="29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E83" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F83" s="3"/>
       <c r="G83" s="41" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H83" s="42"/>
       <c r="I83" s="42"/>
@@ -3716,19 +3734,19 @@
       <c r="L83" s="43"/>
     </row>
     <row r="84" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="101"/>
-      <c r="B84" s="102"/>
+      <c r="A84" s="127"/>
+      <c r="B84" s="128"/>
       <c r="C84" s="11"/>
       <c r="D84" s="11"/>
       <c r="E84" s="10"/>
       <c r="F84" s="3"/>
       <c r="G84" s="41" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H84" s="42"/>
     </row>
     <row r="85" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="78"/>
+      <c r="A85" s="77"/>
       <c r="B85" s="79"/>
       <c r="C85" s="13"/>
       <c r="D85" s="13"/>
@@ -3736,15 +3754,15 @@
       <c r="F85" s="3"/>
     </row>
     <row r="86" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="82"/>
-      <c r="B86" s="83"/>
+      <c r="A86" s="74"/>
+      <c r="B86" s="75"/>
       <c r="C86" s="11"/>
       <c r="D86" s="11"/>
       <c r="E86" s="10"/>
       <c r="F86" s="3"/>
     </row>
     <row r="87" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="78"/>
+      <c r="A87" s="77"/>
       <c r="B87" s="79"/>
       <c r="C87" s="13"/>
       <c r="D87" s="13"/>
@@ -3752,15 +3770,15 @@
       <c r="F87" s="3"/>
     </row>
     <row r="88" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="82"/>
-      <c r="B88" s="83"/>
+      <c r="A88" s="74"/>
+      <c r="B88" s="75"/>
       <c r="C88" s="11"/>
       <c r="D88" s="11"/>
       <c r="E88" s="10"/>
       <c r="F88" s="3"/>
     </row>
     <row r="89" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="78"/>
+      <c r="A89" s="77"/>
       <c r="B89" s="79"/>
       <c r="C89" s="13"/>
       <c r="D89" s="13"/>
@@ -3768,15 +3786,15 @@
       <c r="F89" s="3"/>
     </row>
     <row r="90" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="82"/>
-      <c r="B90" s="83"/>
+      <c r="A90" s="74"/>
+      <c r="B90" s="75"/>
       <c r="C90" s="11"/>
       <c r="D90" s="11"/>
       <c r="E90" s="10"/>
       <c r="F90" s="3"/>
     </row>
     <row r="91" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="78"/>
+      <c r="A91" s="77"/>
       <c r="B91" s="79"/>
       <c r="C91" s="13"/>
       <c r="D91" s="13"/>
@@ -3784,15 +3802,15 @@
       <c r="F91" s="3"/>
     </row>
     <row r="92" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="82"/>
-      <c r="B92" s="83"/>
+      <c r="A92" s="74"/>
+      <c r="B92" s="75"/>
       <c r="C92" s="11"/>
       <c r="D92" s="11"/>
       <c r="E92" s="10"/>
       <c r="F92" s="3"/>
     </row>
     <row r="93" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="78"/>
+      <c r="A93" s="77"/>
       <c r="B93" s="79"/>
       <c r="C93" s="13"/>
       <c r="D93" s="13"/>
@@ -3800,15 +3818,15 @@
       <c r="F93" s="3"/>
     </row>
     <row r="94" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="82"/>
-      <c r="B94" s="83"/>
+      <c r="A94" s="74"/>
+      <c r="B94" s="75"/>
       <c r="C94" s="11"/>
       <c r="D94" s="11"/>
       <c r="E94" s="10"/>
       <c r="F94" s="3"/>
     </row>
     <row r="95" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="78"/>
+      <c r="A95" s="77"/>
       <c r="B95" s="79"/>
       <c r="C95" s="13"/>
       <c r="D95" s="13"/>
@@ -3816,15 +3834,15 @@
       <c r="F95" s="3"/>
     </row>
     <row r="96" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="82"/>
-      <c r="B96" s="83"/>
+      <c r="A96" s="74"/>
+      <c r="B96" s="75"/>
       <c r="C96" s="11"/>
       <c r="D96" s="11"/>
       <c r="E96" s="10"/>
       <c r="F96" s="3"/>
     </row>
     <row r="97" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="78"/>
+      <c r="A97" s="77"/>
       <c r="B97" s="79"/>
       <c r="C97" s="13"/>
       <c r="D97" s="13"/>
@@ -3832,15 +3850,15 @@
       <c r="F97" s="3"/>
     </row>
     <row r="98" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="82"/>
-      <c r="B98" s="83"/>
+      <c r="A98" s="74"/>
+      <c r="B98" s="75"/>
       <c r="C98" s="11"/>
       <c r="D98" s="11"/>
       <c r="E98" s="10"/>
       <c r="F98" s="3"/>
     </row>
     <row r="99" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="78"/>
+      <c r="A99" s="77"/>
       <c r="B99" s="79"/>
       <c r="C99" s="13"/>
       <c r="D99" s="13"/>
@@ -3848,28 +3866,28 @@
       <c r="F99" s="3"/>
     </row>
     <row r="100" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="82"/>
-      <c r="B100" s="83"/>
+      <c r="A100" s="74"/>
+      <c r="B100" s="75"/>
       <c r="C100" s="11"/>
       <c r="D100" s="11"/>
       <c r="E100" s="10"/>
       <c r="F100" s="3"/>
     </row>
     <row r="101" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="134"/>
-      <c r="B101" s="135"/>
+      <c r="A101" s="87"/>
+      <c r="B101" s="88"/>
       <c r="C101" s="13"/>
       <c r="D101" s="13"/>
       <c r="E101" s="12"/>
       <c r="F101" s="3"/>
     </row>
     <row r="102" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="115" t="s">
+      <c r="A102" s="92" t="s">
         <v>14</v>
       </c>
-      <c r="B102" s="116"/>
-      <c r="C102" s="116"/>
-      <c r="D102" s="117"/>
+      <c r="B102" s="93"/>
+      <c r="C102" s="93"/>
+      <c r="D102" s="94"/>
       <c r="E102" s="38"/>
       <c r="F102" s="3"/>
     </row>
@@ -3877,22 +3895,22 @@
       <c r="F103" s="3"/>
     </row>
     <row r="104" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="125" t="s">
+      <c r="A104" s="101" t="s">
         <v>7</v>
       </c>
-      <c r="B104" s="126"/>
-      <c r="C104" s="126"/>
-      <c r="D104" s="126"/>
-      <c r="E104" s="127"/>
+      <c r="B104" s="102"/>
+      <c r="C104" s="102"/>
+      <c r="D104" s="102"/>
+      <c r="E104" s="103"/>
       <c r="F104" s="3"/>
     </row>
     <row r="105" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="128" t="s">
+      <c r="A105" s="104" t="s">
         <v>45</v>
       </c>
-      <c r="B105" s="129"/>
+      <c r="B105" s="105"/>
       <c r="C105" s="21" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D105" s="21" t="s">
         <v>46</v>
@@ -3903,156 +3921,156 @@
       <c r="F105" s="3"/>
     </row>
     <row r="106" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="130"/>
-      <c r="B106" s="131"/>
+      <c r="A106" s="106"/>
+      <c r="B106" s="107"/>
       <c r="C106" s="8"/>
       <c r="D106" s="8"/>
       <c r="E106" s="6"/>
       <c r="F106" s="3"/>
     </row>
     <row r="107" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="124"/>
-      <c r="B107" s="96"/>
+      <c r="A107" s="63"/>
+      <c r="B107" s="64"/>
       <c r="C107" s="11"/>
       <c r="D107" s="11"/>
       <c r="E107" s="10"/>
       <c r="F107" s="3"/>
     </row>
     <row r="108" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="86"/>
-      <c r="B108" s="87"/>
+      <c r="A108" s="61"/>
+      <c r="B108" s="62"/>
       <c r="C108" s="8"/>
       <c r="D108" s="8"/>
       <c r="E108" s="6"/>
       <c r="F108" s="3"/>
     </row>
     <row r="109" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="124"/>
-      <c r="B109" s="96"/>
+      <c r="A109" s="63"/>
+      <c r="B109" s="64"/>
       <c r="C109" s="11"/>
       <c r="D109" s="11"/>
       <c r="E109" s="10"/>
       <c r="F109" s="3"/>
     </row>
     <row r="110" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="86"/>
-      <c r="B110" s="87"/>
+      <c r="A110" s="61"/>
+      <c r="B110" s="62"/>
       <c r="C110" s="8"/>
       <c r="D110" s="8"/>
       <c r="E110" s="6"/>
       <c r="F110" s="3"/>
     </row>
     <row r="111" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="124"/>
-      <c r="B111" s="96"/>
+      <c r="A111" s="63"/>
+      <c r="B111" s="64"/>
       <c r="C111" s="11"/>
       <c r="D111" s="11"/>
       <c r="E111" s="10"/>
       <c r="F111" s="3"/>
     </row>
     <row r="112" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="86"/>
-      <c r="B112" s="87"/>
+      <c r="A112" s="61"/>
+      <c r="B112" s="62"/>
       <c r="C112" s="8"/>
       <c r="D112" s="8"/>
       <c r="E112" s="6"/>
       <c r="F112" s="3"/>
     </row>
     <row r="113" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="124"/>
-      <c r="B113" s="96"/>
+      <c r="A113" s="63"/>
+      <c r="B113" s="64"/>
       <c r="C113" s="11"/>
       <c r="D113" s="11"/>
       <c r="E113" s="10"/>
       <c r="F113" s="3"/>
     </row>
     <row r="114" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="86"/>
-      <c r="B114" s="87"/>
+      <c r="A114" s="61"/>
+      <c r="B114" s="62"/>
       <c r="C114" s="13"/>
       <c r="D114" s="13"/>
       <c r="E114" s="6"/>
       <c r="F114" s="3"/>
     </row>
     <row r="115" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="124"/>
-      <c r="B115" s="96"/>
+      <c r="A115" s="63"/>
+      <c r="B115" s="64"/>
       <c r="C115" s="11"/>
       <c r="D115" s="11"/>
       <c r="E115" s="10"/>
       <c r="F115" s="3"/>
     </row>
     <row r="116" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="86"/>
-      <c r="B116" s="87"/>
+      <c r="A116" s="61"/>
+      <c r="B116" s="62"/>
       <c r="C116" s="13"/>
       <c r="D116" s="13"/>
       <c r="E116" s="6"/>
       <c r="F116" s="3"/>
     </row>
     <row r="117" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="124"/>
-      <c r="B117" s="96"/>
+      <c r="A117" s="63"/>
+      <c r="B117" s="64"/>
       <c r="C117" s="11"/>
       <c r="D117" s="11"/>
       <c r="E117" s="10"/>
       <c r="F117" s="3"/>
     </row>
     <row r="118" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="86"/>
-      <c r="B118" s="87"/>
+      <c r="A118" s="61"/>
+      <c r="B118" s="62"/>
       <c r="C118" s="13"/>
       <c r="D118" s="13"/>
       <c r="E118" s="6"/>
       <c r="F118" s="3"/>
     </row>
     <row r="119" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="124"/>
-      <c r="B119" s="96"/>
+      <c r="A119" s="63"/>
+      <c r="B119" s="64"/>
       <c r="C119" s="11"/>
       <c r="D119" s="11"/>
       <c r="E119" s="10"/>
       <c r="F119" s="3"/>
     </row>
     <row r="120" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="86"/>
-      <c r="B120" s="87"/>
+      <c r="A120" s="61"/>
+      <c r="B120" s="62"/>
       <c r="C120" s="13"/>
       <c r="D120" s="13"/>
       <c r="E120" s="12"/>
       <c r="F120" s="3"/>
     </row>
     <row r="121" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="124"/>
-      <c r="B121" s="96"/>
+      <c r="A121" s="63"/>
+      <c r="B121" s="64"/>
       <c r="C121" s="11"/>
       <c r="D121" s="11"/>
       <c r="E121" s="10"/>
       <c r="F121" s="3"/>
     </row>
     <row r="122" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="86"/>
-      <c r="B122" s="87"/>
+      <c r="A122" s="61"/>
+      <c r="B122" s="62"/>
       <c r="C122" s="13"/>
       <c r="D122" s="13"/>
       <c r="E122" s="12"/>
       <c r="F122" s="3"/>
     </row>
     <row r="123" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="124"/>
-      <c r="B123" s="96"/>
+      <c r="A123" s="63"/>
+      <c r="B123" s="64"/>
       <c r="C123" s="11"/>
       <c r="D123" s="11"/>
       <c r="E123" s="10"/>
       <c r="F123" s="3"/>
     </row>
     <row r="124" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="115" t="s">
-        <v>116</v>
-      </c>
-      <c r="B124" s="116"/>
-      <c r="C124" s="116"/>
-      <c r="D124" s="117"/>
+      <c r="A124" s="92" t="s">
+        <v>114</v>
+      </c>
+      <c r="B124" s="93"/>
+      <c r="C124" s="93"/>
+      <c r="D124" s="94"/>
       <c r="E124" s="38"/>
       <c r="F124" s="3"/>
     </row>
@@ -4629,6 +4647,165 @@
     </row>
   </sheetData>
   <mergeCells count="183">
+    <mergeCell ref="G41:L41"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="G63:H63"/>
+    <mergeCell ref="G64:H64"/>
+    <mergeCell ref="G65:H65"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="G1:L1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="A53:C53"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="A46:E46"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="A82:E82"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="A73:D73"/>
+    <mergeCell ref="G61:H61"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="G70:H70"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="A124:D124"/>
+    <mergeCell ref="A75:E75"/>
+    <mergeCell ref="A76:D76"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="A104:E104"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="G62:H62"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="G59:H59"/>
+    <mergeCell ref="G60:H60"/>
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="G71:H71"/>
+    <mergeCell ref="G72:H72"/>
+    <mergeCell ref="G73:H73"/>
+    <mergeCell ref="G74:H74"/>
+    <mergeCell ref="G75:H75"/>
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="G67:H67"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="G69:H69"/>
+    <mergeCell ref="A102:D102"/>
+    <mergeCell ref="A68:E68"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A116:B116"/>
     <mergeCell ref="A117:B117"/>
@@ -4653,165 +4830,6 @@
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="G59:H59"/>
-    <mergeCell ref="G60:H60"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="G71:H71"/>
-    <mergeCell ref="G72:H72"/>
-    <mergeCell ref="G73:H73"/>
-    <mergeCell ref="G74:H74"/>
-    <mergeCell ref="G75:H75"/>
-    <mergeCell ref="A64:C64"/>
-    <mergeCell ref="G66:H66"/>
-    <mergeCell ref="G67:H67"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="G69:H69"/>
-    <mergeCell ref="A102:D102"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="A124:D124"/>
-    <mergeCell ref="A75:E75"/>
-    <mergeCell ref="A76:D76"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="A104:E104"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="G62:H62"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="A73:D73"/>
-    <mergeCell ref="G61:H61"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="G52:H52"/>
-    <mergeCell ref="G70:H70"/>
-    <mergeCell ref="G53:H53"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="A68:E68"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="A53:C53"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="G57:H57"/>
-    <mergeCell ref="A46:E46"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="A82:E82"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="G41:L41"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="G63:H63"/>
-    <mergeCell ref="G64:H64"/>
-    <mergeCell ref="G65:H65"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="G1:L1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="G6:H6"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Dexotex over concrete and Multicoat Formula update SIKA
</commit_message>
<xml_diff>
--- a/WICR Estimator/SummaryTemplate.xlsx
+++ b/WICR Estimator/SummaryTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Freelancer Projects\Amin_WICr Estimator\WICR Estimator_08-10-18\WICR Estimator_08-10-18\WICR Estimator\WICR Estimator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3160B1FF-9C45-486F-BEB2-2EE0B6D2AAE3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65538CA7-BEED-40CB-84B5-DDBB14F1A8B0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="347" xr2:uid="{C3BB3D69-FD31-4C45-AAE2-714CBD52CC32}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="129">
   <si>
     <t>Job Setup</t>
   </si>
@@ -396,6 +396,42 @@
   </si>
   <si>
     <t>Urethane Slope</t>
+  </si>
+  <si>
+    <t>Workers Compensation TL &gt; 24.00</t>
+  </si>
+  <si>
+    <t>Workers Compensation All &lt; 23.99</t>
+  </si>
+  <si>
+    <t>Workers Compensation Prevailing Wage</t>
+  </si>
+  <si>
+    <t>Payroll Expense (SS, ET, Uemp, Dis, Medi)</t>
+  </si>
+  <si>
+    <t>Sales Tax</t>
+  </si>
+  <si>
+    <t>Subcontractor Mark up</t>
+  </si>
+  <si>
+    <t>General Liability Insurance</t>
+  </si>
+  <si>
+    <t>Direct Expense (gas, small tools, etc.)</t>
+  </si>
+  <si>
+    <t>Contingency</t>
+  </si>
+  <si>
+    <t>Additional Costs</t>
+  </si>
+  <si>
+    <t>Total Price</t>
+  </si>
+  <si>
+    <t>Cost Calculation Details</t>
   </si>
 </sst>
 </file>
@@ -472,7 +508,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="71">
+  <borders count="72">
     <border>
       <left/>
       <right/>
@@ -1412,12 +1448,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="149">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyProtection="1"/>
@@ -1530,6 +1579,102 @@
     <xf numFmtId="2" fontId="4" fillId="5" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="2" fontId="4" fillId="4" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1545,77 +1690,143 @@
     <xf numFmtId="2" fontId="4" fillId="4" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="5" fillId="5" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="5" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="48" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="52" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="53" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="56" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="57" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="58" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="4" fillId="5" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="53" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="52" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="63" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="64" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="65" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="66" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="60" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="61" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="4" borderId="54" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1632,176 +1843,22 @@
     <xf numFmtId="2" fontId="3" fillId="3" borderId="70" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="56" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="57" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="58" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="63" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="64" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="65" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="66" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="60" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="61" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="4" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="4" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="5" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="5" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="48" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="71" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2242,8 +2299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13628510-9764-4D87-A543-465B04714C1D}">
   <dimension ref="A1:BD219"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:D16"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="J96" sqref="J96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2254,7 +2311,7 @@
     <col min="4" max="4" width="9" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" style="2" customWidth="1"/>
     <col min="6" max="6" width="1.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="27.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" style="2" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" style="2" customWidth="1"/>
     <col min="9" max="9" width="8.85546875" style="2"/>
     <col min="10" max="10" width="8.85546875" style="2" customWidth="1"/>
@@ -2289,35 +2346,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="134" t="s">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="135"/>
-      <c r="C1" s="135"/>
-      <c r="D1" s="135"/>
-      <c r="E1" s="136"/>
-      <c r="G1" s="137" t="s">
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="61"/>
+      <c r="G1" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="138"/>
-      <c r="I1" s="138"/>
-      <c r="J1" s="138"/>
-      <c r="K1" s="138"/>
-      <c r="L1" s="139"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="70"/>
     </row>
     <row r="2" spans="1:32" ht="12.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="140" t="s">
+      <c r="A2" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="141"/>
-      <c r="C2" s="141"/>
-      <c r="D2" s="141"/>
-      <c r="E2" s="142"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="73"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="143" t="s">
+      <c r="G2" s="74" t="s">
         <v>84</v>
       </c>
-      <c r="H2" s="144"/>
+      <c r="H2" s="75"/>
       <c r="I2" s="29" t="s">
         <v>55</v>
       </c>
@@ -2335,416 +2392,416 @@
       <c r="AF2" s="5"/>
     </row>
     <row r="3" spans="1:32" s="9" customFormat="1" ht="12.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="145" t="s">
+      <c r="A3" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="146"/>
-      <c r="C3" s="146"/>
-      <c r="D3" s="146"/>
+      <c r="B3" s="77"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
       <c r="E3" s="54"/>
       <c r="F3" s="7"/>
-      <c r="G3" s="131" t="s">
+      <c r="G3" s="78" t="s">
         <v>67</v>
       </c>
-      <c r="H3" s="132"/>
+      <c r="H3" s="79"/>
       <c r="I3" s="32"/>
       <c r="J3" s="32"/>
       <c r="K3" s="32"/>
       <c r="L3" s="33"/>
     </row>
     <row r="4" spans="1:32" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="82" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
+      <c r="B4" s="83"/>
+      <c r="C4" s="83"/>
+      <c r="D4" s="83"/>
       <c r="E4" s="55"/>
       <c r="F4" s="7"/>
-      <c r="G4" s="74" t="s">
+      <c r="G4" s="84" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="75"/>
+      <c r="H4" s="85"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
       <c r="L4" s="26"/>
     </row>
     <row r="5" spans="1:32" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="133" t="s">
+      <c r="A5" s="86" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
+      <c r="B5" s="87"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="87"/>
       <c r="E5" s="56"/>
       <c r="F5" s="7"/>
-      <c r="G5" s="77" t="s">
+      <c r="G5" s="80" t="s">
         <v>68</v>
       </c>
-      <c r="H5" s="79"/>
+      <c r="H5" s="81"/>
       <c r="I5" s="13"/>
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
       <c r="L5" s="27"/>
     </row>
     <row r="6" spans="1:32" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="68" t="s">
+      <c r="A6" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="69"/>
-      <c r="C6" s="69"/>
-      <c r="D6" s="69"/>
+      <c r="B6" s="83"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="83"/>
       <c r="E6" s="55"/>
       <c r="F6" s="7"/>
-      <c r="G6" s="74" t="s">
+      <c r="G6" s="84" t="s">
         <v>69</v>
       </c>
-      <c r="H6" s="75"/>
+      <c r="H6" s="85"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
       <c r="L6" s="26"/>
     </row>
     <row r="7" spans="1:32" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="58" t="s">
+      <c r="A7" s="90" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="59"/>
-      <c r="C7" s="60"/>
+      <c r="B7" s="91"/>
+      <c r="C7" s="92"/>
       <c r="D7" s="13"/>
       <c r="E7" s="56"/>
       <c r="F7" s="7"/>
-      <c r="G7" s="77" t="s">
+      <c r="G7" s="80" t="s">
         <v>70</v>
       </c>
-      <c r="H7" s="79"/>
+      <c r="H7" s="81"/>
       <c r="I7" s="13"/>
       <c r="J7" s="13"/>
       <c r="K7" s="13"/>
       <c r="L7" s="27"/>
     </row>
     <row r="8" spans="1:32" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="82" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="69"/>
-      <c r="C8" s="69"/>
-      <c r="D8" s="69"/>
+      <c r="B8" s="83"/>
+      <c r="C8" s="83"/>
+      <c r="D8" s="83"/>
       <c r="E8" s="55"/>
       <c r="F8" s="7"/>
-      <c r="G8" s="74" t="s">
+      <c r="G8" s="84" t="s">
         <v>71</v>
       </c>
-      <c r="H8" s="75"/>
+      <c r="H8" s="85"/>
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
       <c r="L8" s="26"/>
     </row>
     <row r="9" spans="1:32" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="133" t="s">
+      <c r="A9" s="86" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="70"/>
-      <c r="C9" s="70"/>
-      <c r="D9" s="70"/>
+      <c r="B9" s="87"/>
+      <c r="C9" s="87"/>
+      <c r="D9" s="87"/>
       <c r="E9" s="56"/>
       <c r="F9" s="7"/>
-      <c r="G9" s="77" t="s">
+      <c r="G9" s="80" t="s">
         <v>72</v>
       </c>
-      <c r="H9" s="79"/>
+      <c r="H9" s="81"/>
       <c r="I9" s="13"/>
       <c r="J9" s="13"/>
       <c r="K9" s="13"/>
       <c r="L9" s="27"/>
     </row>
     <row r="10" spans="1:32" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="68" t="s">
+      <c r="A10" s="82" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="69"/>
-      <c r="C10" s="69"/>
-      <c r="D10" s="69"/>
+      <c r="B10" s="83"/>
+      <c r="C10" s="83"/>
+      <c r="D10" s="83"/>
       <c r="E10" s="55"/>
       <c r="F10" s="7"/>
-      <c r="G10" s="74" t="s">
+      <c r="G10" s="84" t="s">
         <v>73</v>
       </c>
-      <c r="H10" s="75"/>
+      <c r="H10" s="85"/>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
       <c r="L10" s="26"/>
     </row>
     <row r="11" spans="1:32" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="133" t="s">
+      <c r="A11" s="86" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="70"/>
-      <c r="C11" s="70"/>
-      <c r="D11" s="70"/>
+      <c r="B11" s="87"/>
+      <c r="C11" s="87"/>
+      <c r="D11" s="87"/>
       <c r="E11" s="56"/>
       <c r="F11" s="7"/>
-      <c r="G11" s="77" t="s">
+      <c r="G11" s="80" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="79"/>
+      <c r="H11" s="81"/>
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
       <c r="L11" s="27"/>
     </row>
     <row r="12" spans="1:32" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="68" t="s">
+      <c r="A12" s="82" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="69"/>
-      <c r="C12" s="69"/>
-      <c r="D12" s="69"/>
+      <c r="B12" s="83"/>
+      <c r="C12" s="83"/>
+      <c r="D12" s="83"/>
       <c r="E12" s="55"/>
       <c r="F12" s="7"/>
-      <c r="G12" s="74" t="s">
+      <c r="G12" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="75"/>
+      <c r="H12" s="85"/>
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
       <c r="L12" s="26"/>
     </row>
     <row r="13" spans="1:32" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="58" t="s">
+      <c r="A13" s="90" t="s">
         <v>65</v>
       </c>
-      <c r="B13" s="59"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="60"/>
+      <c r="B13" s="91"/>
+      <c r="C13" s="91"/>
+      <c r="D13" s="92"/>
       <c r="E13" s="56"/>
       <c r="F13" s="7"/>
-      <c r="G13" s="77" t="s">
+      <c r="G13" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="79"/>
+      <c r="H13" s="81"/>
       <c r="I13" s="13"/>
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
       <c r="L13" s="27"/>
     </row>
     <row r="14" spans="1:32" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="147" t="s">
+      <c r="A14" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="148"/>
-      <c r="C14" s="148"/>
-      <c r="D14" s="148"/>
+      <c r="B14" s="89"/>
+      <c r="C14" s="89"/>
+      <c r="D14" s="89"/>
       <c r="E14" s="57"/>
       <c r="F14" s="7"/>
-      <c r="G14" s="74" t="s">
+      <c r="G14" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="H14" s="75"/>
+      <c r="H14" s="85"/>
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
       <c r="K14" s="11"/>
       <c r="L14" s="26"/>
     </row>
     <row r="15" spans="1:32" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="133" t="s">
+      <c r="A15" s="86" t="s">
         <v>81</v>
       </c>
-      <c r="B15" s="70"/>
-      <c r="C15" s="70"/>
-      <c r="D15" s="70"/>
+      <c r="B15" s="87"/>
+      <c r="C15" s="87"/>
+      <c r="D15" s="87"/>
       <c r="E15" s="56"/>
       <c r="F15" s="7"/>
-      <c r="G15" s="77" t="s">
+      <c r="G15" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="H15" s="79"/>
+      <c r="H15" s="81"/>
       <c r="I15" s="13"/>
       <c r="J15" s="13"/>
       <c r="K15" s="13"/>
       <c r="L15" s="27"/>
     </row>
     <row r="16" spans="1:32" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="68" t="s">
+      <c r="A16" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="B16" s="69"/>
-      <c r="C16" s="69"/>
-      <c r="D16" s="69"/>
+      <c r="B16" s="83"/>
+      <c r="C16" s="83"/>
+      <c r="D16" s="83"/>
       <c r="E16" s="55"/>
       <c r="F16" s="7"/>
-      <c r="G16" s="74" t="s">
+      <c r="G16" s="84" t="s">
         <v>31</v>
       </c>
-      <c r="H16" s="75"/>
+      <c r="H16" s="85"/>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
       <c r="K16" s="11"/>
       <c r="L16" s="26"/>
     </row>
     <row r="17" spans="1:12" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="133" t="s">
+      <c r="A17" s="86" t="s">
         <v>83</v>
       </c>
-      <c r="B17" s="70"/>
-      <c r="C17" s="70"/>
-      <c r="D17" s="70"/>
+      <c r="B17" s="87"/>
+      <c r="C17" s="87"/>
+      <c r="D17" s="87"/>
       <c r="E17" s="56"/>
       <c r="F17" s="7"/>
-      <c r="G17" s="77" t="s">
+      <c r="G17" s="80" t="s">
         <v>32</v>
       </c>
-      <c r="H17" s="79"/>
+      <c r="H17" s="81"/>
       <c r="I17" s="13"/>
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
       <c r="L17" s="27"/>
     </row>
     <row r="18" spans="1:12" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="68"/>
-      <c r="B18" s="69"/>
-      <c r="C18" s="69"/>
-      <c r="D18" s="69"/>
+      <c r="A18" s="82"/>
+      <c r="B18" s="83"/>
+      <c r="C18" s="83"/>
+      <c r="D18" s="83"/>
       <c r="E18" s="55"/>
       <c r="F18" s="7"/>
-      <c r="G18" s="74" t="s">
+      <c r="G18" s="84" t="s">
         <v>33</v>
       </c>
-      <c r="H18" s="75"/>
+      <c r="H18" s="85"/>
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
       <c r="K18" s="11"/>
       <c r="L18" s="26"/>
     </row>
     <row r="19" spans="1:12" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="70"/>
-      <c r="B19" s="70"/>
-      <c r="C19" s="70"/>
-      <c r="D19" s="70"/>
+      <c r="A19" s="87"/>
+      <c r="B19" s="87"/>
+      <c r="C19" s="87"/>
+      <c r="D19" s="87"/>
       <c r="E19" s="52"/>
       <c r="F19" s="7"/>
-      <c r="G19" s="77" t="s">
+      <c r="G19" s="80" t="s">
         <v>74</v>
       </c>
-      <c r="H19" s="79"/>
+      <c r="H19" s="81"/>
       <c r="I19" s="13"/>
       <c r="J19" s="13"/>
       <c r="K19" s="13"/>
       <c r="L19" s="27"/>
     </row>
     <row r="20" spans="1:12" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="69"/>
-      <c r="B20" s="69"/>
-      <c r="C20" s="69"/>
-      <c r="D20" s="69"/>
+      <c r="A20" s="83"/>
+      <c r="B20" s="83"/>
+      <c r="C20" s="83"/>
+      <c r="D20" s="83"/>
       <c r="E20" s="53"/>
       <c r="F20" s="7"/>
-      <c r="G20" s="74" t="s">
+      <c r="G20" s="84" t="s">
         <v>75</v>
       </c>
-      <c r="H20" s="75"/>
+      <c r="H20" s="85"/>
       <c r="I20" s="11"/>
       <c r="J20" s="11"/>
       <c r="K20" s="11"/>
       <c r="L20" s="26"/>
     </row>
     <row r="21" spans="1:12" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="70"/>
-      <c r="B21" s="70"/>
-      <c r="C21" s="70"/>
-      <c r="D21" s="70"/>
+      <c r="A21" s="87"/>
+      <c r="B21" s="87"/>
+      <c r="C21" s="87"/>
+      <c r="D21" s="87"/>
       <c r="E21" s="52"/>
       <c r="F21" s="7"/>
-      <c r="G21" s="61" t="s">
+      <c r="G21" s="93" t="s">
         <v>76</v>
       </c>
-      <c r="H21" s="62"/>
+      <c r="H21" s="94"/>
       <c r="I21" s="13"/>
       <c r="J21" s="13"/>
       <c r="K21" s="13"/>
       <c r="L21" s="27"/>
     </row>
     <row r="22" spans="1:12" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="69"/>
-      <c r="B22" s="69"/>
-      <c r="C22" s="69"/>
-      <c r="D22" s="69"/>
+      <c r="A22" s="83"/>
+      <c r="B22" s="83"/>
+      <c r="C22" s="83"/>
+      <c r="D22" s="83"/>
       <c r="E22" s="53"/>
-      <c r="G22" s="74" t="s">
+      <c r="G22" s="84" t="s">
         <v>85</v>
       </c>
-      <c r="H22" s="75"/>
+      <c r="H22" s="85"/>
       <c r="I22" s="11"/>
       <c r="J22" s="11"/>
       <c r="K22" s="11"/>
       <c r="L22" s="26"/>
     </row>
     <row r="23" spans="1:12" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="70"/>
-      <c r="B23" s="70"/>
-      <c r="C23" s="70"/>
-      <c r="D23" s="70"/>
+      <c r="A23" s="87"/>
+      <c r="B23" s="87"/>
+      <c r="C23" s="87"/>
+      <c r="D23" s="87"/>
       <c r="E23" s="52"/>
-      <c r="G23" s="77" t="s">
+      <c r="G23" s="80" t="s">
         <v>86</v>
       </c>
-      <c r="H23" s="79"/>
+      <c r="H23" s="81"/>
       <c r="I23" s="13"/>
       <c r="J23" s="13"/>
       <c r="K23" s="13"/>
       <c r="L23" s="27"/>
     </row>
     <row r="24" spans="1:12" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="69"/>
-      <c r="B24" s="69"/>
-      <c r="C24" s="69"/>
-      <c r="D24" s="69"/>
+      <c r="A24" s="83"/>
+      <c r="B24" s="83"/>
+      <c r="C24" s="83"/>
+      <c r="D24" s="83"/>
       <c r="E24" s="53"/>
-      <c r="G24" s="74" t="s">
+      <c r="G24" s="84" t="s">
         <v>87</v>
       </c>
-      <c r="H24" s="75"/>
+      <c r="H24" s="85"/>
       <c r="I24" s="11"/>
       <c r="J24" s="11"/>
       <c r="K24" s="11"/>
       <c r="L24" s="26"/>
     </row>
     <row r="25" spans="1:12" s="9" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G25" s="77" t="s">
+      <c r="G25" s="80" t="s">
         <v>88</v>
       </c>
-      <c r="H25" s="79"/>
+      <c r="H25" s="81"/>
       <c r="I25" s="13"/>
       <c r="J25" s="13"/>
       <c r="K25" s="13"/>
       <c r="L25" s="27"/>
     </row>
     <row r="26" spans="1:12" s="9" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="134" t="s">
+      <c r="A26" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="135"/>
-      <c r="C26" s="135"/>
-      <c r="D26" s="135"/>
-      <c r="E26" s="136"/>
-      <c r="G26" s="74" t="s">
+      <c r="B26" s="60"/>
+      <c r="C26" s="60"/>
+      <c r="D26" s="60"/>
+      <c r="E26" s="61"/>
+      <c r="G26" s="84" t="s">
         <v>89</v>
       </c>
-      <c r="H26" s="75"/>
+      <c r="H26" s="85"/>
       <c r="I26" s="11"/>
       <c r="J26" s="11"/>
       <c r="K26" s="11"/>
       <c r="L26" s="26"/>
     </row>
     <row r="27" spans="1:12" s="9" customFormat="1" ht="12.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="113" t="s">
+      <c r="A27" s="62" t="s">
         <v>56</v>
       </c>
-      <c r="B27" s="111"/>
+      <c r="B27" s="63"/>
       <c r="C27" s="29" t="s">
         <v>55</v>
       </c>
@@ -2754,180 +2811,180 @@
       <c r="E27" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G27" s="77" t="s">
+      <c r="G27" s="80" t="s">
         <v>90</v>
       </c>
-      <c r="H27" s="79"/>
+      <c r="H27" s="81"/>
       <c r="I27" s="13"/>
       <c r="J27" s="13"/>
       <c r="K27" s="13"/>
       <c r="L27" s="27"/>
     </row>
     <row r="28" spans="1:12" s="9" customFormat="1" ht="12.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="131" t="s">
+      <c r="A28" s="78" t="s">
         <v>103</v>
       </c>
-      <c r="B28" s="132"/>
+      <c r="B28" s="79"/>
       <c r="C28" s="8" t="s">
         <v>66</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="6"/>
-      <c r="G28" s="74" t="s">
+      <c r="G28" s="84" t="s">
         <v>91</v>
       </c>
-      <c r="H28" s="75"/>
+      <c r="H28" s="85"/>
       <c r="I28" s="11"/>
       <c r="J28" s="11"/>
       <c r="K28" s="11"/>
       <c r="L28" s="26"/>
     </row>
     <row r="29" spans="1:12" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="74" t="s">
+      <c r="A29" s="84" t="s">
         <v>104</v>
       </c>
-      <c r="B29" s="75"/>
+      <c r="B29" s="85"/>
       <c r="C29" s="11" t="s">
         <v>66</v>
       </c>
       <c r="D29" s="11"/>
       <c r="E29" s="10"/>
-      <c r="G29" s="77" t="s">
+      <c r="G29" s="80" t="s">
         <v>92</v>
       </c>
-      <c r="H29" s="79"/>
+      <c r="H29" s="81"/>
       <c r="I29" s="13"/>
       <c r="J29" s="13"/>
       <c r="K29" s="13"/>
       <c r="L29" s="27"/>
     </row>
     <row r="30" spans="1:12" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="77" t="s">
+      <c r="A30" s="80" t="s">
         <v>105</v>
       </c>
-      <c r="B30" s="79"/>
+      <c r="B30" s="81"/>
       <c r="C30" s="13" t="s">
         <v>66</v>
       </c>
       <c r="D30" s="13"/>
       <c r="E30" s="12"/>
       <c r="F30" s="7"/>
-      <c r="G30" s="74" t="s">
+      <c r="G30" s="84" t="s">
         <v>93</v>
       </c>
-      <c r="H30" s="75"/>
+      <c r="H30" s="85"/>
       <c r="I30" s="11"/>
       <c r="J30" s="11"/>
       <c r="K30" s="11"/>
       <c r="L30" s="26"/>
     </row>
     <row r="31" spans="1:12" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="74"/>
-      <c r="B31" s="75"/>
+      <c r="A31" s="84"/>
+      <c r="B31" s="85"/>
       <c r="C31" s="11"/>
       <c r="D31" s="11"/>
       <c r="E31" s="10"/>
       <c r="F31" s="7"/>
-      <c r="G31" s="77" t="s">
+      <c r="G31" s="80" t="s">
         <v>94</v>
       </c>
-      <c r="H31" s="79"/>
+      <c r="H31" s="81"/>
       <c r="I31" s="13"/>
       <c r="J31" s="13"/>
       <c r="K31" s="13"/>
       <c r="L31" s="27"/>
     </row>
     <row r="32" spans="1:12" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="77"/>
-      <c r="B32" s="79"/>
+      <c r="A32" s="80"/>
+      <c r="B32" s="81"/>
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>
       <c r="E32" s="12"/>
       <c r="F32" s="7"/>
-      <c r="G32" s="74" t="s">
+      <c r="G32" s="84" t="s">
         <v>95</v>
       </c>
-      <c r="H32" s="75"/>
+      <c r="H32" s="85"/>
       <c r="I32" s="11"/>
       <c r="J32" s="11"/>
       <c r="K32" s="11"/>
       <c r="L32" s="26"/>
     </row>
     <row r="33" spans="1:56" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="74"/>
-      <c r="B33" s="75"/>
+      <c r="A33" s="84"/>
+      <c r="B33" s="85"/>
       <c r="C33" s="11"/>
       <c r="D33" s="11"/>
       <c r="E33" s="10"/>
       <c r="F33" s="7"/>
-      <c r="G33" s="77" t="s">
+      <c r="G33" s="80" t="s">
         <v>96</v>
       </c>
-      <c r="H33" s="79"/>
+      <c r="H33" s="81"/>
       <c r="I33" s="13"/>
       <c r="J33" s="13"/>
       <c r="K33" s="13"/>
       <c r="L33" s="27"/>
     </row>
     <row r="34" spans="1:56" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="77"/>
-      <c r="B34" s="79"/>
+      <c r="A34" s="80"/>
+      <c r="B34" s="81"/>
       <c r="C34" s="13"/>
       <c r="D34" s="13"/>
       <c r="E34" s="12"/>
       <c r="F34" s="7"/>
-      <c r="G34" s="74" t="s">
+      <c r="G34" s="84" t="s">
         <v>97</v>
       </c>
-      <c r="H34" s="75"/>
+      <c r="H34" s="85"/>
       <c r="I34" s="11"/>
       <c r="J34" s="11"/>
       <c r="K34" s="11"/>
       <c r="L34" s="26"/>
     </row>
     <row r="35" spans="1:56" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="64"/>
-      <c r="B35" s="64"/>
+      <c r="A35" s="100"/>
+      <c r="B35" s="100"/>
       <c r="C35" s="11"/>
       <c r="D35" s="11"/>
       <c r="E35" s="12"/>
       <c r="F35" s="7"/>
-      <c r="G35" s="77" t="s">
+      <c r="G35" s="80" t="s">
         <v>98</v>
       </c>
-      <c r="H35" s="79"/>
+      <c r="H35" s="81"/>
       <c r="I35" s="13"/>
       <c r="J35" s="13"/>
       <c r="K35" s="13"/>
       <c r="L35" s="27"/>
     </row>
     <row r="36" spans="1:56" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="62"/>
-      <c r="B36" s="62"/>
+      <c r="A36" s="94"/>
+      <c r="B36" s="94"/>
       <c r="C36" s="13"/>
       <c r="D36" s="13"/>
       <c r="E36" s="12"/>
       <c r="F36" s="7"/>
-      <c r="G36" s="74" t="s">
+      <c r="G36" s="84" t="s">
         <v>99</v>
       </c>
-      <c r="H36" s="75"/>
+      <c r="H36" s="85"/>
       <c r="I36" s="11"/>
       <c r="J36" s="11"/>
       <c r="K36" s="11"/>
       <c r="L36" s="26"/>
     </row>
     <row r="37" spans="1:56" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="62"/>
-      <c r="B37" s="62"/>
+      <c r="A37" s="94"/>
+      <c r="B37" s="94"/>
       <c r="C37" s="13"/>
       <c r="D37" s="13"/>
       <c r="E37" s="12"/>
       <c r="F37" s="7"/>
-      <c r="G37" s="77" t="s">
+      <c r="G37" s="80" t="s">
         <v>100</v>
       </c>
-      <c r="H37" s="79"/>
+      <c r="H37" s="81"/>
       <c r="I37" s="13"/>
       <c r="J37" s="13"/>
       <c r="K37" s="13"/>
@@ -2943,16 +3000,16 @@
       <c r="AS37" s="5"/>
     </row>
     <row r="38" spans="1:56" s="9" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="62"/>
-      <c r="B38" s="62"/>
+      <c r="A38" s="94"/>
+      <c r="B38" s="94"/>
       <c r="C38" s="13"/>
       <c r="D38" s="13"/>
       <c r="E38" s="12"/>
       <c r="F38" s="7"/>
-      <c r="G38" s="74" t="s">
+      <c r="G38" s="84" t="s">
         <v>101</v>
       </c>
-      <c r="H38" s="75"/>
+      <c r="H38" s="85"/>
       <c r="I38" s="11"/>
       <c r="J38" s="11"/>
       <c r="K38" s="11"/>
@@ -2968,16 +3025,16 @@
       <c r="AS38" s="5"/>
     </row>
     <row r="39" spans="1:56" s="9" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="64"/>
-      <c r="B39" s="64"/>
+      <c r="A39" s="100"/>
+      <c r="B39" s="100"/>
       <c r="C39" s="11"/>
       <c r="D39" s="11"/>
       <c r="E39" s="12"/>
       <c r="F39" s="7"/>
-      <c r="G39" s="123" t="s">
+      <c r="G39" s="101" t="s">
         <v>102</v>
       </c>
-      <c r="H39" s="124"/>
+      <c r="H39" s="102"/>
       <c r="I39" s="20"/>
       <c r="J39" s="20"/>
       <c r="K39" s="20"/>
@@ -2997,8 +3054,8 @@
       <c r="AS39" s="5"/>
     </row>
     <row r="40" spans="1:56" s="9" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="77"/>
-      <c r="B40" s="79"/>
+      <c r="A40" s="80"/>
+      <c r="B40" s="81"/>
       <c r="C40" s="13"/>
       <c r="D40" s="13"/>
       <c r="E40" s="12"/>
@@ -3028,32 +3085,32 @@
       <c r="BD40" s="5"/>
     </row>
     <row r="41" spans="1:56" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="74"/>
-      <c r="B41" s="75"/>
+      <c r="A41" s="84"/>
+      <c r="B41" s="85"/>
       <c r="C41" s="11"/>
       <c r="D41" s="11"/>
       <c r="E41" s="10"/>
       <c r="F41" s="7"/>
-      <c r="G41" s="134" t="s">
+      <c r="G41" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="H41" s="135"/>
-      <c r="I41" s="135"/>
-      <c r="J41" s="135"/>
-      <c r="K41" s="135"/>
-      <c r="L41" s="136"/>
+      <c r="H41" s="60"/>
+      <c r="I41" s="60"/>
+      <c r="J41" s="60"/>
+      <c r="K41" s="60"/>
+      <c r="L41" s="61"/>
     </row>
     <row r="42" spans="1:56" s="5" customFormat="1" ht="12.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="77"/>
-      <c r="B42" s="79"/>
+      <c r="A42" s="80"/>
+      <c r="B42" s="81"/>
       <c r="C42" s="13"/>
       <c r="D42" s="13"/>
       <c r="E42" s="12"/>
       <c r="F42" s="7"/>
-      <c r="G42" s="113" t="s">
+      <c r="G42" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="H42" s="111"/>
+      <c r="H42" s="63"/>
       <c r="I42" s="51" t="s">
         <v>43</v>
       </c>
@@ -3068,28 +3125,28 @@
       </c>
     </row>
     <row r="43" spans="1:56" s="5" customFormat="1" ht="12.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="129"/>
-      <c r="B43" s="130"/>
+      <c r="A43" s="110"/>
+      <c r="B43" s="111"/>
       <c r="C43" s="35"/>
       <c r="D43" s="35"/>
       <c r="E43" s="34"/>
       <c r="F43" s="7"/>
-      <c r="G43" s="125"/>
-      <c r="H43" s="126"/>
+      <c r="G43" s="103"/>
+      <c r="H43" s="104"/>
       <c r="I43" s="8"/>
       <c r="J43" s="8"/>
       <c r="K43" s="32"/>
       <c r="L43" s="25"/>
     </row>
     <row r="44" spans="1:56" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="123"/>
-      <c r="B44" s="124"/>
+      <c r="A44" s="101"/>
+      <c r="B44" s="102"/>
       <c r="C44" s="20"/>
       <c r="D44" s="20"/>
       <c r="E44" s="14"/>
       <c r="F44" s="7"/>
-      <c r="G44" s="85"/>
-      <c r="H44" s="86"/>
+      <c r="G44" s="66"/>
+      <c r="H44" s="67"/>
       <c r="I44" s="11"/>
       <c r="J44" s="11"/>
       <c r="K44" s="11"/>
@@ -3102,24 +3159,24 @@
       <c r="D45" s="9"/>
       <c r="E45" s="9"/>
       <c r="F45" s="7"/>
-      <c r="G45" s="83"/>
-      <c r="H45" s="84"/>
+      <c r="G45" s="64"/>
+      <c r="H45" s="65"/>
       <c r="I45" s="13"/>
       <c r="J45" s="13"/>
       <c r="K45" s="13"/>
       <c r="L45" s="27"/>
     </row>
     <row r="46" spans="1:56" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="71" t="s">
+      <c r="A46" s="107" t="s">
         <v>2</v>
       </c>
-      <c r="B46" s="72"/>
-      <c r="C46" s="72"/>
-      <c r="D46" s="72"/>
-      <c r="E46" s="73"/>
+      <c r="B46" s="108"/>
+      <c r="C46" s="108"/>
+      <c r="D46" s="108"/>
+      <c r="E46" s="109"/>
       <c r="F46" s="3"/>
-      <c r="G46" s="85"/>
-      <c r="H46" s="86"/>
+      <c r="G46" s="66"/>
+      <c r="H46" s="67"/>
       <c r="I46" s="11"/>
       <c r="J46" s="11"/>
       <c r="K46" s="11"/>
@@ -3142,8 +3199,8 @@
         <v>19</v>
       </c>
       <c r="F47" s="3"/>
-      <c r="G47" s="83"/>
-      <c r="H47" s="84"/>
+      <c r="G47" s="64"/>
+      <c r="H47" s="65"/>
       <c r="I47" s="13"/>
       <c r="J47" s="13"/>
       <c r="K47" s="13"/>
@@ -3158,8 +3215,8 @@
       <c r="D48" s="11"/>
       <c r="E48" s="10"/>
       <c r="F48" s="3"/>
-      <c r="G48" s="85"/>
-      <c r="H48" s="86"/>
+      <c r="G48" s="66"/>
+      <c r="H48" s="67"/>
       <c r="I48" s="11"/>
       <c r="J48" s="11"/>
       <c r="K48" s="11"/>
@@ -3174,8 +3231,8 @@
       <c r="D49" s="13"/>
       <c r="E49" s="12"/>
       <c r="F49" s="3"/>
-      <c r="G49" s="83"/>
-      <c r="H49" s="84"/>
+      <c r="G49" s="64"/>
+      <c r="H49" s="65"/>
       <c r="I49" s="13"/>
       <c r="J49" s="13"/>
       <c r="K49" s="13"/>
@@ -3190,8 +3247,8 @@
       <c r="D50" s="11"/>
       <c r="E50" s="10"/>
       <c r="F50" s="3"/>
-      <c r="G50" s="85"/>
-      <c r="H50" s="86"/>
+      <c r="G50" s="66"/>
+      <c r="H50" s="67"/>
       <c r="I50" s="11"/>
       <c r="J50" s="11"/>
       <c r="K50" s="11"/>
@@ -3206,8 +3263,8 @@
       <c r="D51" s="13"/>
       <c r="E51" s="12"/>
       <c r="F51" s="3"/>
-      <c r="G51" s="83"/>
-      <c r="H51" s="84"/>
+      <c r="G51" s="64"/>
+      <c r="H51" s="65"/>
       <c r="I51" s="13"/>
       <c r="J51" s="13"/>
       <c r="K51" s="13"/>
@@ -3222,24 +3279,24 @@
       <c r="D52" s="11"/>
       <c r="E52" s="10"/>
       <c r="F52" s="3"/>
-      <c r="G52" s="85"/>
-      <c r="H52" s="86"/>
+      <c r="G52" s="66"/>
+      <c r="H52" s="67"/>
       <c r="I52" s="11"/>
       <c r="J52" s="11"/>
       <c r="K52" s="11"/>
       <c r="L52" s="26"/>
     </row>
     <row r="53" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="120" t="s">
+      <c r="A53" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="B53" s="121"/>
-      <c r="C53" s="122"/>
+      <c r="B53" s="98"/>
+      <c r="C53" s="99"/>
       <c r="D53" s="30"/>
       <c r="E53" s="17"/>
       <c r="F53" s="3"/>
-      <c r="G53" s="116"/>
-      <c r="H53" s="117"/>
+      <c r="G53" s="125"/>
+      <c r="H53" s="126"/>
       <c r="I53" s="13"/>
       <c r="J53" s="13"/>
       <c r="K53" s="13"/>
@@ -3249,17 +3306,17 @@
       <c r="A54" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="B54" s="110" t="s">
+      <c r="B54" s="112" t="s">
         <v>20</v>
       </c>
-      <c r="C54" s="111"/>
-      <c r="D54" s="110" t="s">
+      <c r="C54" s="63"/>
+      <c r="D54" s="112" t="s">
         <v>106</v>
       </c>
-      <c r="E54" s="112"/>
+      <c r="E54" s="113"/>
       <c r="F54" s="3"/>
-      <c r="G54" s="85"/>
-      <c r="H54" s="86"/>
+      <c r="G54" s="66"/>
+      <c r="H54" s="67"/>
       <c r="I54" s="11"/>
       <c r="J54" s="11"/>
       <c r="K54" s="11"/>
@@ -3267,13 +3324,13 @@
     </row>
     <row r="55" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="37"/>
-      <c r="B55" s="80"/>
-      <c r="C55" s="82"/>
-      <c r="D55" s="80"/>
-      <c r="E55" s="81"/>
+      <c r="B55" s="114"/>
+      <c r="C55" s="115"/>
+      <c r="D55" s="114"/>
+      <c r="E55" s="116"/>
       <c r="F55" s="3"/>
-      <c r="G55" s="83"/>
-      <c r="H55" s="84"/>
+      <c r="G55" s="64"/>
+      <c r="H55" s="65"/>
       <c r="I55" s="13"/>
       <c r="J55" s="13"/>
       <c r="K55" s="13"/>
@@ -3281,24 +3338,24 @@
     </row>
     <row r="56" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F56" s="3"/>
-      <c r="G56" s="118"/>
-      <c r="H56" s="119"/>
+      <c r="G56" s="95"/>
+      <c r="H56" s="96"/>
       <c r="I56" s="11"/>
       <c r="J56" s="11"/>
       <c r="K56" s="11"/>
       <c r="L56" s="26"/>
     </row>
     <row r="57" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="71" t="s">
+      <c r="A57" s="107" t="s">
         <v>116</v>
       </c>
-      <c r="B57" s="72"/>
-      <c r="C57" s="72"/>
-      <c r="D57" s="72"/>
-      <c r="E57" s="73"/>
+      <c r="B57" s="108"/>
+      <c r="C57" s="108"/>
+      <c r="D57" s="108"/>
+      <c r="E57" s="109"/>
       <c r="F57" s="3"/>
-      <c r="G57" s="83"/>
-      <c r="H57" s="84"/>
+      <c r="G57" s="64"/>
+      <c r="H57" s="65"/>
       <c r="I57" s="13"/>
       <c r="J57" s="13"/>
       <c r="K57" s="13"/>
@@ -3321,8 +3378,8 @@
         <v>19</v>
       </c>
       <c r="F58" s="3"/>
-      <c r="G58" s="85"/>
-      <c r="H58" s="86"/>
+      <c r="G58" s="66"/>
+      <c r="H58" s="67"/>
       <c r="I58" s="11"/>
       <c r="J58" s="11"/>
       <c r="K58" s="11"/>
@@ -3337,8 +3394,8 @@
       <c r="D59" s="11"/>
       <c r="E59" s="10"/>
       <c r="F59" s="3"/>
-      <c r="G59" s="83"/>
-      <c r="H59" s="84"/>
+      <c r="G59" s="64"/>
+      <c r="H59" s="65"/>
       <c r="I59" s="13"/>
       <c r="J59" s="13"/>
       <c r="K59" s="13"/>
@@ -3353,8 +3410,8 @@
       <c r="D60" s="13"/>
       <c r="E60" s="12"/>
       <c r="F60" s="3"/>
-      <c r="G60" s="85"/>
-      <c r="H60" s="86"/>
+      <c r="G60" s="66"/>
+      <c r="H60" s="67"/>
       <c r="I60" s="11"/>
       <c r="J60" s="11"/>
       <c r="K60" s="11"/>
@@ -3369,8 +3426,8 @@
       <c r="D61" s="11"/>
       <c r="E61" s="10"/>
       <c r="F61" s="3"/>
-      <c r="G61" s="83"/>
-      <c r="H61" s="84"/>
+      <c r="G61" s="64"/>
+      <c r="H61" s="65"/>
       <c r="I61" s="13"/>
       <c r="J61" s="13"/>
       <c r="K61" s="13"/>
@@ -3385,8 +3442,8 @@
       <c r="D62" s="13"/>
       <c r="E62" s="12"/>
       <c r="F62" s="3"/>
-      <c r="G62" s="85"/>
-      <c r="H62" s="86"/>
+      <c r="G62" s="66"/>
+      <c r="H62" s="67"/>
       <c r="I62" s="11"/>
       <c r="J62" s="11"/>
       <c r="K62" s="11"/>
@@ -3401,24 +3458,24 @@
       <c r="D63" s="11"/>
       <c r="E63" s="10"/>
       <c r="F63" s="3"/>
-      <c r="G63" s="83"/>
-      <c r="H63" s="84"/>
+      <c r="G63" s="64"/>
+      <c r="H63" s="65"/>
       <c r="I63" s="13"/>
       <c r="J63" s="13"/>
       <c r="K63" s="13"/>
       <c r="L63" s="27"/>
     </row>
     <row r="64" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="89" t="s">
+      <c r="A64" s="143" t="s">
         <v>14</v>
       </c>
-      <c r="B64" s="90"/>
-      <c r="C64" s="91"/>
+      <c r="B64" s="144"/>
+      <c r="C64" s="145"/>
       <c r="D64" s="30"/>
       <c r="E64" s="17"/>
       <c r="F64" s="3"/>
-      <c r="G64" s="85"/>
-      <c r="H64" s="86"/>
+      <c r="G64" s="66"/>
+      <c r="H64" s="67"/>
       <c r="I64" s="11"/>
       <c r="J64" s="11"/>
       <c r="K64" s="11"/>
@@ -3428,17 +3485,17 @@
       <c r="A65" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="B65" s="110" t="s">
+      <c r="B65" s="112" t="s">
         <v>20</v>
       </c>
-      <c r="C65" s="111"/>
-      <c r="D65" s="110" t="s">
+      <c r="C65" s="63"/>
+      <c r="D65" s="112" t="s">
         <v>106</v>
       </c>
-      <c r="E65" s="112"/>
+      <c r="E65" s="113"/>
       <c r="F65" s="3"/>
-      <c r="G65" s="83"/>
-      <c r="H65" s="84"/>
+      <c r="G65" s="64"/>
+      <c r="H65" s="65"/>
       <c r="I65" s="13"/>
       <c r="J65" s="13"/>
       <c r="K65" s="13"/>
@@ -3446,13 +3503,13 @@
     </row>
     <row r="66" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="37"/>
-      <c r="B66" s="80"/>
-      <c r="C66" s="82"/>
-      <c r="D66" s="80"/>
-      <c r="E66" s="81"/>
+      <c r="B66" s="114"/>
+      <c r="C66" s="115"/>
+      <c r="D66" s="114"/>
+      <c r="E66" s="116"/>
       <c r="F66" s="3"/>
-      <c r="G66" s="85"/>
-      <c r="H66" s="86"/>
+      <c r="G66" s="66"/>
+      <c r="H66" s="67"/>
       <c r="I66" s="11"/>
       <c r="J66" s="11"/>
       <c r="K66" s="11"/>
@@ -3460,34 +3517,34 @@
     </row>
     <row r="67" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F67" s="3"/>
-      <c r="G67" s="83"/>
-      <c r="H67" s="84"/>
+      <c r="G67" s="64"/>
+      <c r="H67" s="65"/>
       <c r="I67" s="13"/>
       <c r="J67" s="13"/>
       <c r="K67" s="13"/>
       <c r="L67" s="27"/>
     </row>
     <row r="68" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="95" t="s">
+      <c r="A68" s="117" t="s">
         <v>6</v>
       </c>
-      <c r="B68" s="96"/>
-      <c r="C68" s="96"/>
-      <c r="D68" s="96"/>
-      <c r="E68" s="97"/>
+      <c r="B68" s="118"/>
+      <c r="C68" s="118"/>
+      <c r="D68" s="118"/>
+      <c r="E68" s="119"/>
       <c r="F68" s="3"/>
-      <c r="G68" s="85"/>
-      <c r="H68" s="86"/>
+      <c r="G68" s="66"/>
+      <c r="H68" s="67"/>
       <c r="I68" s="11"/>
       <c r="J68" s="11"/>
       <c r="K68" s="11"/>
       <c r="L68" s="26"/>
     </row>
     <row r="69" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="113" t="s">
+      <c r="A69" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="B69" s="111"/>
+      <c r="B69" s="63"/>
       <c r="C69" s="29" t="s">
         <v>43</v>
       </c>
@@ -3498,66 +3555,66 @@
         <v>44</v>
       </c>
       <c r="F69" s="3"/>
-      <c r="G69" s="83"/>
-      <c r="H69" s="84"/>
+      <c r="G69" s="64"/>
+      <c r="H69" s="65"/>
       <c r="I69" s="13"/>
       <c r="J69" s="13"/>
       <c r="K69" s="13"/>
       <c r="L69" s="27"/>
     </row>
     <row r="70" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="114"/>
-      <c r="B70" s="115"/>
+      <c r="A70" s="120"/>
+      <c r="B70" s="121"/>
       <c r="C70" s="32"/>
       <c r="D70" s="32"/>
       <c r="E70" s="31"/>
       <c r="F70" s="3"/>
-      <c r="G70" s="85"/>
-      <c r="H70" s="86"/>
+      <c r="G70" s="66"/>
+      <c r="H70" s="67"/>
       <c r="I70" s="11"/>
       <c r="J70" s="11"/>
       <c r="K70" s="11"/>
       <c r="L70" s="26"/>
     </row>
     <row r="71" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="63"/>
-      <c r="B71" s="64"/>
+      <c r="A71" s="131"/>
+      <c r="B71" s="100"/>
       <c r="C71" s="11"/>
       <c r="D71" s="11"/>
       <c r="E71" s="10"/>
       <c r="F71" s="3"/>
-      <c r="G71" s="83"/>
-      <c r="H71" s="84"/>
+      <c r="G71" s="64"/>
+      <c r="H71" s="65"/>
       <c r="I71" s="13"/>
       <c r="J71" s="13"/>
       <c r="K71" s="13"/>
       <c r="L71" s="27"/>
     </row>
     <row r="72" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="108"/>
-      <c r="B72" s="109"/>
+      <c r="A72" s="139"/>
+      <c r="B72" s="140"/>
       <c r="C72" s="39"/>
       <c r="D72" s="39"/>
       <c r="E72" s="40"/>
       <c r="F72" s="3"/>
-      <c r="G72" s="85"/>
-      <c r="H72" s="86"/>
+      <c r="G72" s="66"/>
+      <c r="H72" s="67"/>
       <c r="I72" s="11"/>
       <c r="J72" s="11"/>
       <c r="K72" s="11"/>
       <c r="L72" s="26"/>
     </row>
     <row r="73" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="92" t="s">
+      <c r="A73" s="122" t="s">
         <v>108</v>
       </c>
-      <c r="B73" s="93"/>
-      <c r="C73" s="93"/>
-      <c r="D73" s="94"/>
+      <c r="B73" s="123"/>
+      <c r="C73" s="123"/>
+      <c r="D73" s="124"/>
       <c r="E73" s="38"/>
       <c r="F73" s="3"/>
-      <c r="G73" s="83"/>
-      <c r="H73" s="84"/>
+      <c r="G73" s="64"/>
+      <c r="H73" s="65"/>
       <c r="I73" s="13"/>
       <c r="J73" s="13"/>
       <c r="K73" s="13"/>
@@ -3565,46 +3622,46 @@
     </row>
     <row r="74" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F74" s="3"/>
-      <c r="G74" s="85"/>
-      <c r="H74" s="86"/>
+      <c r="G74" s="66"/>
+      <c r="H74" s="67"/>
       <c r="I74" s="11"/>
       <c r="J74" s="11"/>
       <c r="K74" s="11"/>
       <c r="L74" s="26"/>
     </row>
     <row r="75" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="98" t="s">
+      <c r="A75" s="127" t="s">
         <v>80</v>
       </c>
-      <c r="B75" s="99"/>
-      <c r="C75" s="99"/>
-      <c r="D75" s="99"/>
-      <c r="E75" s="100"/>
+      <c r="B75" s="128"/>
+      <c r="C75" s="128"/>
+      <c r="D75" s="128"/>
+      <c r="E75" s="129"/>
       <c r="F75" s="3"/>
-      <c r="G75" s="83"/>
-      <c r="H75" s="84"/>
+      <c r="G75" s="64"/>
+      <c r="H75" s="65"/>
       <c r="I75" s="13"/>
       <c r="J75" s="13"/>
       <c r="K75" s="13"/>
       <c r="L75" s="27"/>
     </row>
     <row r="76" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="77" t="s">
+      <c r="A76" s="80" t="s">
         <v>50</v>
       </c>
-      <c r="B76" s="78"/>
-      <c r="C76" s="78"/>
-      <c r="D76" s="79"/>
+      <c r="B76" s="130"/>
+      <c r="C76" s="130"/>
+      <c r="D76" s="81"/>
       <c r="E76" s="19"/>
       <c r="F76" s="3"/>
     </row>
     <row r="77" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="74" t="s">
+      <c r="A77" s="84" t="s">
         <v>51</v>
       </c>
-      <c r="B77" s="76"/>
-      <c r="C77" s="76"/>
-      <c r="D77" s="75"/>
+      <c r="B77" s="149"/>
+      <c r="C77" s="149"/>
+      <c r="D77" s="85"/>
       <c r="E77" s="18"/>
       <c r="F77" s="3"/>
       <c r="G77" s="47" t="s">
@@ -3617,12 +3674,12 @@
       <c r="L77" s="49"/>
     </row>
     <row r="78" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="77" t="s">
+      <c r="A78" s="80" t="s">
         <v>52</v>
       </c>
-      <c r="B78" s="78"/>
-      <c r="C78" s="78"/>
-      <c r="D78" s="79"/>
+      <c r="B78" s="130"/>
+      <c r="C78" s="130"/>
+      <c r="D78" s="81"/>
       <c r="E78" s="19"/>
       <c r="F78" s="3"/>
       <c r="G78" s="50" t="s">
@@ -3645,12 +3702,12 @@
       </c>
     </row>
     <row r="79" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="74" t="s">
+      <c r="A79" s="84" t="s">
         <v>53</v>
       </c>
-      <c r="B79" s="76"/>
-      <c r="C79" s="76"/>
-      <c r="D79" s="75"/>
+      <c r="B79" s="149"/>
+      <c r="C79" s="149"/>
+      <c r="D79" s="85"/>
       <c r="E79" s="18"/>
       <c r="F79" s="3"/>
       <c r="G79" s="45" t="s">
@@ -3663,12 +3720,12 @@
       <c r="L79" s="13"/>
     </row>
     <row r="80" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="65" t="s">
+      <c r="A80" s="146" t="s">
         <v>54</v>
       </c>
-      <c r="B80" s="66"/>
-      <c r="C80" s="66"/>
-      <c r="D80" s="67"/>
+      <c r="B80" s="147"/>
+      <c r="C80" s="147"/>
+      <c r="D80" s="148"/>
       <c r="E80" s="44"/>
       <c r="F80" s="3"/>
       <c r="G80" s="46" t="s">
@@ -3692,13 +3749,13 @@
       <c r="L81" s="13"/>
     </row>
     <row r="82" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="95" t="s">
+      <c r="A82" s="117" t="s">
         <v>4</v>
       </c>
-      <c r="B82" s="96"/>
-      <c r="C82" s="96"/>
-      <c r="D82" s="96"/>
-      <c r="E82" s="97"/>
+      <c r="B82" s="118"/>
+      <c r="C82" s="118"/>
+      <c r="D82" s="118"/>
+      <c r="E82" s="119"/>
       <c r="F82" s="3"/>
       <c r="G82" s="46" t="s">
         <v>111</v>
@@ -3710,10 +3767,10 @@
       <c r="L82" s="11"/>
     </row>
     <row r="83" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="113" t="s">
+      <c r="A83" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="B83" s="111"/>
+      <c r="B83" s="63"/>
       <c r="C83" s="29" t="s">
         <v>34</v>
       </c>
@@ -3734,8 +3791,8 @@
       <c r="L83" s="43"/>
     </row>
     <row r="84" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="127"/>
-      <c r="B84" s="128"/>
+      <c r="A84" s="105"/>
+      <c r="B84" s="106"/>
       <c r="C84" s="11"/>
       <c r="D84" s="11"/>
       <c r="E84" s="10"/>
@@ -3745,149 +3802,195 @@
       </c>
       <c r="H84" s="42"/>
     </row>
-    <row r="85" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="77"/>
-      <c r="B85" s="79"/>
+    <row r="85" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="80"/>
+      <c r="B85" s="81"/>
       <c r="C85" s="13"/>
       <c r="D85" s="13"/>
       <c r="E85" s="12"/>
       <c r="F85" s="3"/>
     </row>
-    <row r="86" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="74"/>
-      <c r="B86" s="75"/>
+    <row r="86" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="84"/>
+      <c r="B86" s="85"/>
       <c r="C86" s="11"/>
       <c r="D86" s="11"/>
       <c r="E86" s="10"/>
       <c r="F86" s="3"/>
-    </row>
-    <row r="87" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="77"/>
-      <c r="B87" s="79"/>
+      <c r="G86" s="59" t="s">
+        <v>128</v>
+      </c>
+      <c r="H86" s="152"/>
+    </row>
+    <row r="87" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="80"/>
+      <c r="B87" s="81"/>
       <c r="C87" s="13"/>
       <c r="D87" s="13"/>
       <c r="E87" s="12"/>
       <c r="F87" s="3"/>
-    </row>
-    <row r="88" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="74"/>
-      <c r="B88" s="75"/>
+      <c r="G87" s="58" t="s">
+        <v>126</v>
+      </c>
+      <c r="H87" s="58" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="84"/>
+      <c r="B88" s="85"/>
       <c r="C88" s="11"/>
       <c r="D88" s="11"/>
       <c r="E88" s="10"/>
       <c r="F88" s="3"/>
+      <c r="G88" s="150" t="s">
+        <v>117</v>
+      </c>
+      <c r="H88" s="150"/>
     </row>
     <row r="89" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="77"/>
-      <c r="B89" s="79"/>
+      <c r="A89" s="80"/>
+      <c r="B89" s="81"/>
       <c r="C89" s="13"/>
       <c r="D89" s="13"/>
       <c r="E89" s="12"/>
       <c r="F89" s="3"/>
+      <c r="G89" s="151" t="s">
+        <v>118</v>
+      </c>
+      <c r="H89" s="151"/>
     </row>
     <row r="90" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="74"/>
-      <c r="B90" s="75"/>
+      <c r="A90" s="84"/>
+      <c r="B90" s="85"/>
       <c r="C90" s="11"/>
       <c r="D90" s="11"/>
       <c r="E90" s="10"/>
       <c r="F90" s="3"/>
+      <c r="G90" s="150" t="s">
+        <v>119</v>
+      </c>
+      <c r="H90" s="150"/>
     </row>
     <row r="91" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="77"/>
-      <c r="B91" s="79"/>
+      <c r="A91" s="80"/>
+      <c r="B91" s="81"/>
       <c r="C91" s="13"/>
       <c r="D91" s="13"/>
       <c r="E91" s="12"/>
       <c r="F91" s="3"/>
+      <c r="G91" s="151" t="s">
+        <v>120</v>
+      </c>
+      <c r="H91" s="150"/>
     </row>
     <row r="92" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="74"/>
-      <c r="B92" s="75"/>
+      <c r="A92" s="84"/>
+      <c r="B92" s="85"/>
       <c r="C92" s="11"/>
       <c r="D92" s="11"/>
       <c r="E92" s="10"/>
       <c r="F92" s="3"/>
+      <c r="G92" s="150" t="s">
+        <v>121</v>
+      </c>
+      <c r="H92" s="151"/>
     </row>
     <row r="93" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="77"/>
-      <c r="B93" s="79"/>
+      <c r="A93" s="80"/>
+      <c r="B93" s="81"/>
       <c r="C93" s="13"/>
       <c r="D93" s="13"/>
       <c r="E93" s="12"/>
       <c r="F93" s="3"/>
+      <c r="G93" s="151" t="s">
+        <v>122</v>
+      </c>
+      <c r="H93" s="150"/>
     </row>
     <row r="94" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="74"/>
-      <c r="B94" s="75"/>
+      <c r="A94" s="84"/>
+      <c r="B94" s="85"/>
       <c r="C94" s="11"/>
       <c r="D94" s="11"/>
       <c r="E94" s="10"/>
       <c r="F94" s="3"/>
+      <c r="G94" s="150" t="s">
+        <v>123</v>
+      </c>
+      <c r="H94" s="150"/>
     </row>
     <row r="95" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="77"/>
-      <c r="B95" s="79"/>
+      <c r="A95" s="80"/>
+      <c r="B95" s="81"/>
       <c r="C95" s="13"/>
       <c r="D95" s="13"/>
       <c r="E95" s="12"/>
       <c r="F95" s="3"/>
+      <c r="G95" s="151" t="s">
+        <v>124</v>
+      </c>
+      <c r="H95" s="151"/>
     </row>
     <row r="96" spans="1:12" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="74"/>
-      <c r="B96" s="75"/>
+      <c r="A96" s="84"/>
+      <c r="B96" s="85"/>
       <c r="C96" s="11"/>
       <c r="D96" s="11"/>
       <c r="E96" s="10"/>
       <c r="F96" s="3"/>
+      <c r="G96" s="150" t="s">
+        <v>125</v>
+      </c>
+      <c r="H96" s="150"/>
     </row>
     <row r="97" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="77"/>
-      <c r="B97" s="79"/>
+      <c r="A97" s="80"/>
+      <c r="B97" s="81"/>
       <c r="C97" s="13"/>
       <c r="D97" s="13"/>
       <c r="E97" s="12"/>
       <c r="F97" s="3"/>
     </row>
     <row r="98" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="74"/>
-      <c r="B98" s="75"/>
+      <c r="A98" s="84"/>
+      <c r="B98" s="85"/>
       <c r="C98" s="11"/>
       <c r="D98" s="11"/>
       <c r="E98" s="10"/>
       <c r="F98" s="3"/>
     </row>
     <row r="99" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="77"/>
-      <c r="B99" s="79"/>
+      <c r="A99" s="80"/>
+      <c r="B99" s="81"/>
       <c r="C99" s="13"/>
       <c r="D99" s="13"/>
       <c r="E99" s="12"/>
       <c r="F99" s="3"/>
     </row>
     <row r="100" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="74"/>
-      <c r="B100" s="75"/>
+      <c r="A100" s="84"/>
+      <c r="B100" s="85"/>
       <c r="C100" s="11"/>
       <c r="D100" s="11"/>
       <c r="E100" s="10"/>
       <c r="F100" s="3"/>
     </row>
     <row r="101" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="87"/>
-      <c r="B101" s="88"/>
+      <c r="A101" s="141"/>
+      <c r="B101" s="142"/>
       <c r="C101" s="13"/>
       <c r="D101" s="13"/>
       <c r="E101" s="12"/>
       <c r="F101" s="3"/>
     </row>
     <row r="102" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="92" t="s">
+      <c r="A102" s="122" t="s">
         <v>14</v>
       </c>
-      <c r="B102" s="93"/>
-      <c r="C102" s="93"/>
-      <c r="D102" s="94"/>
+      <c r="B102" s="123"/>
+      <c r="C102" s="123"/>
+      <c r="D102" s="124"/>
       <c r="E102" s="38"/>
       <c r="F102" s="3"/>
     </row>
@@ -3895,20 +3998,20 @@
       <c r="F103" s="3"/>
     </row>
     <row r="104" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="101" t="s">
+      <c r="A104" s="132" t="s">
         <v>7</v>
       </c>
-      <c r="B104" s="102"/>
-      <c r="C104" s="102"/>
-      <c r="D104" s="102"/>
-      <c r="E104" s="103"/>
+      <c r="B104" s="133"/>
+      <c r="C104" s="133"/>
+      <c r="D104" s="133"/>
+      <c r="E104" s="134"/>
       <c r="F104" s="3"/>
     </row>
     <row r="105" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="104" t="s">
+      <c r="A105" s="135" t="s">
         <v>45</v>
       </c>
-      <c r="B105" s="105"/>
+      <c r="B105" s="136"/>
       <c r="C105" s="21" t="s">
         <v>109</v>
       </c>
@@ -3921,156 +4024,156 @@
       <c r="F105" s="3"/>
     </row>
     <row r="106" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="106"/>
-      <c r="B106" s="107"/>
+      <c r="A106" s="137"/>
+      <c r="B106" s="138"/>
       <c r="C106" s="8"/>
       <c r="D106" s="8"/>
       <c r="E106" s="6"/>
       <c r="F106" s="3"/>
     </row>
     <row r="107" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="63"/>
-      <c r="B107" s="64"/>
+      <c r="A107" s="131"/>
+      <c r="B107" s="100"/>
       <c r="C107" s="11"/>
       <c r="D107" s="11"/>
       <c r="E107" s="10"/>
       <c r="F107" s="3"/>
     </row>
     <row r="108" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="61"/>
-      <c r="B108" s="62"/>
+      <c r="A108" s="93"/>
+      <c r="B108" s="94"/>
       <c r="C108" s="8"/>
       <c r="D108" s="8"/>
       <c r="E108" s="6"/>
       <c r="F108" s="3"/>
     </row>
     <row r="109" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="63"/>
-      <c r="B109" s="64"/>
+      <c r="A109" s="131"/>
+      <c r="B109" s="100"/>
       <c r="C109" s="11"/>
       <c r="D109" s="11"/>
       <c r="E109" s="10"/>
       <c r="F109" s="3"/>
     </row>
     <row r="110" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="61"/>
-      <c r="B110" s="62"/>
+      <c r="A110" s="93"/>
+      <c r="B110" s="94"/>
       <c r="C110" s="8"/>
       <c r="D110" s="8"/>
       <c r="E110" s="6"/>
       <c r="F110" s="3"/>
     </row>
     <row r="111" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="63"/>
-      <c r="B111" s="64"/>
+      <c r="A111" s="131"/>
+      <c r="B111" s="100"/>
       <c r="C111" s="11"/>
       <c r="D111" s="11"/>
       <c r="E111" s="10"/>
       <c r="F111" s="3"/>
     </row>
     <row r="112" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="61"/>
-      <c r="B112" s="62"/>
+      <c r="A112" s="93"/>
+      <c r="B112" s="94"/>
       <c r="C112" s="8"/>
       <c r="D112" s="8"/>
       <c r="E112" s="6"/>
       <c r="F112" s="3"/>
     </row>
     <row r="113" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="63"/>
-      <c r="B113" s="64"/>
+      <c r="A113" s="131"/>
+      <c r="B113" s="100"/>
       <c r="C113" s="11"/>
       <c r="D113" s="11"/>
       <c r="E113" s="10"/>
       <c r="F113" s="3"/>
     </row>
     <row r="114" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="61"/>
-      <c r="B114" s="62"/>
+      <c r="A114" s="93"/>
+      <c r="B114" s="94"/>
       <c r="C114" s="13"/>
       <c r="D114" s="13"/>
       <c r="E114" s="6"/>
       <c r="F114" s="3"/>
     </row>
     <row r="115" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="63"/>
-      <c r="B115" s="64"/>
+      <c r="A115" s="131"/>
+      <c r="B115" s="100"/>
       <c r="C115" s="11"/>
       <c r="D115" s="11"/>
       <c r="E115" s="10"/>
       <c r="F115" s="3"/>
     </row>
     <row r="116" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="61"/>
-      <c r="B116" s="62"/>
+      <c r="A116" s="93"/>
+      <c r="B116" s="94"/>
       <c r="C116" s="13"/>
       <c r="D116" s="13"/>
       <c r="E116" s="6"/>
       <c r="F116" s="3"/>
     </row>
     <row r="117" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="63"/>
-      <c r="B117" s="64"/>
+      <c r="A117" s="131"/>
+      <c r="B117" s="100"/>
       <c r="C117" s="11"/>
       <c r="D117" s="11"/>
       <c r="E117" s="10"/>
       <c r="F117" s="3"/>
     </row>
     <row r="118" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="61"/>
-      <c r="B118" s="62"/>
+      <c r="A118" s="93"/>
+      <c r="B118" s="94"/>
       <c r="C118" s="13"/>
       <c r="D118" s="13"/>
       <c r="E118" s="6"/>
       <c r="F118" s="3"/>
     </row>
     <row r="119" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="63"/>
-      <c r="B119" s="64"/>
+      <c r="A119" s="131"/>
+      <c r="B119" s="100"/>
       <c r="C119" s="11"/>
       <c r="D119" s="11"/>
       <c r="E119" s="10"/>
       <c r="F119" s="3"/>
     </row>
     <row r="120" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="61"/>
-      <c r="B120" s="62"/>
+      <c r="A120" s="93"/>
+      <c r="B120" s="94"/>
       <c r="C120" s="13"/>
       <c r="D120" s="13"/>
       <c r="E120" s="12"/>
       <c r="F120" s="3"/>
     </row>
     <row r="121" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="63"/>
-      <c r="B121" s="64"/>
+      <c r="A121" s="131"/>
+      <c r="B121" s="100"/>
       <c r="C121" s="11"/>
       <c r="D121" s="11"/>
       <c r="E121" s="10"/>
       <c r="F121" s="3"/>
     </row>
     <row r="122" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="61"/>
-      <c r="B122" s="62"/>
+      <c r="A122" s="93"/>
+      <c r="B122" s="94"/>
       <c r="C122" s="13"/>
       <c r="D122" s="13"/>
       <c r="E122" s="12"/>
       <c r="F122" s="3"/>
     </row>
     <row r="123" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="63"/>
-      <c r="B123" s="64"/>
+      <c r="A123" s="131"/>
+      <c r="B123" s="100"/>
       <c r="C123" s="11"/>
       <c r="D123" s="11"/>
       <c r="E123" s="10"/>
       <c r="F123" s="3"/>
     </row>
     <row r="124" spans="1:6" s="5" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="92" t="s">
+      <c r="A124" s="122" t="s">
         <v>114</v>
       </c>
-      <c r="B124" s="93"/>
-      <c r="C124" s="93"/>
-      <c r="D124" s="94"/>
+      <c r="B124" s="123"/>
+      <c r="C124" s="123"/>
+      <c r="D124" s="124"/>
       <c r="E124" s="38"/>
       <c r="F124" s="3"/>
     </row>
@@ -4646,7 +4749,167 @@
       <c r="E219" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="183">
+  <mergeCells count="184">
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A116:B116"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="A80:D80"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A57:E57"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A77:D77"/>
+    <mergeCell ref="A78:D78"/>
+    <mergeCell ref="A79:D79"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="A114:B114"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="G59:H59"/>
+    <mergeCell ref="G60:H60"/>
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="G71:H71"/>
+    <mergeCell ref="G72:H72"/>
+    <mergeCell ref="G73:H73"/>
+    <mergeCell ref="G74:H74"/>
+    <mergeCell ref="G75:H75"/>
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="G67:H67"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="G69:H69"/>
+    <mergeCell ref="A102:D102"/>
+    <mergeCell ref="A68:E68"/>
+    <mergeCell ref="G86:H86"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="A124:D124"/>
+    <mergeCell ref="A75:E75"/>
+    <mergeCell ref="A76:D76"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="A104:E104"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="G62:H62"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="A73:D73"/>
+    <mergeCell ref="G61:H61"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="G70:H70"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="A53:C53"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="A46:E46"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="A82:E82"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="A13:D13"/>
     <mergeCell ref="G41:L41"/>
     <mergeCell ref="G42:H42"/>
     <mergeCell ref="G63:H63"/>
@@ -4671,165 +4934,6 @@
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="A14:D14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="A53:C53"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="G57:H57"/>
-    <mergeCell ref="A46:E46"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="A82:E82"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="A73:D73"/>
-    <mergeCell ref="G61:H61"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="G52:H52"/>
-    <mergeCell ref="G70:H70"/>
-    <mergeCell ref="G53:H53"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="A124:D124"/>
-    <mergeCell ref="A75:E75"/>
-    <mergeCell ref="A76:D76"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="A104:E104"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="G62:H62"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="G59:H59"/>
-    <mergeCell ref="G60:H60"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="G71:H71"/>
-    <mergeCell ref="G72:H72"/>
-    <mergeCell ref="G73:H73"/>
-    <mergeCell ref="G74:H74"/>
-    <mergeCell ref="G75:H75"/>
-    <mergeCell ref="A64:C64"/>
-    <mergeCell ref="G66:H66"/>
-    <mergeCell ref="G67:H67"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="G69:H69"/>
-    <mergeCell ref="A102:D102"/>
-    <mergeCell ref="A68:E68"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A116:B116"/>
-    <mergeCell ref="A117:B117"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="A80:D80"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="A57:E57"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A77:D77"/>
-    <mergeCell ref="A78:D78"/>
-    <mergeCell ref="A79:D79"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="A114:B114"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A39:B39"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
1.       Tremco 201 and 250 GC.  Add two lines to material and labor pages, to add an extra 30 mils. 2.       Text box for notes to be exported to summary sheet.  “NOTES TO BILL.” 3.       Replicated sheets  the title of the replicated sheet reflects the “work area” that it is named on the job set up page.
</commit_message>
<xml_diff>
--- a/WICR Estimator/SummaryTemplate.xlsx
+++ b/WICR Estimator/SummaryTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\priya\Downloads\WICR Estimator\WICR Estimator\WICR Estimator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\priya\Downloads\WICR Estimator_No Apply button\WICR Estimator\WICR Estimator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55585C20-3965-41C5-B4D3-B408A521E5B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC50BD0-EB52-4879-87AE-8D8803FF2411}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="347" xr2:uid="{C3BB3D69-FD31-4C45-AAE2-714CBD52CC32}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="130">
   <si>
     <t>Job Setup</t>
   </si>
@@ -432,6 +432,9 @@
   </si>
   <si>
     <t>Cost Calculation Details</t>
+  </si>
+  <si>
+    <t>Notes to Bill:</t>
   </si>
 </sst>
 </file>
@@ -494,7 +497,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="63">
+  <borders count="71">
     <border>
       <left/>
       <right/>
@@ -1326,12 +1329,94 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyProtection="1"/>
@@ -1339,54 +1424,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="5" fillId="3" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="3" borderId="35" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="3" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="3" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="5" fillId="3" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1399,42 +1439,15 @@
     <xf numFmtId="2" fontId="5" fillId="3" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="5" fillId="3" borderId="40" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="5" fillId="3" borderId="41" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="3" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="3" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="3" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="42" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="5" fillId="3" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="3" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="3" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="3" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="5" fillId="3" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1451,158 +1464,38 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="50" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="5" fillId="3" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="52" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="53" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="54" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="55" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="3" borderId="35" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1617,20 +1510,207 @@
     <xf numFmtId="2" fontId="5" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="59" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="53" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="62" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="52" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="50" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="35" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="53" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="54" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="55" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="5" fillId="3" borderId="35" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="59" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="42" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="53" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="3" borderId="61" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1638,16 +1718,57 @@
     <xf numFmtId="2" fontId="5" fillId="3" borderId="60" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="62" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="69" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="70" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="63" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="64" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="65" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="66" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="67" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="68" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2092,8 +2213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13628510-9764-4D87-A543-465B04714C1D}">
   <dimension ref="A1:BD219"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H84" sqref="H84"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="G99" sqref="G99:L102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -2139,45 +2260,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="10"/>
-      <c r="G1" s="11" t="s">
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="55"/>
+      <c r="G1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="12"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="14"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="63"/>
     </row>
     <row r="2" spans="1:32" ht="12.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="93"/>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="94"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="66"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="95" t="s">
+      <c r="G2" s="67" t="s">
         <v>84</v>
       </c>
-      <c r="H2" s="96"/>
-      <c r="I2" s="97" t="s">
+      <c r="H2" s="68"/>
+      <c r="I2" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="J2" s="97" t="s">
+      <c r="J2" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="97" t="s">
+      <c r="K2" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="L2" s="97" t="s">
+      <c r="L2" s="41" t="s">
         <v>115</v>
       </c>
       <c r="P2" s="4"/>
@@ -2185,603 +2306,603 @@
       <c r="AF2" s="4"/>
     </row>
     <row r="3" spans="1:32" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="54"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="23"/>
       <c r="F3" s="5"/>
-      <c r="G3" s="68" t="s">
+      <c r="G3" s="71" t="s">
         <v>67</v>
       </c>
-      <c r="H3" s="69"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
-      <c r="L3" s="87"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="40"/>
     </row>
     <row r="4" spans="1:32" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="75" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="47"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="21"/>
       <c r="F4" s="5"/>
-      <c r="G4" s="56" t="s">
+      <c r="G4" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="57"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="58"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="25"/>
     </row>
     <row r="5" spans="1:32" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="75" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="47"/>
+      <c r="B5" s="76"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="21"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="56" t="s">
+      <c r="G5" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="H5" s="57"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="51"/>
-      <c r="K5" s="51"/>
-      <c r="L5" s="58"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="25"/>
     </row>
     <row r="6" spans="1:32" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="47"/>
+      <c r="B6" s="76"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="21"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="56" t="s">
+      <c r="G6" s="73" t="s">
         <v>69</v>
       </c>
-      <c r="H6" s="57"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="51"/>
-      <c r="K6" s="51"/>
-      <c r="L6" s="58"/>
+      <c r="H6" s="74"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="25"/>
     </row>
     <row r="7" spans="1:32" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="77" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="49"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="47"/>
+      <c r="B7" s="78"/>
+      <c r="C7" s="79"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="21"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="56" t="s">
+      <c r="G7" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="H7" s="57"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="58"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="25"/>
     </row>
     <row r="8" spans="1:32" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="75" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="47"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="21"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="56" t="s">
+      <c r="G8" s="73" t="s">
         <v>71</v>
       </c>
-      <c r="H8" s="57"/>
-      <c r="I8" s="51"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="51"/>
-      <c r="L8" s="58"/>
+      <c r="H8" s="74"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="25"/>
     </row>
     <row r="9" spans="1:32" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="75" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="46"/>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="47"/>
+      <c r="B9" s="76"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="21"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="56" t="s">
+      <c r="G9" s="73" t="s">
         <v>72</v>
       </c>
-      <c r="H9" s="57"/>
-      <c r="I9" s="51"/>
-      <c r="J9" s="51"/>
-      <c r="K9" s="51"/>
-      <c r="L9" s="58"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="25"/>
     </row>
     <row r="10" spans="1:32" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="47"/>
+      <c r="B10" s="76"/>
+      <c r="C10" s="76"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="21"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="56" t="s">
+      <c r="G10" s="73" t="s">
         <v>73</v>
       </c>
-      <c r="H10" s="57"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="51"/>
-      <c r="L10" s="58"/>
+      <c r="H10" s="74"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="25"/>
     </row>
     <row r="11" spans="1:32" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="47"/>
+      <c r="B11" s="76"/>
+      <c r="C11" s="76"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="21"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="56" t="s">
+      <c r="G11" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="57"/>
-      <c r="I11" s="51"/>
-      <c r="J11" s="51"/>
-      <c r="K11" s="51"/>
-      <c r="L11" s="58"/>
+      <c r="H11" s="74"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="25"/>
     </row>
     <row r="12" spans="1:32" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="75" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="46"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="47"/>
+      <c r="B12" s="76"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="5"/>
-      <c r="G12" s="56" t="s">
+      <c r="G12" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="57"/>
-      <c r="I12" s="51"/>
-      <c r="J12" s="51"/>
-      <c r="K12" s="51"/>
-      <c r="L12" s="58"/>
+      <c r="H12" s="74"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="25"/>
     </row>
     <row r="13" spans="1:32" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="77" t="s">
         <v>65</v>
       </c>
-      <c r="B13" s="49"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="47"/>
+      <c r="B13" s="78"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="79"/>
+      <c r="E13" s="21"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="56" t="s">
+      <c r="G13" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="57"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="51"/>
-      <c r="K13" s="51"/>
-      <c r="L13" s="58"/>
+      <c r="H13" s="74"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="25"/>
     </row>
     <row r="14" spans="1:32" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="52" t="s">
+      <c r="A14" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="53"/>
-      <c r="C14" s="53"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="54"/>
+      <c r="B14" s="70"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="70"/>
+      <c r="E14" s="23"/>
       <c r="F14" s="5"/>
-      <c r="G14" s="56" t="s">
+      <c r="G14" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="H14" s="57"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="51"/>
-      <c r="K14" s="51"/>
-      <c r="L14" s="58"/>
+      <c r="H14" s="74"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="25"/>
     </row>
     <row r="15" spans="1:32" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="75" t="s">
         <v>81</v>
       </c>
-      <c r="B15" s="46"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="47"/>
+      <c r="B15" s="76"/>
+      <c r="C15" s="76"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="21"/>
       <c r="F15" s="5"/>
-      <c r="G15" s="56" t="s">
+      <c r="G15" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="H15" s="57"/>
-      <c r="I15" s="51"/>
-      <c r="J15" s="51"/>
-      <c r="K15" s="51"/>
-      <c r="L15" s="58"/>
+      <c r="H15" s="74"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="25"/>
     </row>
     <row r="16" spans="1:32" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="75" t="s">
         <v>82</v>
       </c>
-      <c r="B16" s="46"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="47"/>
+      <c r="B16" s="76"/>
+      <c r="C16" s="76"/>
+      <c r="D16" s="76"/>
+      <c r="E16" s="21"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="56" t="s">
+      <c r="G16" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="H16" s="57"/>
-      <c r="I16" s="51"/>
-      <c r="J16" s="51"/>
-      <c r="K16" s="51"/>
-      <c r="L16" s="58"/>
+      <c r="H16" s="74"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="25"/>
     </row>
     <row r="17" spans="1:12" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="45" t="s">
+      <c r="A17" s="75" t="s">
         <v>83</v>
       </c>
-      <c r="B17" s="46"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="47"/>
+      <c r="B17" s="76"/>
+      <c r="C17" s="76"/>
+      <c r="D17" s="76"/>
+      <c r="E17" s="21"/>
       <c r="F17" s="5"/>
-      <c r="G17" s="56" t="s">
+      <c r="G17" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="H17" s="57"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="51"/>
-      <c r="K17" s="51"/>
-      <c r="L17" s="58"/>
+      <c r="H17" s="74"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="25"/>
     </row>
     <row r="18" spans="1:12" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="45"/>
-      <c r="B18" s="46"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="47"/>
+      <c r="A18" s="75"/>
+      <c r="B18" s="76"/>
+      <c r="C18" s="76"/>
+      <c r="D18" s="76"/>
+      <c r="E18" s="21"/>
       <c r="F18" s="5"/>
-      <c r="G18" s="56" t="s">
+      <c r="G18" s="73" t="s">
         <v>33</v>
       </c>
-      <c r="H18" s="57"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="51"/>
-      <c r="K18" s="51"/>
-      <c r="L18" s="58"/>
+      <c r="H18" s="74"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="25"/>
     </row>
     <row r="19" spans="1:12" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="46"/>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="55"/>
+      <c r="A19" s="76"/>
+      <c r="B19" s="76"/>
+      <c r="C19" s="76"/>
+      <c r="D19" s="76"/>
+      <c r="E19" s="24"/>
       <c r="F19" s="5"/>
-      <c r="G19" s="56" t="s">
+      <c r="G19" s="73" t="s">
         <v>74</v>
       </c>
-      <c r="H19" s="57"/>
-      <c r="I19" s="51"/>
-      <c r="J19" s="51"/>
-      <c r="K19" s="51"/>
-      <c r="L19" s="58"/>
+      <c r="H19" s="74"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="25"/>
     </row>
     <row r="20" spans="1:12" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="46"/>
-      <c r="B20" s="46"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="55"/>
+      <c r="A20" s="76"/>
+      <c r="B20" s="76"/>
+      <c r="C20" s="76"/>
+      <c r="D20" s="76"/>
+      <c r="E20" s="24"/>
       <c r="F20" s="5"/>
-      <c r="G20" s="56" t="s">
+      <c r="G20" s="73" t="s">
         <v>75</v>
       </c>
-      <c r="H20" s="57"/>
-      <c r="I20" s="51"/>
-      <c r="J20" s="51"/>
-      <c r="K20" s="51"/>
-      <c r="L20" s="58"/>
+      <c r="H20" s="74"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="25"/>
     </row>
     <row r="21" spans="1:12" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="46"/>
-      <c r="B21" s="46"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="55"/>
+      <c r="A21" s="76"/>
+      <c r="B21" s="76"/>
+      <c r="C21" s="76"/>
+      <c r="D21" s="76"/>
+      <c r="E21" s="24"/>
       <c r="F21" s="5"/>
-      <c r="G21" s="59" t="s">
+      <c r="G21" s="83" t="s">
         <v>76</v>
       </c>
-      <c r="H21" s="60"/>
-      <c r="I21" s="51"/>
-      <c r="J21" s="51"/>
-      <c r="K21" s="51"/>
-      <c r="L21" s="58"/>
+      <c r="H21" s="84"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="25"/>
     </row>
     <row r="22" spans="1:12" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="46"/>
-      <c r="B22" s="46"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="55"/>
-      <c r="G22" s="56" t="s">
+      <c r="A22" s="76"/>
+      <c r="B22" s="76"/>
+      <c r="C22" s="76"/>
+      <c r="D22" s="76"/>
+      <c r="E22" s="24"/>
+      <c r="G22" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="H22" s="57"/>
-      <c r="I22" s="51"/>
-      <c r="J22" s="51"/>
-      <c r="K22" s="51"/>
-      <c r="L22" s="58"/>
+      <c r="H22" s="74"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="25"/>
     </row>
     <row r="23" spans="1:12" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="46"/>
-      <c r="B23" s="46"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="55"/>
-      <c r="G23" s="56" t="s">
+      <c r="A23" s="76"/>
+      <c r="B23" s="76"/>
+      <c r="C23" s="76"/>
+      <c r="D23" s="76"/>
+      <c r="E23" s="24"/>
+      <c r="G23" s="73" t="s">
         <v>86</v>
       </c>
-      <c r="H23" s="57"/>
-      <c r="I23" s="51"/>
-      <c r="J23" s="51"/>
-      <c r="K23" s="51"/>
-      <c r="L23" s="58"/>
+      <c r="H23" s="74"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="25"/>
     </row>
     <row r="24" spans="1:12" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="46"/>
-      <c r="B24" s="46"/>
-      <c r="C24" s="46"/>
-      <c r="D24" s="46"/>
-      <c r="E24" s="55"/>
-      <c r="G24" s="56" t="s">
+      <c r="A24" s="76"/>
+      <c r="B24" s="76"/>
+      <c r="C24" s="76"/>
+      <c r="D24" s="76"/>
+      <c r="E24" s="24"/>
+      <c r="G24" s="73" t="s">
         <v>87</v>
       </c>
-      <c r="H24" s="57"/>
-      <c r="I24" s="51"/>
-      <c r="J24" s="51"/>
-      <c r="K24" s="51"/>
-      <c r="L24" s="58"/>
+      <c r="H24" s="74"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
+      <c r="L24" s="25"/>
     </row>
     <row r="25" spans="1:12" s="6" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G25" s="56" t="s">
+      <c r="G25" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="H25" s="57"/>
-      <c r="I25" s="51"/>
-      <c r="J25" s="51"/>
-      <c r="K25" s="51"/>
-      <c r="L25" s="58"/>
+      <c r="H25" s="74"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="25"/>
     </row>
     <row r="26" spans="1:12" s="6" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="17"/>
-      <c r="G26" s="56" t="s">
+      <c r="B26" s="81"/>
+      <c r="C26" s="81"/>
+      <c r="D26" s="81"/>
+      <c r="E26" s="82"/>
+      <c r="G26" s="73" t="s">
         <v>89</v>
       </c>
-      <c r="H26" s="57"/>
-      <c r="I26" s="51"/>
-      <c r="J26" s="51"/>
-      <c r="K26" s="51"/>
-      <c r="L26" s="58"/>
+      <c r="H26" s="74"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="22"/>
+      <c r="L26" s="25"/>
     </row>
     <row r="27" spans="1:12" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="98" t="s">
+      <c r="A27" s="56" t="s">
         <v>56</v>
       </c>
-      <c r="B27" s="99"/>
-      <c r="C27" s="120" t="s">
+      <c r="B27" s="57"/>
+      <c r="C27" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="D27" s="97" t="s">
+      <c r="D27" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="109" t="s">
+      <c r="E27" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="G27" s="56" t="s">
+      <c r="G27" s="73" t="s">
         <v>90</v>
       </c>
-      <c r="H27" s="57"/>
-      <c r="I27" s="51"/>
-      <c r="J27" s="51"/>
-      <c r="K27" s="51"/>
-      <c r="L27" s="58"/>
+      <c r="H27" s="74"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="25"/>
     </row>
     <row r="28" spans="1:12" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="68" t="s">
+      <c r="A28" s="71" t="s">
         <v>103</v>
       </c>
-      <c r="B28" s="69"/>
-      <c r="C28" s="51" t="s">
+      <c r="B28" s="72"/>
+      <c r="C28" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="D28" s="65"/>
-      <c r="E28" s="67"/>
-      <c r="G28" s="56" t="s">
+      <c r="D28" s="28"/>
+      <c r="E28" s="30"/>
+      <c r="G28" s="73" t="s">
         <v>91</v>
       </c>
-      <c r="H28" s="57"/>
-      <c r="I28" s="51"/>
-      <c r="J28" s="51"/>
-      <c r="K28" s="51"/>
-      <c r="L28" s="58"/>
+      <c r="H28" s="74"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="25"/>
     </row>
     <row r="29" spans="1:12" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="56" t="s">
+      <c r="A29" s="73" t="s">
         <v>104</v>
       </c>
-      <c r="B29" s="57"/>
-      <c r="C29" s="51" t="s">
+      <c r="B29" s="74"/>
+      <c r="C29" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="D29" s="51"/>
-      <c r="E29" s="67"/>
-      <c r="G29" s="56" t="s">
+      <c r="D29" s="22"/>
+      <c r="E29" s="30"/>
+      <c r="G29" s="73" t="s">
         <v>92</v>
       </c>
-      <c r="H29" s="57"/>
-      <c r="I29" s="51"/>
-      <c r="J29" s="51"/>
-      <c r="K29" s="51"/>
-      <c r="L29" s="58"/>
+      <c r="H29" s="74"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="22"/>
+      <c r="L29" s="25"/>
     </row>
     <row r="30" spans="1:12" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="56" t="s">
+      <c r="A30" s="73" t="s">
         <v>105</v>
       </c>
-      <c r="B30" s="57"/>
-      <c r="C30" s="51" t="s">
+      <c r="B30" s="74"/>
+      <c r="C30" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="D30" s="51"/>
-      <c r="E30" s="67"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="30"/>
       <c r="F30" s="5"/>
-      <c r="G30" s="56" t="s">
+      <c r="G30" s="73" t="s">
         <v>93</v>
       </c>
-      <c r="H30" s="57"/>
-      <c r="I30" s="51"/>
-      <c r="J30" s="51"/>
-      <c r="K30" s="51"/>
-      <c r="L30" s="58"/>
+      <c r="H30" s="74"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="22"/>
+      <c r="L30" s="25"/>
     </row>
     <row r="31" spans="1:12" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="56"/>
-      <c r="B31" s="57"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="67"/>
+      <c r="A31" s="73"/>
+      <c r="B31" s="74"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="30"/>
       <c r="F31" s="5"/>
-      <c r="G31" s="56" t="s">
+      <c r="G31" s="73" t="s">
         <v>94</v>
       </c>
-      <c r="H31" s="57"/>
-      <c r="I31" s="51"/>
-      <c r="J31" s="51"/>
-      <c r="K31" s="51"/>
-      <c r="L31" s="58"/>
+      <c r="H31" s="74"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="22"/>
+      <c r="L31" s="25"/>
     </row>
     <row r="32" spans="1:12" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="56"/>
-      <c r="B32" s="57"/>
-      <c r="C32" s="51"/>
-      <c r="D32" s="51"/>
-      <c r="E32" s="67"/>
+      <c r="A32" s="73"/>
+      <c r="B32" s="74"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="30"/>
       <c r="F32" s="5"/>
-      <c r="G32" s="56" t="s">
+      <c r="G32" s="73" t="s">
         <v>95</v>
       </c>
-      <c r="H32" s="57"/>
-      <c r="I32" s="51"/>
-      <c r="J32" s="51"/>
-      <c r="K32" s="51"/>
-      <c r="L32" s="58"/>
+      <c r="H32" s="74"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="22"/>
+      <c r="L32" s="25"/>
     </row>
     <row r="33" spans="1:56" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="56"/>
-      <c r="B33" s="57"/>
-      <c r="C33" s="51"/>
-      <c r="D33" s="51"/>
-      <c r="E33" s="67"/>
+      <c r="A33" s="73"/>
+      <c r="B33" s="74"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="30"/>
       <c r="F33" s="5"/>
-      <c r="G33" s="56" t="s">
+      <c r="G33" s="73" t="s">
         <v>96</v>
       </c>
-      <c r="H33" s="57"/>
-      <c r="I33" s="51"/>
-      <c r="J33" s="51"/>
-      <c r="K33" s="51"/>
-      <c r="L33" s="58"/>
+      <c r="H33" s="74"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="22"/>
+      <c r="L33" s="25"/>
     </row>
     <row r="34" spans="1:56" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="56"/>
-      <c r="B34" s="57"/>
-      <c r="C34" s="51"/>
-      <c r="D34" s="51"/>
-      <c r="E34" s="67"/>
+      <c r="A34" s="73"/>
+      <c r="B34" s="74"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="30"/>
       <c r="F34" s="5"/>
-      <c r="G34" s="56" t="s">
+      <c r="G34" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="H34" s="57"/>
-      <c r="I34" s="51"/>
-      <c r="J34" s="51"/>
-      <c r="K34" s="51"/>
-      <c r="L34" s="58"/>
+      <c r="H34" s="74"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="22"/>
+      <c r="K34" s="22"/>
+      <c r="L34" s="25"/>
     </row>
     <row r="35" spans="1:56" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="60"/>
-      <c r="B35" s="60"/>
-      <c r="C35" s="51"/>
-      <c r="D35" s="51"/>
-      <c r="E35" s="67"/>
+      <c r="A35" s="84"/>
+      <c r="B35" s="84"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="30"/>
       <c r="F35" s="5"/>
-      <c r="G35" s="56" t="s">
+      <c r="G35" s="73" t="s">
         <v>98</v>
       </c>
-      <c r="H35" s="57"/>
-      <c r="I35" s="51"/>
-      <c r="J35" s="51"/>
-      <c r="K35" s="51"/>
-      <c r="L35" s="58"/>
+      <c r="H35" s="74"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="22"/>
+      <c r="L35" s="25"/>
     </row>
     <row r="36" spans="1:56" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="60"/>
-      <c r="B36" s="60"/>
-      <c r="C36" s="51"/>
-      <c r="D36" s="51"/>
-      <c r="E36" s="67"/>
+      <c r="A36" s="84"/>
+      <c r="B36" s="84"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="30"/>
       <c r="F36" s="5"/>
-      <c r="G36" s="56" t="s">
+      <c r="G36" s="73" t="s">
         <v>99</v>
       </c>
-      <c r="H36" s="57"/>
-      <c r="I36" s="51"/>
-      <c r="J36" s="51"/>
-      <c r="K36" s="51"/>
-      <c r="L36" s="58"/>
+      <c r="H36" s="74"/>
+      <c r="I36" s="22"/>
+      <c r="J36" s="22"/>
+      <c r="K36" s="22"/>
+      <c r="L36" s="25"/>
     </row>
     <row r="37" spans="1:56" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="60"/>
-      <c r="B37" s="60"/>
-      <c r="C37" s="51"/>
-      <c r="D37" s="51"/>
-      <c r="E37" s="67"/>
+      <c r="A37" s="84"/>
+      <c r="B37" s="84"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="30"/>
       <c r="F37" s="5"/>
-      <c r="G37" s="56" t="s">
+      <c r="G37" s="73" t="s">
         <v>100</v>
       </c>
-      <c r="H37" s="57"/>
-      <c r="I37" s="51"/>
-      <c r="J37" s="51"/>
-      <c r="K37" s="51"/>
-      <c r="L37" s="58"/>
+      <c r="H37" s="74"/>
+      <c r="I37" s="22"/>
+      <c r="J37" s="22"/>
+      <c r="K37" s="22"/>
+      <c r="L37" s="25"/>
       <c r="M37" s="4"/>
       <c r="N37" s="4"/>
       <c r="O37" s="4"/>
@@ -2793,20 +2914,20 @@
       <c r="AS37" s="4"/>
     </row>
     <row r="38" spans="1:56" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="60"/>
-      <c r="B38" s="60"/>
-      <c r="C38" s="51"/>
-      <c r="D38" s="51"/>
-      <c r="E38" s="67"/>
+      <c r="A38" s="84"/>
+      <c r="B38" s="84"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="30"/>
       <c r="F38" s="5"/>
-      <c r="G38" s="56" t="s">
+      <c r="G38" s="73" t="s">
         <v>101</v>
       </c>
-      <c r="H38" s="57"/>
-      <c r="I38" s="51"/>
-      <c r="J38" s="51"/>
-      <c r="K38" s="51"/>
-      <c r="L38" s="58"/>
+      <c r="H38" s="74"/>
+      <c r="I38" s="22"/>
+      <c r="J38" s="22"/>
+      <c r="K38" s="22"/>
+      <c r="L38" s="25"/>
       <c r="M38" s="4"/>
       <c r="N38" s="4"/>
       <c r="O38" s="4"/>
@@ -2818,20 +2939,20 @@
       <c r="AS38" s="4"/>
     </row>
     <row r="39" spans="1:56" s="6" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="60"/>
-      <c r="B39" s="60"/>
-      <c r="C39" s="51"/>
-      <c r="D39" s="51"/>
-      <c r="E39" s="67"/>
+      <c r="A39" s="84"/>
+      <c r="B39" s="84"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="30"/>
       <c r="F39" s="5"/>
-      <c r="G39" s="61" t="s">
+      <c r="G39" s="90" t="s">
         <v>102</v>
       </c>
-      <c r="H39" s="62"/>
-      <c r="I39" s="63"/>
-      <c r="J39" s="63"/>
-      <c r="K39" s="63"/>
-      <c r="L39" s="64"/>
+      <c r="H39" s="91"/>
+      <c r="I39" s="26"/>
+      <c r="J39" s="26"/>
+      <c r="K39" s="26"/>
+      <c r="L39" s="27"/>
       <c r="M39" s="4"/>
       <c r="N39" s="4"/>
       <c r="O39" s="4"/>
@@ -2847,11 +2968,11 @@
       <c r="AS39" s="4"/>
     </row>
     <row r="40" spans="1:56" s="6" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="56"/>
-      <c r="B40" s="57"/>
-      <c r="C40" s="51"/>
-      <c r="D40" s="51"/>
-      <c r="E40" s="67"/>
+      <c r="A40" s="73"/>
+      <c r="B40" s="74"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="30"/>
       <c r="F40" s="5"/>
       <c r="M40" s="4"/>
       <c r="N40" s="4"/>
@@ -2878,72 +2999,72 @@
       <c r="BD40" s="4"/>
     </row>
     <row r="41" spans="1:56" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="56"/>
-      <c r="B41" s="57"/>
-      <c r="C41" s="51"/>
-      <c r="D41" s="51"/>
-      <c r="E41" s="67"/>
+      <c r="A41" s="73"/>
+      <c r="B41" s="74"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="30"/>
       <c r="F41" s="5"/>
-      <c r="G41" s="8" t="s">
+      <c r="G41" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="H41" s="9"/>
-      <c r="I41" s="9"/>
-      <c r="J41" s="9"/>
-      <c r="K41" s="9"/>
-      <c r="L41" s="10"/>
+      <c r="H41" s="54"/>
+      <c r="I41" s="54"/>
+      <c r="J41" s="54"/>
+      <c r="K41" s="54"/>
+      <c r="L41" s="55"/>
     </row>
     <row r="42" spans="1:56" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="56"/>
-      <c r="B42" s="57"/>
-      <c r="C42" s="51"/>
-      <c r="D42" s="51"/>
-      <c r="E42" s="67"/>
+      <c r="A42" s="73"/>
+      <c r="B42" s="74"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="30"/>
       <c r="F42" s="5"/>
-      <c r="G42" s="98" t="s">
+      <c r="G42" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="H42" s="99"/>
-      <c r="I42" s="115" t="s">
+      <c r="H42" s="57"/>
+      <c r="I42" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="J42" s="115" t="s">
+      <c r="J42" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="K42" s="97" t="s">
+      <c r="K42" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="L42" s="112" t="s">
+      <c r="L42" s="47" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:56" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="68"/>
-      <c r="B43" s="69"/>
-      <c r="C43" s="65"/>
-      <c r="D43" s="65"/>
-      <c r="E43" s="66"/>
+      <c r="A43" s="71"/>
+      <c r="B43" s="72"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="29"/>
       <c r="F43" s="5"/>
-      <c r="G43" s="118"/>
-      <c r="H43" s="119"/>
-      <c r="I43" s="51"/>
-      <c r="J43" s="51"/>
-      <c r="K43" s="65"/>
-      <c r="L43" s="87"/>
+      <c r="G43" s="92"/>
+      <c r="H43" s="93"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
+      <c r="K43" s="28"/>
+      <c r="L43" s="40"/>
     </row>
     <row r="44" spans="1:56" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="61"/>
-      <c r="B44" s="62"/>
-      <c r="C44" s="63"/>
-      <c r="D44" s="63"/>
-      <c r="E44" s="70"/>
+      <c r="A44" s="90"/>
+      <c r="B44" s="91"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="31"/>
       <c r="F44" s="5"/>
-      <c r="G44" s="88"/>
-      <c r="H44" s="89"/>
-      <c r="I44" s="51"/>
-      <c r="J44" s="51"/>
-      <c r="K44" s="51"/>
-      <c r="L44" s="58"/>
+      <c r="G44" s="58"/>
+      <c r="H44" s="59"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
+      <c r="K44" s="22"/>
+      <c r="L44" s="25"/>
     </row>
     <row r="45" spans="1:56" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="6"/>
@@ -2952,1026 +3073,1058 @@
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="5"/>
-      <c r="G45" s="88"/>
-      <c r="H45" s="89"/>
-      <c r="I45" s="51"/>
-      <c r="J45" s="51"/>
-      <c r="K45" s="51"/>
-      <c r="L45" s="58"/>
+      <c r="G45" s="58"/>
+      <c r="H45" s="59"/>
+      <c r="I45" s="22"/>
+      <c r="J45" s="22"/>
+      <c r="K45" s="22"/>
+      <c r="L45" s="25"/>
     </row>
     <row r="46" spans="1:56" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="19" t="s">
+      <c r="A46" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="B46" s="20"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="21"/>
+      <c r="B46" s="95"/>
+      <c r="C46" s="95"/>
+      <c r="D46" s="95"/>
+      <c r="E46" s="96"/>
       <c r="F46" s="3"/>
-      <c r="G46" s="88"/>
-      <c r="H46" s="89"/>
-      <c r="I46" s="51"/>
-      <c r="J46" s="51"/>
-      <c r="K46" s="51"/>
-      <c r="L46" s="58"/>
+      <c r="G46" s="58"/>
+      <c r="H46" s="59"/>
+      <c r="I46" s="22"/>
+      <c r="J46" s="22"/>
+      <c r="K46" s="22"/>
+      <c r="L46" s="25"/>
     </row>
     <row r="47" spans="1:56" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="22" t="s">
+      <c r="A47" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B47" s="23" t="s">
+      <c r="B47" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C47" s="23" t="s">
+      <c r="C47" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D47" s="25" t="s">
+      <c r="D47" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E47" s="24" t="s">
+      <c r="E47" s="9" t="s">
         <v>19</v>
       </c>
       <c r="F47" s="3"/>
-      <c r="G47" s="88"/>
-      <c r="H47" s="89"/>
-      <c r="I47" s="51"/>
-      <c r="J47" s="51"/>
-      <c r="K47" s="51"/>
-      <c r="L47" s="58"/>
+      <c r="G47" s="58"/>
+      <c r="H47" s="59"/>
+      <c r="I47" s="22"/>
+      <c r="J47" s="22"/>
+      <c r="K47" s="22"/>
+      <c r="L47" s="25"/>
     </row>
     <row r="48" spans="1:56" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="71" t="s">
+      <c r="A48" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B48" s="51"/>
-      <c r="C48" s="51"/>
-      <c r="D48" s="51"/>
-      <c r="E48" s="67"/>
+      <c r="B48" s="22"/>
+      <c r="C48" s="22"/>
+      <c r="D48" s="22"/>
+      <c r="E48" s="30"/>
       <c r="F48" s="3"/>
-      <c r="G48" s="88"/>
-      <c r="H48" s="89"/>
-      <c r="I48" s="51"/>
-      <c r="J48" s="51"/>
-      <c r="K48" s="51"/>
-      <c r="L48" s="58"/>
+      <c r="G48" s="58"/>
+      <c r="H48" s="59"/>
+      <c r="I48" s="22"/>
+      <c r="J48" s="22"/>
+      <c r="K48" s="22"/>
+      <c r="L48" s="25"/>
     </row>
     <row r="49" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="71" t="s">
+      <c r="A49" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B49" s="51"/>
-      <c r="C49" s="51"/>
-      <c r="D49" s="51"/>
-      <c r="E49" s="67"/>
+      <c r="B49" s="22"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="22"/>
+      <c r="E49" s="30"/>
       <c r="F49" s="3"/>
-      <c r="G49" s="88"/>
-      <c r="H49" s="89"/>
-      <c r="I49" s="51"/>
-      <c r="J49" s="51"/>
-      <c r="K49" s="51"/>
-      <c r="L49" s="58"/>
+      <c r="G49" s="58"/>
+      <c r="H49" s="59"/>
+      <c r="I49" s="22"/>
+      <c r="J49" s="22"/>
+      <c r="K49" s="22"/>
+      <c r="L49" s="25"/>
     </row>
     <row r="50" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="71" t="s">
+      <c r="A50" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B50" s="51"/>
-      <c r="C50" s="51"/>
-      <c r="D50" s="51"/>
-      <c r="E50" s="67"/>
+      <c r="B50" s="22"/>
+      <c r="C50" s="22"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="30"/>
       <c r="F50" s="3"/>
-      <c r="G50" s="88"/>
-      <c r="H50" s="89"/>
-      <c r="I50" s="51"/>
-      <c r="J50" s="51"/>
-      <c r="K50" s="51"/>
-      <c r="L50" s="58"/>
+      <c r="G50" s="58"/>
+      <c r="H50" s="59"/>
+      <c r="I50" s="22"/>
+      <c r="J50" s="22"/>
+      <c r="K50" s="22"/>
+      <c r="L50" s="25"/>
     </row>
     <row r="51" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="71" t="s">
+      <c r="A51" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="B51" s="51"/>
-      <c r="C51" s="51"/>
-      <c r="D51" s="51"/>
-      <c r="E51" s="67"/>
+      <c r="B51" s="22"/>
+      <c r="C51" s="22"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="30"/>
       <c r="F51" s="3"/>
-      <c r="G51" s="88"/>
-      <c r="H51" s="89"/>
-      <c r="I51" s="51"/>
-      <c r="J51" s="51"/>
-      <c r="K51" s="51"/>
-      <c r="L51" s="58"/>
+      <c r="G51" s="58"/>
+      <c r="H51" s="59"/>
+      <c r="I51" s="22"/>
+      <c r="J51" s="22"/>
+      <c r="K51" s="22"/>
+      <c r="L51" s="25"/>
     </row>
     <row r="52" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="71" t="s">
+      <c r="A52" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B52" s="51"/>
-      <c r="C52" s="51"/>
-      <c r="D52" s="51"/>
-      <c r="E52" s="67"/>
+      <c r="B52" s="22"/>
+      <c r="C52" s="22"/>
+      <c r="D52" s="22"/>
+      <c r="E52" s="30"/>
       <c r="F52" s="3"/>
-      <c r="G52" s="88"/>
-      <c r="H52" s="89"/>
-      <c r="I52" s="51"/>
-      <c r="J52" s="51"/>
-      <c r="K52" s="51"/>
-      <c r="L52" s="58"/>
+      <c r="G52" s="58"/>
+      <c r="H52" s="59"/>
+      <c r="I52" s="22"/>
+      <c r="J52" s="22"/>
+      <c r="K52" s="22"/>
+      <c r="L52" s="25"/>
     </row>
     <row r="53" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="18" t="s">
+      <c r="A53" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="B53" s="26"/>
-      <c r="C53" s="29"/>
-      <c r="D53" s="22"/>
-      <c r="E53" s="30"/>
+      <c r="B53" s="88"/>
+      <c r="C53" s="89"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="13"/>
       <c r="F53" s="3"/>
-      <c r="G53" s="90"/>
-      <c r="H53" s="91"/>
-      <c r="I53" s="51"/>
-      <c r="J53" s="51"/>
-      <c r="K53" s="51"/>
-      <c r="L53" s="58"/>
+      <c r="G53" s="85"/>
+      <c r="H53" s="86"/>
+      <c r="I53" s="22"/>
+      <c r="J53" s="22"/>
+      <c r="K53" s="22"/>
+      <c r="L53" s="25"/>
     </row>
     <row r="54" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="106" t="s">
+      <c r="A54" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="B54" s="100" t="s">
+      <c r="B54" s="97" t="s">
         <v>20</v>
       </c>
-      <c r="C54" s="101"/>
-      <c r="D54" s="103" t="s">
+      <c r="C54" s="98"/>
+      <c r="D54" s="99" t="s">
         <v>106</v>
       </c>
-      <c r="E54" s="104"/>
+      <c r="E54" s="100"/>
       <c r="F54" s="3"/>
-      <c r="G54" s="88"/>
-      <c r="H54" s="89"/>
-      <c r="I54" s="51"/>
-      <c r="J54" s="51"/>
-      <c r="K54" s="51"/>
-      <c r="L54" s="58"/>
+      <c r="G54" s="58"/>
+      <c r="H54" s="59"/>
+      <c r="I54" s="22"/>
+      <c r="J54" s="22"/>
+      <c r="K54" s="22"/>
+      <c r="L54" s="25"/>
     </row>
     <row r="55" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="107"/>
-      <c r="B55" s="102"/>
-      <c r="C55" s="7"/>
-      <c r="D55" s="102"/>
-      <c r="E55" s="105"/>
+      <c r="A55" s="43"/>
+      <c r="B55" s="101"/>
+      <c r="C55" s="102"/>
+      <c r="D55" s="101"/>
+      <c r="E55" s="103"/>
       <c r="F55" s="3"/>
-      <c r="G55" s="88"/>
-      <c r="H55" s="89"/>
-      <c r="I55" s="51"/>
-      <c r="J55" s="51"/>
-      <c r="K55" s="51"/>
-      <c r="L55" s="58"/>
+      <c r="G55" s="58"/>
+      <c r="H55" s="59"/>
+      <c r="I55" s="22"/>
+      <c r="J55" s="22"/>
+      <c r="K55" s="22"/>
+      <c r="L55" s="25"/>
     </row>
     <row r="56" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F56" s="3"/>
-      <c r="G56" s="90"/>
-      <c r="H56" s="91"/>
-      <c r="I56" s="51"/>
-      <c r="J56" s="51"/>
-      <c r="K56" s="51"/>
-      <c r="L56" s="58"/>
+      <c r="G56" s="85"/>
+      <c r="H56" s="86"/>
+      <c r="I56" s="22"/>
+      <c r="J56" s="22"/>
+      <c r="K56" s="22"/>
+      <c r="L56" s="25"/>
     </row>
     <row r="57" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A57" s="19" t="s">
+      <c r="A57" s="94" t="s">
         <v>116</v>
       </c>
-      <c r="B57" s="20"/>
-      <c r="C57" s="20"/>
-      <c r="D57" s="20"/>
-      <c r="E57" s="21"/>
+      <c r="B57" s="95"/>
+      <c r="C57" s="95"/>
+      <c r="D57" s="95"/>
+      <c r="E57" s="96"/>
       <c r="F57" s="3"/>
-      <c r="G57" s="88"/>
-      <c r="H57" s="89"/>
-      <c r="I57" s="51"/>
-      <c r="J57" s="51"/>
-      <c r="K57" s="51"/>
-      <c r="L57" s="58"/>
+      <c r="G57" s="58"/>
+      <c r="H57" s="59"/>
+      <c r="I57" s="22"/>
+      <c r="J57" s="22"/>
+      <c r="K57" s="22"/>
+      <c r="L57" s="25"/>
     </row>
     <row r="58" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="108" t="s">
+      <c r="A58" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="B58" s="27" t="s">
+      <c r="B58" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C58" s="23" t="s">
+      <c r="C58" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D58" s="23" t="s">
+      <c r="D58" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="28" t="s">
+      <c r="E58" s="12" t="s">
         <v>19</v>
       </c>
       <c r="F58" s="3"/>
-      <c r="G58" s="88"/>
-      <c r="H58" s="89"/>
-      <c r="I58" s="51"/>
-      <c r="J58" s="51"/>
-      <c r="K58" s="51"/>
-      <c r="L58" s="58"/>
+      <c r="G58" s="58"/>
+      <c r="H58" s="59"/>
+      <c r="I58" s="22"/>
+      <c r="J58" s="22"/>
+      <c r="K58" s="22"/>
+      <c r="L58" s="25"/>
     </row>
     <row r="59" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="71" t="s">
+      <c r="A59" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B59" s="51"/>
-      <c r="C59" s="51"/>
-      <c r="D59" s="51"/>
-      <c r="E59" s="67"/>
+      <c r="B59" s="22"/>
+      <c r="C59" s="22"/>
+      <c r="D59" s="22"/>
+      <c r="E59" s="30"/>
       <c r="F59" s="3"/>
-      <c r="G59" s="88"/>
-      <c r="H59" s="89"/>
-      <c r="I59" s="51"/>
-      <c r="J59" s="51"/>
-      <c r="K59" s="51"/>
-      <c r="L59" s="58"/>
+      <c r="G59" s="58"/>
+      <c r="H59" s="59"/>
+      <c r="I59" s="22"/>
+      <c r="J59" s="22"/>
+      <c r="K59" s="22"/>
+      <c r="L59" s="25"/>
     </row>
     <row r="60" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="71" t="s">
+      <c r="A60" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B60" s="51"/>
-      <c r="C60" s="51"/>
-      <c r="D60" s="51"/>
-      <c r="E60" s="67"/>
+      <c r="B60" s="22"/>
+      <c r="C60" s="22"/>
+      <c r="D60" s="22"/>
+      <c r="E60" s="30"/>
       <c r="F60" s="3"/>
-      <c r="G60" s="88"/>
-      <c r="H60" s="89"/>
-      <c r="I60" s="51"/>
-      <c r="J60" s="51"/>
-      <c r="K60" s="51"/>
-      <c r="L60" s="58"/>
+      <c r="G60" s="58"/>
+      <c r="H60" s="59"/>
+      <c r="I60" s="22"/>
+      <c r="J60" s="22"/>
+      <c r="K60" s="22"/>
+      <c r="L60" s="25"/>
     </row>
     <row r="61" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="71" t="s">
+      <c r="A61" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B61" s="51"/>
-      <c r="C61" s="51"/>
-      <c r="D61" s="51"/>
-      <c r="E61" s="67"/>
+      <c r="B61" s="22"/>
+      <c r="C61" s="22"/>
+      <c r="D61" s="22"/>
+      <c r="E61" s="30"/>
       <c r="F61" s="3"/>
-      <c r="G61" s="88"/>
-      <c r="H61" s="89"/>
-      <c r="I61" s="51"/>
-      <c r="J61" s="51"/>
-      <c r="K61" s="51"/>
-      <c r="L61" s="58"/>
+      <c r="G61" s="58"/>
+      <c r="H61" s="59"/>
+      <c r="I61" s="22"/>
+      <c r="J61" s="22"/>
+      <c r="K61" s="22"/>
+      <c r="L61" s="25"/>
     </row>
     <row r="62" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="71" t="s">
+      <c r="A62" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="B62" s="51"/>
-      <c r="C62" s="51"/>
-      <c r="D62" s="51"/>
-      <c r="E62" s="67"/>
+      <c r="B62" s="22"/>
+      <c r="C62" s="22"/>
+      <c r="D62" s="22"/>
+      <c r="E62" s="30"/>
       <c r="F62" s="3"/>
-      <c r="G62" s="88"/>
-      <c r="H62" s="89"/>
-      <c r="I62" s="51"/>
-      <c r="J62" s="51"/>
-      <c r="K62" s="51"/>
-      <c r="L62" s="58"/>
+      <c r="G62" s="58"/>
+      <c r="H62" s="59"/>
+      <c r="I62" s="22"/>
+      <c r="J62" s="22"/>
+      <c r="K62" s="22"/>
+      <c r="L62" s="25"/>
     </row>
     <row r="63" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="71" t="s">
+      <c r="A63" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B63" s="51"/>
-      <c r="C63" s="51"/>
-      <c r="D63" s="51"/>
-      <c r="E63" s="67"/>
+      <c r="B63" s="22"/>
+      <c r="C63" s="22"/>
+      <c r="D63" s="22"/>
+      <c r="E63" s="30"/>
       <c r="F63" s="3"/>
-      <c r="G63" s="88"/>
-      <c r="H63" s="89"/>
-      <c r="I63" s="51"/>
-      <c r="J63" s="51"/>
-      <c r="K63" s="51"/>
-      <c r="L63" s="58"/>
+      <c r="G63" s="58"/>
+      <c r="H63" s="59"/>
+      <c r="I63" s="22"/>
+      <c r="J63" s="22"/>
+      <c r="K63" s="22"/>
+      <c r="L63" s="25"/>
     </row>
     <row r="64" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="18" t="s">
+      <c r="A64" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="B64" s="26"/>
-      <c r="C64" s="29"/>
-      <c r="D64" s="22"/>
-      <c r="E64" s="30"/>
+      <c r="B64" s="88"/>
+      <c r="C64" s="89"/>
+      <c r="D64" s="7"/>
+      <c r="E64" s="13"/>
       <c r="F64" s="3"/>
-      <c r="G64" s="88"/>
-      <c r="H64" s="89"/>
-      <c r="I64" s="51"/>
-      <c r="J64" s="51"/>
-      <c r="K64" s="51"/>
-      <c r="L64" s="58"/>
+      <c r="G64" s="58"/>
+      <c r="H64" s="59"/>
+      <c r="I64" s="22"/>
+      <c r="J64" s="22"/>
+      <c r="K64" s="22"/>
+      <c r="L64" s="25"/>
     </row>
     <row r="65" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="106" t="s">
+      <c r="A65" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="B65" s="100" t="s">
+      <c r="B65" s="97" t="s">
         <v>20</v>
       </c>
-      <c r="C65" s="101"/>
-      <c r="D65" s="103" t="s">
+      <c r="C65" s="98"/>
+      <c r="D65" s="99" t="s">
         <v>106</v>
       </c>
-      <c r="E65" s="104"/>
+      <c r="E65" s="100"/>
       <c r="F65" s="3"/>
-      <c r="G65" s="88"/>
-      <c r="H65" s="89"/>
-      <c r="I65" s="51"/>
-      <c r="J65" s="51"/>
-      <c r="K65" s="51"/>
-      <c r="L65" s="58"/>
+      <c r="G65" s="58"/>
+      <c r="H65" s="59"/>
+      <c r="I65" s="22"/>
+      <c r="J65" s="22"/>
+      <c r="K65" s="22"/>
+      <c r="L65" s="25"/>
     </row>
     <row r="66" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="107"/>
-      <c r="B66" s="102"/>
-      <c r="C66" s="7"/>
-      <c r="D66" s="102"/>
-      <c r="E66" s="105"/>
+      <c r="A66" s="43"/>
+      <c r="B66" s="101"/>
+      <c r="C66" s="102"/>
+      <c r="D66" s="101"/>
+      <c r="E66" s="103"/>
       <c r="F66" s="3"/>
-      <c r="G66" s="88"/>
-      <c r="H66" s="89"/>
-      <c r="I66" s="51"/>
-      <c r="J66" s="51"/>
-      <c r="K66" s="51"/>
-      <c r="L66" s="58"/>
+      <c r="G66" s="58"/>
+      <c r="H66" s="59"/>
+      <c r="I66" s="22"/>
+      <c r="J66" s="22"/>
+      <c r="K66" s="22"/>
+      <c r="L66" s="25"/>
     </row>
     <row r="67" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F67" s="3"/>
-      <c r="G67" s="88"/>
-      <c r="H67" s="89"/>
-      <c r="I67" s="51"/>
-      <c r="J67" s="51"/>
-      <c r="K67" s="51"/>
-      <c r="L67" s="58"/>
+      <c r="G67" s="58"/>
+      <c r="H67" s="59"/>
+      <c r="I67" s="22"/>
+      <c r="J67" s="22"/>
+      <c r="K67" s="22"/>
+      <c r="L67" s="25"/>
     </row>
     <row r="68" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A68" s="31" t="s">
+      <c r="A68" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="B68" s="32"/>
-      <c r="C68" s="32"/>
-      <c r="D68" s="32"/>
-      <c r="E68" s="33"/>
+      <c r="B68" s="105"/>
+      <c r="C68" s="105"/>
+      <c r="D68" s="105"/>
+      <c r="E68" s="106"/>
       <c r="F68" s="3"/>
-      <c r="G68" s="88"/>
-      <c r="H68" s="89"/>
-      <c r="I68" s="51"/>
-      <c r="J68" s="51"/>
-      <c r="K68" s="51"/>
-      <c r="L68" s="58"/>
+      <c r="G68" s="58"/>
+      <c r="H68" s="59"/>
+      <c r="I68" s="22"/>
+      <c r="J68" s="22"/>
+      <c r="K68" s="22"/>
+      <c r="L68" s="25"/>
     </row>
     <row r="69" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="98" t="s">
+      <c r="A69" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="B69" s="99"/>
-      <c r="C69" s="97" t="s">
+      <c r="B69" s="57"/>
+      <c r="C69" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="D69" s="110" t="s">
+      <c r="D69" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="E69" s="109" t="s">
+      <c r="E69" s="45" t="s">
         <v>44</v>
       </c>
       <c r="F69" s="3"/>
-      <c r="G69" s="88"/>
-      <c r="H69" s="89"/>
-      <c r="I69" s="51"/>
-      <c r="J69" s="51"/>
-      <c r="K69" s="51"/>
-      <c r="L69" s="58"/>
+      <c r="G69" s="58"/>
+      <c r="H69" s="59"/>
+      <c r="I69" s="22"/>
+      <c r="J69" s="22"/>
+      <c r="K69" s="22"/>
+      <c r="L69" s="25"/>
     </row>
     <row r="70" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="82"/>
-      <c r="B70" s="83"/>
-      <c r="C70" s="65"/>
-      <c r="D70" s="51"/>
-      <c r="E70" s="67"/>
+      <c r="A70" s="108"/>
+      <c r="B70" s="109"/>
+      <c r="C70" s="28"/>
+      <c r="D70" s="22"/>
+      <c r="E70" s="30"/>
       <c r="F70" s="3"/>
-      <c r="G70" s="88"/>
-      <c r="H70" s="89"/>
-      <c r="I70" s="51"/>
-      <c r="J70" s="51"/>
-      <c r="K70" s="51"/>
-      <c r="L70" s="58"/>
+      <c r="G70" s="58"/>
+      <c r="H70" s="59"/>
+      <c r="I70" s="22"/>
+      <c r="J70" s="22"/>
+      <c r="K70" s="22"/>
+      <c r="L70" s="25"/>
     </row>
     <row r="71" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="59"/>
-      <c r="B71" s="60"/>
-      <c r="C71" s="51"/>
-      <c r="D71" s="51"/>
-      <c r="E71" s="67"/>
+      <c r="A71" s="83"/>
+      <c r="B71" s="84"/>
+      <c r="C71" s="22"/>
+      <c r="D71" s="22"/>
+      <c r="E71" s="30"/>
       <c r="F71" s="3"/>
-      <c r="G71" s="88"/>
-      <c r="H71" s="89"/>
-      <c r="I71" s="51"/>
-      <c r="J71" s="51"/>
-      <c r="K71" s="51"/>
-      <c r="L71" s="58"/>
+      <c r="G71" s="58"/>
+      <c r="H71" s="59"/>
+      <c r="I71" s="22"/>
+      <c r="J71" s="22"/>
+      <c r="K71" s="22"/>
+      <c r="L71" s="25"/>
     </row>
     <row r="72" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="72"/>
-      <c r="B72" s="73"/>
-      <c r="C72" s="74"/>
-      <c r="D72" s="74"/>
-      <c r="E72" s="75"/>
+      <c r="A72" s="117"/>
+      <c r="B72" s="118"/>
+      <c r="C72" s="33"/>
+      <c r="D72" s="33"/>
+      <c r="E72" s="34"/>
       <c r="F72" s="3"/>
-      <c r="G72" s="88"/>
-      <c r="H72" s="89"/>
-      <c r="I72" s="51"/>
-      <c r="J72" s="51"/>
-      <c r="K72" s="51"/>
-      <c r="L72" s="58"/>
+      <c r="G72" s="58"/>
+      <c r="H72" s="59"/>
+      <c r="I72" s="22"/>
+      <c r="J72" s="22"/>
+      <c r="K72" s="22"/>
+      <c r="L72" s="25"/>
     </row>
     <row r="73" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="18" t="s">
+      <c r="A73" s="87" t="s">
         <v>108</v>
       </c>
-      <c r="B73" s="26"/>
-      <c r="C73" s="26"/>
-      <c r="D73" s="34"/>
-      <c r="E73" s="35"/>
+      <c r="B73" s="88"/>
+      <c r="C73" s="88"/>
+      <c r="D73" s="110"/>
+      <c r="E73" s="14"/>
       <c r="F73" s="3"/>
-      <c r="G73" s="88"/>
-      <c r="H73" s="89"/>
-      <c r="I73" s="51"/>
-      <c r="J73" s="51"/>
-      <c r="K73" s="51"/>
-      <c r="L73" s="58"/>
+      <c r="G73" s="58"/>
+      <c r="H73" s="59"/>
+      <c r="I73" s="22"/>
+      <c r="J73" s="22"/>
+      <c r="K73" s="22"/>
+      <c r="L73" s="25"/>
     </row>
     <row r="74" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F74" s="3"/>
-      <c r="G74" s="88"/>
-      <c r="H74" s="89"/>
-      <c r="I74" s="51"/>
-      <c r="J74" s="51"/>
-      <c r="K74" s="51"/>
-      <c r="L74" s="58"/>
+      <c r="G74" s="58"/>
+      <c r="H74" s="59"/>
+      <c r="I74" s="22"/>
+      <c r="J74" s="22"/>
+      <c r="K74" s="22"/>
+      <c r="L74" s="25"/>
     </row>
     <row r="75" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A75" s="8" t="s">
+      <c r="A75" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="B75" s="9"/>
-      <c r="C75" s="9"/>
-      <c r="D75" s="9"/>
-      <c r="E75" s="10"/>
+      <c r="B75" s="54"/>
+      <c r="C75" s="54"/>
+      <c r="D75" s="54"/>
+      <c r="E75" s="55"/>
       <c r="F75" s="3"/>
-      <c r="G75" s="88"/>
-      <c r="H75" s="89"/>
-      <c r="I75" s="51"/>
-      <c r="J75" s="51"/>
-      <c r="K75" s="51"/>
-      <c r="L75" s="58"/>
+      <c r="G75" s="58"/>
+      <c r="H75" s="59"/>
+      <c r="I75" s="22"/>
+      <c r="J75" s="22"/>
+      <c r="K75" s="22"/>
+      <c r="L75" s="25"/>
     </row>
     <row r="76" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="56" t="s">
+      <c r="A76" s="73" t="s">
         <v>50</v>
       </c>
-      <c r="B76" s="76"/>
-      <c r="C76" s="76"/>
-      <c r="D76" s="57"/>
-      <c r="E76" s="77"/>
+      <c r="B76" s="111"/>
+      <c r="C76" s="111"/>
+      <c r="D76" s="74"/>
+      <c r="E76" s="35"/>
       <c r="F76" s="3"/>
     </row>
     <row r="77" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A77" s="56" t="s">
+      <c r="A77" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="B77" s="76"/>
-      <c r="C77" s="76"/>
-      <c r="D77" s="57"/>
-      <c r="E77" s="77"/>
+      <c r="B77" s="111"/>
+      <c r="C77" s="111"/>
+      <c r="D77" s="74"/>
+      <c r="E77" s="35"/>
       <c r="F77" s="3"/>
-      <c r="G77" s="8" t="s">
+      <c r="G77" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="H77" s="9"/>
-      <c r="I77" s="9"/>
-      <c r="J77" s="9"/>
-      <c r="K77" s="9"/>
-      <c r="L77" s="10"/>
+      <c r="H77" s="54"/>
+      <c r="I77" s="54"/>
+      <c r="J77" s="54"/>
+      <c r="K77" s="54"/>
+      <c r="L77" s="55"/>
     </row>
     <row r="78" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="56" t="s">
+      <c r="A78" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="B78" s="76"/>
-      <c r="C78" s="76"/>
-      <c r="D78" s="57"/>
-      <c r="E78" s="77"/>
+      <c r="B78" s="111"/>
+      <c r="C78" s="111"/>
+      <c r="D78" s="74"/>
+      <c r="E78" s="35"/>
       <c r="F78" s="3"/>
-      <c r="G78" s="114" t="s">
+      <c r="G78" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="H78" s="97" t="s">
+      <c r="H78" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="I78" s="113" t="s">
+      <c r="I78" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="J78" s="115" t="s">
+      <c r="J78" s="50" t="s">
         <v>110</v>
       </c>
-      <c r="K78" s="115" t="s">
+      <c r="K78" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="L78" s="112" t="s">
+      <c r="L78" s="47" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="79" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="56" t="s">
+      <c r="A79" s="73" t="s">
         <v>53</v>
       </c>
-      <c r="B79" s="76"/>
-      <c r="C79" s="76"/>
-      <c r="D79" s="57"/>
-      <c r="E79" s="77"/>
+      <c r="B79" s="111"/>
+      <c r="C79" s="111"/>
+      <c r="D79" s="74"/>
+      <c r="E79" s="35"/>
       <c r="F79" s="3"/>
-      <c r="G79" s="85" t="s">
+      <c r="G79" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="H79" s="65"/>
-      <c r="I79" s="51"/>
-      <c r="J79" s="51"/>
-      <c r="K79" s="51"/>
-      <c r="L79" s="65"/>
+      <c r="H79" s="28"/>
+      <c r="I79" s="22"/>
+      <c r="J79" s="22"/>
+      <c r="K79" s="22"/>
+      <c r="L79" s="28"/>
     </row>
     <row r="80" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="61" t="s">
+      <c r="A80" s="90" t="s">
         <v>54</v>
       </c>
-      <c r="B80" s="78"/>
-      <c r="C80" s="78"/>
-      <c r="D80" s="62"/>
-      <c r="E80" s="79"/>
+      <c r="B80" s="121"/>
+      <c r="C80" s="121"/>
+      <c r="D80" s="91"/>
+      <c r="E80" s="36"/>
       <c r="F80" s="3"/>
-      <c r="G80" s="86" t="s">
+      <c r="G80" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="H80" s="51"/>
-      <c r="I80" s="51"/>
-      <c r="J80" s="51"/>
-      <c r="K80" s="51"/>
-      <c r="L80" s="51"/>
+      <c r="H80" s="22"/>
+      <c r="I80" s="22"/>
+      <c r="J80" s="22"/>
+      <c r="K80" s="22"/>
+      <c r="L80" s="22"/>
     </row>
     <row r="81" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F81" s="3"/>
-      <c r="G81" s="85" t="s">
+      <c r="G81" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="H81" s="51"/>
-      <c r="I81" s="51"/>
-      <c r="J81" s="51"/>
-      <c r="K81" s="51"/>
-      <c r="L81" s="51"/>
+      <c r="H81" s="22"/>
+      <c r="I81" s="22"/>
+      <c r="J81" s="22"/>
+      <c r="K81" s="22"/>
+      <c r="L81" s="22"/>
     </row>
     <row r="82" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A82" s="31" t="s">
+      <c r="A82" s="104" t="s">
         <v>4</v>
       </c>
-      <c r="B82" s="32"/>
-      <c r="C82" s="32"/>
-      <c r="D82" s="32"/>
-      <c r="E82" s="33"/>
+      <c r="B82" s="105"/>
+      <c r="C82" s="105"/>
+      <c r="D82" s="105"/>
+      <c r="E82" s="106"/>
       <c r="F82" s="3"/>
-      <c r="G82" s="86" t="s">
+      <c r="G82" s="39" t="s">
         <v>111</v>
       </c>
-      <c r="H82" s="51"/>
-      <c r="I82" s="51"/>
-      <c r="J82" s="51"/>
-      <c r="K82" s="51"/>
-      <c r="L82" s="51"/>
+      <c r="H82" s="22"/>
+      <c r="I82" s="22"/>
+      <c r="J82" s="22"/>
+      <c r="K82" s="22"/>
+      <c r="L82" s="22"/>
     </row>
     <row r="83" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="111" t="s">
+      <c r="A83" s="107" t="s">
         <v>35</v>
       </c>
-      <c r="B83" s="103"/>
-      <c r="C83" s="97" t="s">
+      <c r="B83" s="99"/>
+      <c r="C83" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="D83" s="113" t="s">
+      <c r="D83" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="E83" s="112" t="s">
+      <c r="E83" s="47" t="s">
         <v>37</v>
       </c>
       <c r="F83" s="3"/>
-      <c r="G83" s="39" t="s">
+      <c r="G83" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="H83" s="40"/>
-      <c r="I83" s="40"/>
-      <c r="J83" s="40"/>
-      <c r="K83" s="40"/>
-      <c r="L83" s="41"/>
+      <c r="H83" s="16"/>
+      <c r="I83" s="16"/>
+      <c r="J83" s="16"/>
+      <c r="K83" s="16"/>
+      <c r="L83" s="17"/>
     </row>
     <row r="84" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="56"/>
-      <c r="B84" s="57"/>
-      <c r="C84" s="65"/>
-      <c r="D84" s="51"/>
-      <c r="E84" s="66"/>
+      <c r="A84" s="73"/>
+      <c r="B84" s="74"/>
+      <c r="C84" s="28"/>
+      <c r="D84" s="22"/>
+      <c r="E84" s="29"/>
       <c r="F84" s="3"/>
-      <c r="G84" s="42" t="s">
+      <c r="G84" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="H84" s="43"/>
-      <c r="I84" s="121"/>
-      <c r="J84" s="44"/>
-      <c r="K84" s="44"/>
-      <c r="L84" s="44"/>
+      <c r="H84" s="19"/>
+      <c r="I84" s="52"/>
+      <c r="J84" s="20"/>
+      <c r="K84" s="20"/>
+      <c r="L84" s="20"/>
     </row>
     <row r="85" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="56"/>
-      <c r="B85" s="57"/>
-      <c r="C85" s="51"/>
-      <c r="D85" s="51"/>
-      <c r="E85" s="67"/>
+      <c r="A85" s="73"/>
+      <c r="B85" s="74"/>
+      <c r="C85" s="22"/>
+      <c r="D85" s="22"/>
+      <c r="E85" s="30"/>
       <c r="F85" s="3"/>
     </row>
     <row r="86" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A86" s="56"/>
-      <c r="B86" s="57"/>
-      <c r="C86" s="51"/>
-      <c r="D86" s="51"/>
-      <c r="E86" s="67"/>
+      <c r="A86" s="73"/>
+      <c r="B86" s="74"/>
+      <c r="C86" s="22"/>
+      <c r="D86" s="22"/>
+      <c r="E86" s="30"/>
       <c r="F86" s="3"/>
-      <c r="G86" s="8" t="s">
+      <c r="G86" s="53" t="s">
         <v>128</v>
       </c>
-      <c r="H86" s="10"/>
+      <c r="H86" s="55"/>
     </row>
     <row r="87" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="56"/>
-      <c r="B87" s="57"/>
-      <c r="C87" s="51"/>
-      <c r="D87" s="51"/>
-      <c r="E87" s="67"/>
+      <c r="A87" s="73"/>
+      <c r="B87" s="74"/>
+      <c r="C87" s="22"/>
+      <c r="D87" s="22"/>
+      <c r="E87" s="30"/>
       <c r="F87" s="3"/>
-      <c r="G87" s="22" t="s">
+      <c r="G87" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="H87" s="28" t="s">
+      <c r="H87" s="12" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="88" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="56"/>
-      <c r="B88" s="57"/>
-      <c r="C88" s="51"/>
-      <c r="D88" s="51"/>
-      <c r="E88" s="67"/>
+      <c r="A88" s="73"/>
+      <c r="B88" s="74"/>
+      <c r="C88" s="22"/>
+      <c r="D88" s="22"/>
+      <c r="E88" s="30"/>
       <c r="F88" s="3"/>
-      <c r="G88" s="84" t="s">
+      <c r="G88" s="37" t="s">
         <v>117</v>
       </c>
-      <c r="H88" s="84"/>
+      <c r="H88" s="37"/>
     </row>
     <row r="89" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="56"/>
-      <c r="B89" s="57"/>
-      <c r="C89" s="51"/>
-      <c r="D89" s="51"/>
-      <c r="E89" s="67"/>
+      <c r="A89" s="73"/>
+      <c r="B89" s="74"/>
+      <c r="C89" s="22"/>
+      <c r="D89" s="22"/>
+      <c r="E89" s="30"/>
       <c r="F89" s="3"/>
-      <c r="G89" s="84" t="s">
+      <c r="G89" s="37" t="s">
         <v>118</v>
       </c>
-      <c r="H89" s="84"/>
+      <c r="H89" s="37"/>
     </row>
     <row r="90" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="56"/>
-      <c r="B90" s="57"/>
-      <c r="C90" s="51"/>
-      <c r="D90" s="51"/>
-      <c r="E90" s="67"/>
+      <c r="A90" s="73"/>
+      <c r="B90" s="74"/>
+      <c r="C90" s="22"/>
+      <c r="D90" s="22"/>
+      <c r="E90" s="30"/>
       <c r="F90" s="3"/>
-      <c r="G90" s="84" t="s">
+      <c r="G90" s="37" t="s">
         <v>119</v>
       </c>
-      <c r="H90" s="84"/>
+      <c r="H90" s="37"/>
     </row>
     <row r="91" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="56"/>
-      <c r="B91" s="57"/>
-      <c r="C91" s="51"/>
-      <c r="D91" s="51"/>
-      <c r="E91" s="67"/>
+      <c r="A91" s="73"/>
+      <c r="B91" s="74"/>
+      <c r="C91" s="22"/>
+      <c r="D91" s="22"/>
+      <c r="E91" s="30"/>
       <c r="F91" s="3"/>
-      <c r="G91" s="84" t="s">
+      <c r="G91" s="37" t="s">
         <v>120</v>
       </c>
-      <c r="H91" s="84"/>
+      <c r="H91" s="37"/>
     </row>
     <row r="92" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="56"/>
-      <c r="B92" s="57"/>
-      <c r="C92" s="51"/>
-      <c r="D92" s="51"/>
-      <c r="E92" s="67"/>
+      <c r="A92" s="73"/>
+      <c r="B92" s="74"/>
+      <c r="C92" s="22"/>
+      <c r="D92" s="22"/>
+      <c r="E92" s="30"/>
       <c r="F92" s="3"/>
-      <c r="G92" s="84" t="s">
+      <c r="G92" s="37" t="s">
         <v>121</v>
       </c>
-      <c r="H92" s="84"/>
+      <c r="H92" s="37"/>
     </row>
     <row r="93" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="56"/>
-      <c r="B93" s="57"/>
-      <c r="C93" s="51"/>
-      <c r="D93" s="51"/>
-      <c r="E93" s="67"/>
+      <c r="A93" s="73"/>
+      <c r="B93" s="74"/>
+      <c r="C93" s="22"/>
+      <c r="D93" s="22"/>
+      <c r="E93" s="30"/>
       <c r="F93" s="3"/>
-      <c r="G93" s="84" t="s">
+      <c r="G93" s="37" t="s">
         <v>122</v>
       </c>
-      <c r="H93" s="84"/>
+      <c r="H93" s="37"/>
     </row>
     <row r="94" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="56"/>
-      <c r="B94" s="57"/>
-      <c r="C94" s="51"/>
-      <c r="D94" s="51"/>
-      <c r="E94" s="67"/>
+      <c r="A94" s="73"/>
+      <c r="B94" s="74"/>
+      <c r="C94" s="22"/>
+      <c r="D94" s="22"/>
+      <c r="E94" s="30"/>
       <c r="F94" s="3"/>
-      <c r="G94" s="84" t="s">
+      <c r="G94" s="37" t="s">
         <v>123</v>
       </c>
-      <c r="H94" s="84"/>
+      <c r="H94" s="37"/>
     </row>
     <row r="95" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="56"/>
-      <c r="B95" s="57"/>
-      <c r="C95" s="51"/>
-      <c r="D95" s="51"/>
-      <c r="E95" s="67"/>
+      <c r="A95" s="73"/>
+      <c r="B95" s="74"/>
+      <c r="C95" s="22"/>
+      <c r="D95" s="22"/>
+      <c r="E95" s="30"/>
       <c r="F95" s="3"/>
-      <c r="G95" s="84" t="s">
+      <c r="G95" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="H95" s="84"/>
+      <c r="H95" s="37"/>
     </row>
     <row r="96" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="56"/>
-      <c r="B96" s="57"/>
-      <c r="C96" s="51"/>
-      <c r="D96" s="51"/>
-      <c r="E96" s="67"/>
+      <c r="A96" s="73"/>
+      <c r="B96" s="74"/>
+      <c r="C96" s="22"/>
+      <c r="D96" s="22"/>
+      <c r="E96" s="30"/>
       <c r="F96" s="3"/>
-      <c r="G96" s="84" t="s">
+      <c r="G96" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="H96" s="84"/>
-    </row>
-    <row r="97" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="56"/>
-      <c r="B97" s="57"/>
-      <c r="C97" s="51"/>
-      <c r="D97" s="51"/>
-      <c r="E97" s="67"/>
+      <c r="H96" s="37"/>
+    </row>
+    <row r="97" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="73"/>
+      <c r="B97" s="74"/>
+      <c r="C97" s="22"/>
+      <c r="D97" s="22"/>
+      <c r="E97" s="30"/>
       <c r="F97" s="3"/>
     </row>
-    <row r="98" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="56"/>
-      <c r="B98" s="57"/>
-      <c r="C98" s="51"/>
-      <c r="D98" s="51"/>
-      <c r="E98" s="67"/>
+    <row r="98" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="73"/>
+      <c r="B98" s="74"/>
+      <c r="C98" s="22"/>
+      <c r="D98" s="22"/>
+      <c r="E98" s="30"/>
       <c r="F98" s="3"/>
-    </row>
-    <row r="99" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="56"/>
-      <c r="B99" s="57"/>
-      <c r="C99" s="51"/>
-      <c r="D99" s="51"/>
-      <c r="E99" s="67"/>
+      <c r="G98" s="123" t="s">
+        <v>129</v>
+      </c>
+      <c r="H98" s="124"/>
+      <c r="I98" s="124"/>
+      <c r="J98" s="124"/>
+      <c r="K98" s="124"/>
+      <c r="L98" s="125"/>
+    </row>
+    <row r="99" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="73"/>
+      <c r="B99" s="74"/>
+      <c r="C99" s="22"/>
+      <c r="D99" s="22"/>
+      <c r="E99" s="30"/>
       <c r="F99" s="3"/>
-    </row>
-    <row r="100" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="56"/>
-      <c r="B100" s="57"/>
-      <c r="C100" s="51"/>
-      <c r="D100" s="51"/>
-      <c r="E100" s="67"/>
+      <c r="G99" s="126"/>
+      <c r="H99" s="127"/>
+      <c r="I99" s="127"/>
+      <c r="J99" s="127"/>
+      <c r="K99" s="127"/>
+      <c r="L99" s="128"/>
+    </row>
+    <row r="100" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="73"/>
+      <c r="B100" s="74"/>
+      <c r="C100" s="22"/>
+      <c r="D100" s="22"/>
+      <c r="E100" s="30"/>
       <c r="F100" s="3"/>
-    </row>
-    <row r="101" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="80"/>
-      <c r="B101" s="81"/>
-      <c r="C101" s="51"/>
-      <c r="D101" s="51"/>
-      <c r="E101" s="67"/>
+      <c r="G100" s="129"/>
+      <c r="H100" s="130"/>
+      <c r="I100" s="130"/>
+      <c r="J100" s="130"/>
+      <c r="K100" s="130"/>
+      <c r="L100" s="131"/>
+    </row>
+    <row r="101" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A101" s="119"/>
+      <c r="B101" s="120"/>
+      <c r="C101" s="22"/>
+      <c r="D101" s="22"/>
+      <c r="E101" s="30"/>
       <c r="F101" s="3"/>
-    </row>
-    <row r="102" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="18" t="s">
+      <c r="G101" s="129"/>
+      <c r="H101" s="130"/>
+      <c r="I101" s="130"/>
+      <c r="J101" s="130"/>
+      <c r="K101" s="130"/>
+      <c r="L101" s="131"/>
+    </row>
+    <row r="102" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A102" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="B102" s="26"/>
-      <c r="C102" s="26"/>
-      <c r="D102" s="34"/>
-      <c r="E102" s="35"/>
+      <c r="B102" s="88"/>
+      <c r="C102" s="88"/>
+      <c r="D102" s="110"/>
+      <c r="E102" s="14"/>
       <c r="F102" s="3"/>
-    </row>
-    <row r="103" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G102" s="132"/>
+      <c r="H102" s="122"/>
+      <c r="I102" s="122"/>
+      <c r="J102" s="122"/>
+      <c r="K102" s="122"/>
+      <c r="L102" s="133"/>
+    </row>
+    <row r="103" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F103" s="3"/>
     </row>
-    <row r="104" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A104" s="36" t="s">
+    <row r="104" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A104" s="112" t="s">
         <v>7</v>
       </c>
-      <c r="B104" s="37"/>
-      <c r="C104" s="37"/>
-      <c r="D104" s="37"/>
-      <c r="E104" s="38"/>
+      <c r="B104" s="113"/>
+      <c r="C104" s="113"/>
+      <c r="D104" s="113"/>
+      <c r="E104" s="114"/>
       <c r="F104" s="3"/>
     </row>
-    <row r="105" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="116" t="s">
+    <row r="105" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="115" t="s">
         <v>45</v>
       </c>
-      <c r="B105" s="117"/>
-      <c r="C105" s="97" t="s">
+      <c r="B105" s="116"/>
+      <c r="C105" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="D105" s="97" t="s">
+      <c r="D105" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="E105" s="112" t="s">
+      <c r="E105" s="47" t="s">
         <v>48</v>
       </c>
       <c r="F105" s="3"/>
     </row>
-    <row r="106" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="82"/>
-      <c r="B106" s="83"/>
-      <c r="C106" s="65"/>
-      <c r="D106" s="65"/>
-      <c r="E106" s="66"/>
+    <row r="106" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="108"/>
+      <c r="B106" s="109"/>
+      <c r="C106" s="28"/>
+      <c r="D106" s="28"/>
+      <c r="E106" s="29"/>
       <c r="F106" s="3"/>
     </row>
-    <row r="107" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="59"/>
-      <c r="B107" s="60"/>
-      <c r="C107" s="51"/>
-      <c r="D107" s="51"/>
-      <c r="E107" s="67"/>
+    <row r="107" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="83"/>
+      <c r="B107" s="84"/>
+      <c r="C107" s="22"/>
+      <c r="D107" s="22"/>
+      <c r="E107" s="30"/>
       <c r="F107" s="3"/>
     </row>
-    <row r="108" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="59"/>
-      <c r="B108" s="60"/>
-      <c r="C108" s="65"/>
-      <c r="D108" s="65"/>
-      <c r="E108" s="66"/>
+    <row r="108" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="83"/>
+      <c r="B108" s="84"/>
+      <c r="C108" s="28"/>
+      <c r="D108" s="28"/>
+      <c r="E108" s="29"/>
       <c r="F108" s="3"/>
     </row>
-    <row r="109" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="59"/>
-      <c r="B109" s="60"/>
-      <c r="C109" s="51"/>
-      <c r="D109" s="51"/>
-      <c r="E109" s="67"/>
+    <row r="109" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="83"/>
+      <c r="B109" s="84"/>
+      <c r="C109" s="22"/>
+      <c r="D109" s="22"/>
+      <c r="E109" s="30"/>
       <c r="F109" s="3"/>
     </row>
-    <row r="110" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="59"/>
-      <c r="B110" s="60"/>
-      <c r="C110" s="65"/>
-      <c r="D110" s="65"/>
-      <c r="E110" s="66"/>
+    <row r="110" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="83"/>
+      <c r="B110" s="84"/>
+      <c r="C110" s="28"/>
+      <c r="D110" s="28"/>
+      <c r="E110" s="29"/>
       <c r="F110" s="3"/>
     </row>
-    <row r="111" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="59"/>
-      <c r="B111" s="60"/>
-      <c r="C111" s="51"/>
-      <c r="D111" s="51"/>
-      <c r="E111" s="67"/>
+    <row r="111" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="83"/>
+      <c r="B111" s="84"/>
+      <c r="C111" s="22"/>
+      <c r="D111" s="22"/>
+      <c r="E111" s="30"/>
       <c r="F111" s="3"/>
     </row>
-    <row r="112" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="59"/>
-      <c r="B112" s="60"/>
-      <c r="C112" s="65"/>
-      <c r="D112" s="65"/>
-      <c r="E112" s="66"/>
+    <row r="112" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="83"/>
+      <c r="B112" s="84"/>
+      <c r="C112" s="28"/>
+      <c r="D112" s="28"/>
+      <c r="E112" s="29"/>
       <c r="F112" s="3"/>
     </row>
     <row r="113" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="59"/>
-      <c r="B113" s="60"/>
-      <c r="C113" s="51"/>
-      <c r="D113" s="51"/>
-      <c r="E113" s="67"/>
+      <c r="A113" s="83"/>
+      <c r="B113" s="84"/>
+      <c r="C113" s="22"/>
+      <c r="D113" s="22"/>
+      <c r="E113" s="30"/>
       <c r="F113" s="3"/>
     </row>
     <row r="114" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="59"/>
-      <c r="B114" s="60"/>
-      <c r="C114" s="51"/>
-      <c r="D114" s="51"/>
-      <c r="E114" s="66"/>
+      <c r="A114" s="83"/>
+      <c r="B114" s="84"/>
+      <c r="C114" s="22"/>
+      <c r="D114" s="22"/>
+      <c r="E114" s="29"/>
       <c r="F114" s="3"/>
     </row>
     <row r="115" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="59"/>
-      <c r="B115" s="60"/>
-      <c r="C115" s="51"/>
-      <c r="D115" s="51"/>
-      <c r="E115" s="67"/>
+      <c r="A115" s="83"/>
+      <c r="B115" s="84"/>
+      <c r="C115" s="22"/>
+      <c r="D115" s="22"/>
+      <c r="E115" s="30"/>
       <c r="F115" s="3"/>
     </row>
     <row r="116" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="59"/>
-      <c r="B116" s="60"/>
-      <c r="C116" s="51"/>
-      <c r="D116" s="51"/>
-      <c r="E116" s="66"/>
+      <c r="A116" s="83"/>
+      <c r="B116" s="84"/>
+      <c r="C116" s="22"/>
+      <c r="D116" s="22"/>
+      <c r="E116" s="29"/>
       <c r="F116" s="3"/>
     </row>
     <row r="117" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="59"/>
-      <c r="B117" s="60"/>
-      <c r="C117" s="51"/>
-      <c r="D117" s="51"/>
-      <c r="E117" s="67"/>
+      <c r="A117" s="83"/>
+      <c r="B117" s="84"/>
+      <c r="C117" s="22"/>
+      <c r="D117" s="22"/>
+      <c r="E117" s="30"/>
       <c r="F117" s="3"/>
     </row>
     <row r="118" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="59"/>
-      <c r="B118" s="60"/>
-      <c r="C118" s="51"/>
-      <c r="D118" s="51"/>
-      <c r="E118" s="66"/>
+      <c r="A118" s="83"/>
+      <c r="B118" s="84"/>
+      <c r="C118" s="22"/>
+      <c r="D118" s="22"/>
+      <c r="E118" s="29"/>
       <c r="F118" s="3"/>
     </row>
     <row r="119" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="59"/>
-      <c r="B119" s="60"/>
-      <c r="C119" s="51"/>
-      <c r="D119" s="51"/>
-      <c r="E119" s="67"/>
+      <c r="A119" s="83"/>
+      <c r="B119" s="84"/>
+      <c r="C119" s="22"/>
+      <c r="D119" s="22"/>
+      <c r="E119" s="30"/>
       <c r="F119" s="3"/>
     </row>
     <row r="120" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="59"/>
-      <c r="B120" s="60"/>
-      <c r="C120" s="51"/>
-      <c r="D120" s="51"/>
-      <c r="E120" s="67"/>
+      <c r="A120" s="83"/>
+      <c r="B120" s="84"/>
+      <c r="C120" s="22"/>
+      <c r="D120" s="22"/>
+      <c r="E120" s="30"/>
       <c r="F120" s="3"/>
     </row>
     <row r="121" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="59"/>
-      <c r="B121" s="60"/>
-      <c r="C121" s="51"/>
-      <c r="D121" s="51"/>
-      <c r="E121" s="67"/>
+      <c r="A121" s="83"/>
+      <c r="B121" s="84"/>
+      <c r="C121" s="22"/>
+      <c r="D121" s="22"/>
+      <c r="E121" s="30"/>
       <c r="F121" s="3"/>
     </row>
     <row r="122" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="59"/>
-      <c r="B122" s="60"/>
-      <c r="C122" s="51"/>
-      <c r="D122" s="51"/>
-      <c r="E122" s="67"/>
+      <c r="A122" s="83"/>
+      <c r="B122" s="84"/>
+      <c r="C122" s="22"/>
+      <c r="D122" s="22"/>
+      <c r="E122" s="30"/>
       <c r="F122" s="3"/>
     </row>
     <row r="123" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A123" s="59"/>
-      <c r="B123" s="60"/>
-      <c r="C123" s="51"/>
-      <c r="D123" s="51"/>
-      <c r="E123" s="67"/>
+      <c r="A123" s="83"/>
+      <c r="B123" s="84"/>
+      <c r="C123" s="22"/>
+      <c r="D123" s="22"/>
+      <c r="E123" s="30"/>
       <c r="F123" s="3"/>
     </row>
     <row r="124" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A124" s="18" t="s">
+      <c r="A124" s="87" t="s">
         <v>114</v>
       </c>
-      <c r="B124" s="26"/>
-      <c r="C124" s="26"/>
-      <c r="D124" s="34"/>
-      <c r="E124" s="35"/>
+      <c r="B124" s="88"/>
+      <c r="C124" s="88"/>
+      <c r="D124" s="110"/>
+      <c r="E124" s="14"/>
       <c r="F124" s="3"/>
     </row>
     <row r="125" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -4546,7 +4699,170 @@
       <c r="E219" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="185">
+  <mergeCells count="187">
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A116:B116"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="A80:D80"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A57:E57"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A77:D77"/>
+    <mergeCell ref="A78:D78"/>
+    <mergeCell ref="A79:D79"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="A114:B114"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="G59:H59"/>
+    <mergeCell ref="G60:H60"/>
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="G71:H71"/>
+    <mergeCell ref="G72:H72"/>
+    <mergeCell ref="G73:H73"/>
+    <mergeCell ref="G74:H74"/>
+    <mergeCell ref="G75:H75"/>
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="G67:H67"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="G69:H69"/>
+    <mergeCell ref="A102:D102"/>
+    <mergeCell ref="A68:E68"/>
+    <mergeCell ref="G86:H86"/>
+    <mergeCell ref="G99:L102"/>
+    <mergeCell ref="G98:L98"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="A124:D124"/>
+    <mergeCell ref="A75:E75"/>
+    <mergeCell ref="A76:D76"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="A104:E104"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="G62:H62"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="A73:D73"/>
+    <mergeCell ref="G61:H61"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="G70:H70"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="A53:C53"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="A46:E46"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="A82:E82"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="A13:D13"/>
     <mergeCell ref="G77:L77"/>
     <mergeCell ref="G41:L41"/>
     <mergeCell ref="G42:H42"/>
@@ -4571,167 +4887,6 @@
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="G13:H13"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="A53:C53"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="G57:H57"/>
-    <mergeCell ref="A46:E46"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="A82:E82"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="A73:D73"/>
-    <mergeCell ref="G61:H61"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="G52:H52"/>
-    <mergeCell ref="G70:H70"/>
-    <mergeCell ref="G53:H53"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="A124:D124"/>
-    <mergeCell ref="A75:E75"/>
-    <mergeCell ref="A76:D76"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="A104:E104"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="G62:H62"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="G59:H59"/>
-    <mergeCell ref="G60:H60"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="G71:H71"/>
-    <mergeCell ref="G72:H72"/>
-    <mergeCell ref="G73:H73"/>
-    <mergeCell ref="G74:H74"/>
-    <mergeCell ref="G75:H75"/>
-    <mergeCell ref="A64:C64"/>
-    <mergeCell ref="G66:H66"/>
-    <mergeCell ref="G67:H67"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="G69:H69"/>
-    <mergeCell ref="A102:D102"/>
-    <mergeCell ref="A68:E68"/>
-    <mergeCell ref="G86:H86"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A116:B116"/>
-    <mergeCell ref="A117:B117"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="A80:D80"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="A57:E57"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A77:D77"/>
-    <mergeCell ref="A78:D78"/>
-    <mergeCell ref="A79:D79"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="A114:B114"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A39:B39"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
1.Version 2.0 Updation for estimates and Tool 2. MinLabor issue for Reseal all systems 3. 201/250 old estimate load issue. 4. Copied/replicated estimates causing issue in selection pane.
</commit_message>
<xml_diff>
--- a/WICR Estimator/SummaryTemplate.xlsx
+++ b/WICR Estimator/SummaryTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\priya\Downloads\WICR Estimator_No Apply button\WICR Estimator\WICR Estimator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC50BD0-EB52-4879-87AE-8D8803FF2411}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BECA53B-9D72-4767-BB91-59AEB3AE160C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="347" xr2:uid="{C3BB3D69-FD31-4C45-AAE2-714CBD52CC32}"/>
   </bookViews>
@@ -29,7 +29,7 @@
     <definedName name="PRate">'[1]Job set up'!$B$19</definedName>
     <definedName name="stairWidth">'[1]Job set up'!$B$12</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="132">
   <si>
     <t>Job Setup</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Sq ft</t>
   </si>
   <si>
-    <t># decks or areas</t>
-  </si>
-  <si>
     <t xml:space="preserve">Total </t>
   </si>
   <si>
@@ -164,9 +161,6 @@
     <t>Sales Price</t>
   </si>
   <si>
-    <t>Sub Contract Labor</t>
-  </si>
-  <si>
     <t>Item</t>
   </si>
   <si>
@@ -435,13 +429,25 @@
   </si>
   <si>
     <t>Notes to Bill:</t>
+  </si>
+  <si>
+    <t>SubContract Labor</t>
+  </si>
+  <si>
+    <t>MATERIAL EXTN</t>
+  </si>
+  <si>
+    <t>LABOR EXTN</t>
+  </si>
+  <si>
+    <t>Areas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -456,11 +462,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="6"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -497,7 +498,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="71">
+  <borders count="74">
     <border>
       <left/>
       <right/>
@@ -1411,12 +1412,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyProtection="1"/>
@@ -1424,43 +1458,43 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="40" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="40" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="41" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="41" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1469,9 +1503,6 @@
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1494,84 +1525,270 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="35" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="35" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="56" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="57" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="57" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="58" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="58" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="59" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="59" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="53" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="53" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="62" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="62" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="35" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="55" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="52" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="42" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="63" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="64" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="65" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="66" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="67" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="68" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="69" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="70" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="61" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="60" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="53" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="54" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="50" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="35" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="52" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="50" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1580,195 +1797,28 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="71" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="56" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="3" borderId="35" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="3" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="3" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="53" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="54" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="55" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="3" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="3" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="3" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="35" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="42" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="3" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="3" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="3" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="61" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="60" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="69" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="70" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="63" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="64" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="65" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="66" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="67" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="68" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="70" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="72" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="73" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2213,24 +2263,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13628510-9764-4D87-A543-465B04714C1D}">
   <dimension ref="A1:BD219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="G99" sqref="G99:L102"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.1328125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="8.3984375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="24.9296875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="7.1328125" style="2" customWidth="1"/>
     <col min="3" max="3" width="9.73046875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.06640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="13.73046875" style="2" customWidth="1"/>
     <col min="6" max="6" width="1.73046875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="29.1328125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.3984375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="27.265625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="8.53125" style="2" customWidth="1"/>
     <col min="9" max="9" width="8.86328125" style="2"/>
     <col min="10" max="10" width="8.86328125" style="2" customWidth="1"/>
     <col min="11" max="11" width="9.265625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="11.3984375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="13.53125" style="2" customWidth="1"/>
     <col min="13" max="14" width="8.86328125" style="2"/>
     <col min="15" max="15" width="10.59765625" style="2" customWidth="1"/>
     <col min="16" max="16" width="2.73046875" style="2" customWidth="1"/>
@@ -2260,649 +2310,655 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="55"/>
-      <c r="G1" s="60" t="s">
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="86"/>
+      <c r="G1" s="121" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="61"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="63"/>
+      <c r="H1" s="122"/>
+      <c r="I1" s="123"/>
+      <c r="J1" s="123"/>
+      <c r="K1" s="123"/>
+      <c r="L1" s="124"/>
     </row>
     <row r="2" spans="1:32" ht="12.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="64" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="66"/>
+      <c r="A2" s="125" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="126"/>
+      <c r="C2" s="126"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="127"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="67" t="s">
-        <v>84</v>
-      </c>
-      <c r="H2" s="68"/>
-      <c r="I2" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="J2" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="K2" s="41" t="s">
-        <v>77</v>
-      </c>
-      <c r="L2" s="41" t="s">
-        <v>115</v>
+      <c r="G2" s="128" t="s">
+        <v>82</v>
+      </c>
+      <c r="H2" s="129"/>
+      <c r="I2" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="L2" s="40" t="s">
+        <v>113</v>
       </c>
       <c r="P2" s="4"/>
       <c r="AA2" s="4"/>
       <c r="AF2" s="4"/>
     </row>
     <row r="3" spans="1:32" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="69" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
+      <c r="A3" s="130" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="131"/>
+      <c r="C3" s="131"/>
+      <c r="D3" s="131"/>
       <c r="E3" s="23"/>
       <c r="F3" s="5"/>
-      <c r="G3" s="71" t="s">
-        <v>67</v>
-      </c>
-      <c r="H3" s="72"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="40"/>
+      <c r="G3" s="116" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="117"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="39"/>
     </row>
     <row r="4" spans="1:32" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="75" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" s="76"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
+      <c r="A4" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="62"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
       <c r="E4" s="21"/>
       <c r="F4" s="5"/>
-      <c r="G4" s="73" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="74"/>
+      <c r="G4" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="67"/>
       <c r="I4" s="22"/>
       <c r="J4" s="22"/>
       <c r="K4" s="22"/>
-      <c r="L4" s="25"/>
+      <c r="L4" s="24"/>
     </row>
     <row r="5" spans="1:32" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="75" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" s="76"/>
-      <c r="C5" s="76"/>
-      <c r="D5" s="76"/>
+      <c r="A5" s="61" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="62"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
       <c r="E5" s="21"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="73" t="s">
-        <v>68</v>
-      </c>
-      <c r="H5" s="74"/>
+      <c r="G5" s="66" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" s="67"/>
       <c r="I5" s="22"/>
       <c r="J5" s="22"/>
       <c r="K5" s="22"/>
-      <c r="L5" s="25"/>
+      <c r="L5" s="24"/>
     </row>
     <row r="6" spans="1:32" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="75" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="76"/>
-      <c r="C6" s="76"/>
-      <c r="D6" s="76"/>
+      <c r="A6" s="61" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="62"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
       <c r="E6" s="21"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="73" t="s">
-        <v>69</v>
-      </c>
-      <c r="H6" s="74"/>
+      <c r="G6" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="H6" s="67"/>
       <c r="I6" s="22"/>
       <c r="J6" s="22"/>
       <c r="K6" s="22"/>
-      <c r="L6" s="25"/>
+      <c r="L6" s="24"/>
     </row>
     <row r="7" spans="1:32" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="77" t="s">
-        <v>60</v>
-      </c>
-      <c r="B7" s="78"/>
-      <c r="C7" s="79"/>
+      <c r="A7" s="53" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
       <c r="D7" s="22"/>
       <c r="E7" s="21"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="73" t="s">
-        <v>70</v>
-      </c>
-      <c r="H7" s="74"/>
+      <c r="G7" s="66" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" s="67"/>
       <c r="I7" s="22"/>
       <c r="J7" s="22"/>
       <c r="K7" s="22"/>
-      <c r="L7" s="25"/>
+      <c r="L7" s="24"/>
     </row>
     <row r="8" spans="1:32" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="75" t="s">
-        <v>61</v>
-      </c>
-      <c r="B8" s="76"/>
-      <c r="C8" s="76"/>
-      <c r="D8" s="76"/>
+      <c r="A8" s="61" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="62"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="62"/>
       <c r="E8" s="21"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="73" t="s">
-        <v>71</v>
-      </c>
-      <c r="H8" s="74"/>
+      <c r="G8" s="66" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" s="67"/>
       <c r="I8" s="22"/>
       <c r="J8" s="22"/>
       <c r="K8" s="22"/>
-      <c r="L8" s="25"/>
+      <c r="L8" s="24"/>
     </row>
     <row r="9" spans="1:32" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="75" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" s="76"/>
-      <c r="C9" s="76"/>
-      <c r="D9" s="76"/>
+      <c r="A9" s="61" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="62"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="62"/>
       <c r="E9" s="21"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="73" t="s">
-        <v>72</v>
-      </c>
-      <c r="H9" s="74"/>
+      <c r="G9" s="66" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" s="67"/>
       <c r="I9" s="22"/>
       <c r="J9" s="22"/>
       <c r="K9" s="22"/>
-      <c r="L9" s="25"/>
+      <c r="L9" s="24"/>
     </row>
     <row r="10" spans="1:32" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="75" t="s">
-        <v>63</v>
-      </c>
-      <c r="B10" s="76"/>
-      <c r="C10" s="76"/>
-      <c r="D10" s="76"/>
+      <c r="A10" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="62"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
       <c r="E10" s="21"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="73" t="s">
-        <v>73</v>
-      </c>
-      <c r="H10" s="74"/>
+      <c r="G10" s="66" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10" s="67"/>
       <c r="I10" s="22"/>
       <c r="J10" s="22"/>
       <c r="K10" s="22"/>
-      <c r="L10" s="25"/>
+      <c r="L10" s="24"/>
     </row>
     <row r="11" spans="1:32" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="75" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="76"/>
-      <c r="C11" s="76"/>
-      <c r="D11" s="76"/>
+      <c r="A11" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="62"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
       <c r="E11" s="21"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="73" t="s">
-        <v>26</v>
-      </c>
-      <c r="H11" s="74"/>
+      <c r="G11" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="67"/>
       <c r="I11" s="22"/>
       <c r="J11" s="22"/>
       <c r="K11" s="22"/>
-      <c r="L11" s="25"/>
+      <c r="L11" s="24"/>
     </row>
     <row r="12" spans="1:32" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="75" t="s">
-        <v>64</v>
-      </c>
-      <c r="B12" s="76"/>
-      <c r="C12" s="76"/>
-      <c r="D12" s="76"/>
+      <c r="A12" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="62"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="62"/>
       <c r="E12" s="21"/>
       <c r="F12" s="5"/>
-      <c r="G12" s="73" t="s">
-        <v>27</v>
-      </c>
-      <c r="H12" s="74"/>
+      <c r="G12" s="66" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="67"/>
       <c r="I12" s="22"/>
       <c r="J12" s="22"/>
       <c r="K12" s="22"/>
-      <c r="L12" s="25"/>
+      <c r="L12" s="24"/>
     </row>
     <row r="13" spans="1:32" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="77" t="s">
-        <v>65</v>
-      </c>
-      <c r="B13" s="78"/>
-      <c r="C13" s="78"/>
-      <c r="D13" s="79"/>
+      <c r="A13" s="53" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="54"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="55"/>
       <c r="E13" s="21"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="73" t="s">
-        <v>28</v>
-      </c>
-      <c r="H13" s="74"/>
+      <c r="G13" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" s="67"/>
       <c r="I13" s="22"/>
       <c r="J13" s="22"/>
       <c r="K13" s="22"/>
-      <c r="L13" s="25"/>
+      <c r="L13" s="24"/>
     </row>
     <row r="14" spans="1:32" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="69" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="70"/>
-      <c r="C14" s="70"/>
-      <c r="D14" s="70"/>
+      <c r="A14" s="130" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="131"/>
+      <c r="C14" s="131"/>
+      <c r="D14" s="131"/>
       <c r="E14" s="23"/>
       <c r="F14" s="5"/>
-      <c r="G14" s="73" t="s">
-        <v>29</v>
-      </c>
-      <c r="H14" s="74"/>
+      <c r="G14" s="66" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="67"/>
       <c r="I14" s="22"/>
       <c r="J14" s="22"/>
       <c r="K14" s="22"/>
-      <c r="L14" s="25"/>
+      <c r="L14" s="24"/>
     </row>
     <row r="15" spans="1:32" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="75" t="s">
-        <v>81</v>
-      </c>
-      <c r="B15" s="76"/>
-      <c r="C15" s="76"/>
-      <c r="D15" s="76"/>
+      <c r="A15" s="61" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" s="62"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="62"/>
       <c r="E15" s="21"/>
       <c r="F15" s="5"/>
-      <c r="G15" s="73" t="s">
-        <v>30</v>
-      </c>
-      <c r="H15" s="74"/>
+      <c r="G15" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15" s="67"/>
       <c r="I15" s="22"/>
       <c r="J15" s="22"/>
       <c r="K15" s="22"/>
-      <c r="L15" s="25"/>
+      <c r="L15" s="24"/>
     </row>
     <row r="16" spans="1:32" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="75" t="s">
-        <v>82</v>
-      </c>
-      <c r="B16" s="76"/>
-      <c r="C16" s="76"/>
-      <c r="D16" s="76"/>
+      <c r="A16" s="61" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="62"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="62"/>
       <c r="E16" s="21"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="73" t="s">
-        <v>31</v>
-      </c>
-      <c r="H16" s="74"/>
+      <c r="G16" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="67"/>
       <c r="I16" s="22"/>
       <c r="J16" s="22"/>
       <c r="K16" s="22"/>
-      <c r="L16" s="25"/>
+      <c r="L16" s="24"/>
     </row>
     <row r="17" spans="1:12" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="75" t="s">
-        <v>83</v>
-      </c>
-      <c r="B17" s="76"/>
-      <c r="C17" s="76"/>
-      <c r="D17" s="76"/>
+      <c r="A17" s="61" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="62"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="62"/>
       <c r="E17" s="21"/>
       <c r="F17" s="5"/>
-      <c r="G17" s="73" t="s">
-        <v>32</v>
-      </c>
-      <c r="H17" s="74"/>
+      <c r="G17" s="66" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" s="67"/>
       <c r="I17" s="22"/>
       <c r="J17" s="22"/>
       <c r="K17" s="22"/>
-      <c r="L17" s="25"/>
+      <c r="L17" s="24"/>
     </row>
     <row r="18" spans="1:12" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="75"/>
-      <c r="B18" s="76"/>
-      <c r="C18" s="76"/>
-      <c r="D18" s="76"/>
+      <c r="A18" s="61"/>
+      <c r="B18" s="62"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="62"/>
       <c r="E18" s="21"/>
       <c r="F18" s="5"/>
-      <c r="G18" s="73" t="s">
-        <v>33</v>
-      </c>
-      <c r="H18" s="74"/>
+      <c r="G18" s="66" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" s="67"/>
       <c r="I18" s="22"/>
       <c r="J18" s="22"/>
       <c r="K18" s="22"/>
-      <c r="L18" s="25"/>
+      <c r="L18" s="24"/>
     </row>
     <row r="19" spans="1:12" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="76"/>
-      <c r="B19" s="76"/>
-      <c r="C19" s="76"/>
-      <c r="D19" s="76"/>
-      <c r="E19" s="24"/>
+      <c r="A19" s="61"/>
+      <c r="B19" s="62"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="21"/>
       <c r="F19" s="5"/>
-      <c r="G19" s="73" t="s">
-        <v>74</v>
-      </c>
-      <c r="H19" s="74"/>
+      <c r="G19" s="66" t="s">
+        <v>72</v>
+      </c>
+      <c r="H19" s="67"/>
       <c r="I19" s="22"/>
       <c r="J19" s="22"/>
       <c r="K19" s="22"/>
-      <c r="L19" s="25"/>
+      <c r="L19" s="24"/>
     </row>
     <row r="20" spans="1:12" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="76"/>
-      <c r="B20" s="76"/>
-      <c r="C20" s="76"/>
-      <c r="D20" s="76"/>
-      <c r="E20" s="24"/>
+      <c r="A20" s="61"/>
+      <c r="B20" s="62"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="21"/>
       <c r="F20" s="5"/>
-      <c r="G20" s="73" t="s">
-        <v>75</v>
-      </c>
-      <c r="H20" s="74"/>
+      <c r="G20" s="66" t="s">
+        <v>73</v>
+      </c>
+      <c r="H20" s="67"/>
       <c r="I20" s="22"/>
       <c r="J20" s="22"/>
       <c r="K20" s="22"/>
-      <c r="L20" s="25"/>
+      <c r="L20" s="24"/>
     </row>
     <row r="21" spans="1:12" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="76"/>
-      <c r="B21" s="76"/>
-      <c r="C21" s="76"/>
-      <c r="D21" s="76"/>
-      <c r="E21" s="24"/>
+      <c r="A21" s="61"/>
+      <c r="B21" s="62"/>
+      <c r="C21" s="62"/>
+      <c r="D21" s="62"/>
+      <c r="E21" s="21"/>
       <c r="F21" s="5"/>
-      <c r="G21" s="83" t="s">
-        <v>76</v>
-      </c>
-      <c r="H21" s="84"/>
+      <c r="G21" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="H21" s="57"/>
       <c r="I21" s="22"/>
       <c r="J21" s="22"/>
       <c r="K21" s="22"/>
-      <c r="L21" s="25"/>
+      <c r="L21" s="24"/>
     </row>
     <row r="22" spans="1:12" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="76"/>
-      <c r="B22" s="76"/>
-      <c r="C22" s="76"/>
-      <c r="D22" s="76"/>
-      <c r="E22" s="24"/>
-      <c r="G22" s="73" t="s">
-        <v>85</v>
-      </c>
-      <c r="H22" s="74"/>
+      <c r="A22" s="61"/>
+      <c r="B22" s="62"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="21"/>
+      <c r="G22" s="66" t="s">
+        <v>83</v>
+      </c>
+      <c r="H22" s="67"/>
       <c r="I22" s="22"/>
       <c r="J22" s="22"/>
       <c r="K22" s="22"/>
-      <c r="L22" s="25"/>
+      <c r="L22" s="24"/>
     </row>
     <row r="23" spans="1:12" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="76"/>
-      <c r="B23" s="76"/>
-      <c r="C23" s="76"/>
-      <c r="D23" s="76"/>
-      <c r="E23" s="24"/>
-      <c r="G23" s="73" t="s">
-        <v>86</v>
-      </c>
-      <c r="H23" s="74"/>
+      <c r="A23" s="61"/>
+      <c r="B23" s="62"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="21"/>
+      <c r="G23" s="66" t="s">
+        <v>84</v>
+      </c>
+      <c r="H23" s="67"/>
       <c r="I23" s="22"/>
       <c r="J23" s="22"/>
       <c r="K23" s="22"/>
-      <c r="L23" s="25"/>
-    </row>
-    <row r="24" spans="1:12" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="76"/>
-      <c r="B24" s="76"/>
-      <c r="C24" s="76"/>
-      <c r="D24" s="76"/>
-      <c r="E24" s="24"/>
-      <c r="G24" s="73" t="s">
-        <v>87</v>
-      </c>
-      <c r="H24" s="74"/>
+      <c r="L23" s="24"/>
+    </row>
+    <row r="24" spans="1:12" s="6" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="140"/>
+      <c r="B24" s="139"/>
+      <c r="C24" s="139"/>
+      <c r="D24" s="139"/>
+      <c r="E24" s="137"/>
+      <c r="G24" s="66" t="s">
+        <v>85</v>
+      </c>
+      <c r="H24" s="67"/>
       <c r="I24" s="22"/>
       <c r="J24" s="22"/>
       <c r="K24" s="22"/>
-      <c r="L24" s="25"/>
+      <c r="L24" s="24"/>
     </row>
     <row r="25" spans="1:12" s="6" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G25" s="73" t="s">
-        <v>88</v>
-      </c>
-      <c r="H25" s="74"/>
+      <c r="A25" s="138"/>
+      <c r="B25" s="138"/>
+      <c r="D25" s="138"/>
+      <c r="E25" s="136"/>
+      <c r="G25" s="66" t="s">
+        <v>86</v>
+      </c>
+      <c r="H25" s="67"/>
       <c r="I25" s="22"/>
       <c r="J25" s="22"/>
       <c r="K25" s="22"/>
-      <c r="L25" s="25"/>
+      <c r="L25" s="24"/>
     </row>
     <row r="26" spans="1:12" s="6" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="80" t="s">
+      <c r="A26" s="118" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="81"/>
-      <c r="C26" s="81"/>
-      <c r="D26" s="81"/>
-      <c r="E26" s="82"/>
-      <c r="G26" s="73" t="s">
-        <v>89</v>
-      </c>
-      <c r="H26" s="74"/>
+      <c r="B26" s="119"/>
+      <c r="C26" s="119"/>
+      <c r="D26" s="119"/>
+      <c r="E26" s="120"/>
+      <c r="G26" s="66" t="s">
+        <v>87</v>
+      </c>
+      <c r="H26" s="67"/>
       <c r="I26" s="22"/>
       <c r="J26" s="22"/>
       <c r="K26" s="22"/>
-      <c r="L26" s="25"/>
+      <c r="L26" s="24"/>
     </row>
     <row r="27" spans="1:12" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="B27" s="57"/>
-      <c r="C27" s="51" t="s">
-        <v>55</v>
-      </c>
-      <c r="D27" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="E27" s="45" t="s">
-        <v>36</v>
-      </c>
-      <c r="G27" s="73" t="s">
-        <v>90</v>
-      </c>
-      <c r="H27" s="74"/>
+      <c r="A27" s="134" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="52" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="50" t="s">
+        <v>130</v>
+      </c>
+      <c r="D27" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" s="44" t="s">
+        <v>129</v>
+      </c>
+      <c r="G27" s="66" t="s">
+        <v>88</v>
+      </c>
+      <c r="H27" s="67"/>
       <c r="I27" s="22"/>
       <c r="J27" s="22"/>
       <c r="K27" s="22"/>
-      <c r="L27" s="25"/>
+      <c r="L27" s="24"/>
     </row>
     <row r="28" spans="1:12" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="71" t="s">
-        <v>103</v>
-      </c>
-      <c r="B28" s="72"/>
+      <c r="A28" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" s="133"/>
       <c r="C28" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="D28" s="28"/>
-      <c r="E28" s="30"/>
-      <c r="G28" s="73" t="s">
-        <v>91</v>
-      </c>
-      <c r="H28" s="74"/>
+        <v>64</v>
+      </c>
+      <c r="D28" s="27"/>
+      <c r="E28" s="29"/>
+      <c r="G28" s="66" t="s">
+        <v>89</v>
+      </c>
+      <c r="H28" s="67"/>
       <c r="I28" s="22"/>
       <c r="J28" s="22"/>
       <c r="K28" s="22"/>
-      <c r="L28" s="25"/>
+      <c r="L28" s="24"/>
     </row>
     <row r="29" spans="1:12" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="73" t="s">
-        <v>104</v>
-      </c>
-      <c r="B29" s="74"/>
+      <c r="A29" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="B29" s="133"/>
       <c r="C29" s="22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D29" s="22"/>
-      <c r="E29" s="30"/>
-      <c r="G29" s="73" t="s">
-        <v>92</v>
-      </c>
-      <c r="H29" s="74"/>
+      <c r="E29" s="29"/>
+      <c r="G29" s="66" t="s">
+        <v>90</v>
+      </c>
+      <c r="H29" s="67"/>
       <c r="I29" s="22"/>
       <c r="J29" s="22"/>
       <c r="K29" s="22"/>
-      <c r="L29" s="25"/>
+      <c r="L29" s="24"/>
     </row>
     <row r="30" spans="1:12" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="73" t="s">
-        <v>105</v>
-      </c>
-      <c r="B30" s="74"/>
+      <c r="A30" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="B30" s="133"/>
       <c r="C30" s="22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D30" s="22"/>
-      <c r="E30" s="30"/>
+      <c r="E30" s="29"/>
       <c r="F30" s="5"/>
-      <c r="G30" s="73" t="s">
-        <v>93</v>
-      </c>
-      <c r="H30" s="74"/>
+      <c r="G30" s="66" t="s">
+        <v>91</v>
+      </c>
+      <c r="H30" s="67"/>
       <c r="I30" s="22"/>
       <c r="J30" s="22"/>
       <c r="K30" s="22"/>
-      <c r="L30" s="25"/>
+      <c r="L30" s="24"/>
     </row>
     <row r="31" spans="1:12" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="73"/>
-      <c r="B31" s="74"/>
+      <c r="A31" s="22"/>
+      <c r="B31" s="22"/>
       <c r="C31" s="22"/>
       <c r="D31" s="22"/>
-      <c r="E31" s="30"/>
+      <c r="E31" s="29"/>
       <c r="F31" s="5"/>
-      <c r="G31" s="73" t="s">
-        <v>94</v>
-      </c>
-      <c r="H31" s="74"/>
+      <c r="G31" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="H31" s="67"/>
       <c r="I31" s="22"/>
       <c r="J31" s="22"/>
       <c r="K31" s="22"/>
-      <c r="L31" s="25"/>
+      <c r="L31" s="24"/>
     </row>
     <row r="32" spans="1:12" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="73"/>
-      <c r="B32" s="74"/>
+      <c r="A32" s="22"/>
+      <c r="B32" s="22"/>
       <c r="C32" s="22"/>
       <c r="D32" s="22"/>
-      <c r="E32" s="30"/>
+      <c r="E32" s="29"/>
       <c r="F32" s="5"/>
-      <c r="G32" s="73" t="s">
-        <v>95</v>
-      </c>
-      <c r="H32" s="74"/>
+      <c r="G32" s="66" t="s">
+        <v>93</v>
+      </c>
+      <c r="H32" s="67"/>
       <c r="I32" s="22"/>
       <c r="J32" s="22"/>
       <c r="K32" s="22"/>
-      <c r="L32" s="25"/>
+      <c r="L32" s="24"/>
     </row>
     <row r="33" spans="1:56" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="73"/>
-      <c r="B33" s="74"/>
+      <c r="A33" s="22"/>
+      <c r="B33" s="22"/>
       <c r="C33" s="22"/>
       <c r="D33" s="22"/>
-      <c r="E33" s="30"/>
+      <c r="E33" s="29"/>
       <c r="F33" s="5"/>
-      <c r="G33" s="73" t="s">
-        <v>96</v>
-      </c>
-      <c r="H33" s="74"/>
+      <c r="G33" s="66" t="s">
+        <v>94</v>
+      </c>
+      <c r="H33" s="67"/>
       <c r="I33" s="22"/>
       <c r="J33" s="22"/>
       <c r="K33" s="22"/>
-      <c r="L33" s="25"/>
+      <c r="L33" s="24"/>
     </row>
     <row r="34" spans="1:56" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="73"/>
-      <c r="B34" s="74"/>
+      <c r="A34" s="22"/>
+      <c r="B34" s="22"/>
       <c r="C34" s="22"/>
       <c r="D34" s="22"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="73" t="s">
-        <v>97</v>
-      </c>
-      <c r="H34" s="74"/>
+      <c r="E34" s="141"/>
+      <c r="F34" s="142"/>
+      <c r="G34" s="66" t="s">
+        <v>95</v>
+      </c>
+      <c r="H34" s="67"/>
       <c r="I34" s="22"/>
       <c r="J34" s="22"/>
       <c r="K34" s="22"/>
-      <c r="L34" s="25"/>
+      <c r="L34" s="24"/>
     </row>
     <row r="35" spans="1:56" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="84"/>
-      <c r="B35" s="84"/>
+      <c r="A35" s="22"/>
+      <c r="B35" s="22"/>
       <c r="C35" s="22"/>
       <c r="D35" s="22"/>
-      <c r="E35" s="30"/>
+      <c r="E35" s="29"/>
       <c r="F35" s="5"/>
-      <c r="G35" s="73" t="s">
-        <v>98</v>
-      </c>
-      <c r="H35" s="74"/>
+      <c r="G35" s="66" t="s">
+        <v>96</v>
+      </c>
+      <c r="H35" s="67"/>
       <c r="I35" s="22"/>
       <c r="J35" s="22"/>
       <c r="K35" s="22"/>
-      <c r="L35" s="25"/>
+      <c r="L35" s="24"/>
     </row>
     <row r="36" spans="1:56" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="84"/>
-      <c r="B36" s="84"/>
+      <c r="A36" s="22"/>
+      <c r="B36" s="22"/>
       <c r="C36" s="22"/>
       <c r="D36" s="22"/>
-      <c r="E36" s="30"/>
+      <c r="E36" s="29"/>
       <c r="F36" s="5"/>
-      <c r="G36" s="73" t="s">
-        <v>99</v>
-      </c>
-      <c r="H36" s="74"/>
+      <c r="G36" s="66" t="s">
+        <v>97</v>
+      </c>
+      <c r="H36" s="67"/>
       <c r="I36" s="22"/>
       <c r="J36" s="22"/>
       <c r="K36" s="22"/>
-      <c r="L36" s="25"/>
+      <c r="L36" s="24"/>
     </row>
     <row r="37" spans="1:56" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="84"/>
-      <c r="B37" s="84"/>
+      <c r="A37" s="22"/>
+      <c r="B37" s="22"/>
       <c r="C37" s="22"/>
       <c r="D37" s="22"/>
-      <c r="E37" s="30"/>
+      <c r="E37" s="29"/>
       <c r="F37" s="5"/>
-      <c r="G37" s="73" t="s">
-        <v>100</v>
-      </c>
-      <c r="H37" s="74"/>
+      <c r="G37" s="66" t="s">
+        <v>98</v>
+      </c>
+      <c r="H37" s="67"/>
       <c r="I37" s="22"/>
       <c r="J37" s="22"/>
       <c r="K37" s="22"/>
-      <c r="L37" s="25"/>
+      <c r="L37" s="24"/>
       <c r="M37" s="4"/>
       <c r="N37" s="4"/>
       <c r="O37" s="4"/>
@@ -2914,20 +2970,20 @@
       <c r="AS37" s="4"/>
     </row>
     <row r="38" spans="1:56" s="6" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="84"/>
-      <c r="B38" s="84"/>
+      <c r="A38" s="22"/>
+      <c r="B38" s="22"/>
       <c r="C38" s="22"/>
       <c r="D38" s="22"/>
-      <c r="E38" s="30"/>
+      <c r="E38" s="29"/>
       <c r="F38" s="5"/>
-      <c r="G38" s="73" t="s">
-        <v>101</v>
-      </c>
-      <c r="H38" s="74"/>
+      <c r="G38" s="66" t="s">
+        <v>99</v>
+      </c>
+      <c r="H38" s="67"/>
       <c r="I38" s="22"/>
       <c r="J38" s="22"/>
       <c r="K38" s="22"/>
-      <c r="L38" s="25"/>
+      <c r="L38" s="24"/>
       <c r="M38" s="4"/>
       <c r="N38" s="4"/>
       <c r="O38" s="4"/>
@@ -2939,20 +2995,20 @@
       <c r="AS38" s="4"/>
     </row>
     <row r="39" spans="1:56" s="6" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="84"/>
-      <c r="B39" s="84"/>
+      <c r="A39" s="22"/>
+      <c r="B39" s="22"/>
       <c r="C39" s="22"/>
       <c r="D39" s="22"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="90" t="s">
-        <v>102</v>
-      </c>
-      <c r="H39" s="91"/>
-      <c r="I39" s="26"/>
-      <c r="J39" s="26"/>
-      <c r="K39" s="26"/>
-      <c r="L39" s="27"/>
+      <c r="E39" s="141"/>
+      <c r="F39" s="142"/>
+      <c r="G39" s="58" t="s">
+        <v>100</v>
+      </c>
+      <c r="H39" s="60"/>
+      <c r="I39" s="25"/>
+      <c r="J39" s="25"/>
+      <c r="K39" s="25"/>
+      <c r="L39" s="26"/>
       <c r="M39" s="4"/>
       <c r="N39" s="4"/>
       <c r="O39" s="4"/>
@@ -2968,12 +3024,14 @@
       <c r="AS39" s="4"/>
     </row>
     <row r="40" spans="1:56" s="6" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="73"/>
-      <c r="B40" s="74"/>
+      <c r="A40" s="22"/>
+      <c r="B40" s="22"/>
       <c r="C40" s="22"/>
       <c r="D40" s="22"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="5"/>
+      <c r="E40" s="141"/>
+      <c r="F40" s="143"/>
+      <c r="G40" s="132"/>
+      <c r="H40" s="132"/>
       <c r="M40" s="4"/>
       <c r="N40" s="4"/>
       <c r="O40" s="4"/>
@@ -2999,72 +3057,72 @@
       <c r="BD40" s="4"/>
     </row>
     <row r="41" spans="1:56" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="73"/>
-      <c r="B41" s="74"/>
+      <c r="A41" s="22"/>
+      <c r="B41" s="22"/>
       <c r="C41" s="22"/>
       <c r="D41" s="22"/>
-      <c r="E41" s="30"/>
+      <c r="E41" s="29"/>
       <c r="F41" s="5"/>
-      <c r="G41" s="53" t="s">
+      <c r="G41" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="H41" s="54"/>
-      <c r="I41" s="54"/>
-      <c r="J41" s="54"/>
-      <c r="K41" s="54"/>
-      <c r="L41" s="55"/>
+      <c r="H41" s="99"/>
+      <c r="I41" s="99"/>
+      <c r="J41" s="99"/>
+      <c r="K41" s="99"/>
+      <c r="L41" s="86"/>
     </row>
     <row r="42" spans="1:56" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="73"/>
-      <c r="B42" s="74"/>
+      <c r="A42" s="22"/>
+      <c r="B42" s="22"/>
       <c r="C42" s="22"/>
       <c r="D42" s="22"/>
-      <c r="E42" s="30"/>
+      <c r="E42" s="29"/>
       <c r="F42" s="5"/>
-      <c r="G42" s="56" t="s">
-        <v>47</v>
-      </c>
-      <c r="H42" s="57"/>
-      <c r="I42" s="50" t="s">
-        <v>43</v>
-      </c>
-      <c r="J42" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="K42" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="L42" s="47" t="s">
-        <v>115</v>
+      <c r="G42" s="114" t="s">
+        <v>45</v>
+      </c>
+      <c r="H42" s="115"/>
+      <c r="I42" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="J42" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="K42" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="L42" s="46" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:56" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="71"/>
-      <c r="B43" s="72"/>
-      <c r="C43" s="28"/>
-      <c r="D43" s="28"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22"/>
       <c r="E43" s="29"/>
       <c r="F43" s="5"/>
-      <c r="G43" s="92"/>
-      <c r="H43" s="93"/>
+      <c r="G43" s="72"/>
+      <c r="H43" s="73"/>
       <c r="I43" s="22"/>
       <c r="J43" s="22"/>
-      <c r="K43" s="28"/>
-      <c r="L43" s="40"/>
+      <c r="K43" s="27"/>
+      <c r="L43" s="39"/>
     </row>
     <row r="44" spans="1:56" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="90"/>
-      <c r="B44" s="91"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="31"/>
+      <c r="A44" s="135"/>
+      <c r="B44" s="25"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="25"/>
+      <c r="E44" s="30"/>
       <c r="F44" s="5"/>
-      <c r="G44" s="58"/>
-      <c r="H44" s="59"/>
+      <c r="G44" s="72"/>
+      <c r="H44" s="73"/>
       <c r="I44" s="22"/>
       <c r="J44" s="22"/>
-      <c r="K44" s="22"/>
-      <c r="L44" s="25"/>
+      <c r="K44" s="27"/>
+      <c r="L44" s="39"/>
     </row>
     <row r="45" spans="1:56" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="6"/>
@@ -3073,28 +3131,28 @@
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="5"/>
-      <c r="G45" s="58"/>
-      <c r="H45" s="59"/>
+      <c r="G45" s="72"/>
+      <c r="H45" s="73"/>
       <c r="I45" s="22"/>
       <c r="J45" s="22"/>
-      <c r="K45" s="22"/>
-      <c r="L45" s="25"/>
+      <c r="K45" s="27"/>
+      <c r="L45" s="39"/>
     </row>
     <row r="46" spans="1:56" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="94" t="s">
+      <c r="A46" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="B46" s="95"/>
-      <c r="C46" s="95"/>
-      <c r="D46" s="95"/>
-      <c r="E46" s="96"/>
+      <c r="B46" s="64"/>
+      <c r="C46" s="64"/>
+      <c r="D46" s="64"/>
+      <c r="E46" s="65"/>
       <c r="F46" s="3"/>
-      <c r="G46" s="58"/>
-      <c r="H46" s="59"/>
+      <c r="G46" s="72"/>
+      <c r="H46" s="73"/>
       <c r="I46" s="22"/>
       <c r="J46" s="22"/>
-      <c r="K46" s="22"/>
-      <c r="L46" s="25"/>
+      <c r="K46" s="27"/>
+      <c r="L46" s="39"/>
     </row>
     <row r="47" spans="1:56" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="7" t="s">
@@ -3104,545 +3162,545 @@
         <v>16</v>
       </c>
       <c r="C47" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="D47" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D47" s="10" t="s">
+      <c r="E47" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E47" s="9" t="s">
-        <v>19</v>
-      </c>
       <c r="F47" s="3"/>
-      <c r="G47" s="58"/>
-      <c r="H47" s="59"/>
+      <c r="G47" s="72"/>
+      <c r="H47" s="73"/>
       <c r="I47" s="22"/>
       <c r="J47" s="22"/>
-      <c r="K47" s="22"/>
-      <c r="L47" s="25"/>
+      <c r="K47" s="27"/>
+      <c r="L47" s="39"/>
     </row>
     <row r="48" spans="1:56" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="32" t="s">
+      <c r="A48" s="31" t="s">
         <v>9</v>
       </c>
       <c r="B48" s="22"/>
       <c r="C48" s="22"/>
       <c r="D48" s="22"/>
-      <c r="E48" s="30"/>
+      <c r="E48" s="29"/>
       <c r="F48" s="3"/>
-      <c r="G48" s="58"/>
-      <c r="H48" s="59"/>
+      <c r="G48" s="72"/>
+      <c r="H48" s="73"/>
       <c r="I48" s="22"/>
       <c r="J48" s="22"/>
-      <c r="K48" s="22"/>
-      <c r="L48" s="25"/>
+      <c r="K48" s="27"/>
+      <c r="L48" s="39"/>
     </row>
     <row r="49" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="32" t="s">
+      <c r="A49" s="31" t="s">
         <v>10</v>
       </c>
       <c r="B49" s="22"/>
       <c r="C49" s="22"/>
       <c r="D49" s="22"/>
-      <c r="E49" s="30"/>
+      <c r="E49" s="29"/>
       <c r="F49" s="3"/>
-      <c r="G49" s="58"/>
-      <c r="H49" s="59"/>
+      <c r="G49" s="72"/>
+      <c r="H49" s="73"/>
       <c r="I49" s="22"/>
       <c r="J49" s="22"/>
-      <c r="K49" s="22"/>
-      <c r="L49" s="25"/>
+      <c r="K49" s="27"/>
+      <c r="L49" s="39"/>
     </row>
     <row r="50" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="32" t="s">
+      <c r="A50" s="31" t="s">
         <v>11</v>
       </c>
       <c r="B50" s="22"/>
       <c r="C50" s="22"/>
       <c r="D50" s="22"/>
-      <c r="E50" s="30"/>
+      <c r="E50" s="29"/>
       <c r="F50" s="3"/>
-      <c r="G50" s="58"/>
-      <c r="H50" s="59"/>
+      <c r="G50" s="72"/>
+      <c r="H50" s="73"/>
       <c r="I50" s="22"/>
       <c r="J50" s="22"/>
-      <c r="K50" s="22"/>
-      <c r="L50" s="25"/>
+      <c r="K50" s="27"/>
+      <c r="L50" s="39"/>
     </row>
     <row r="51" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="32" t="s">
+      <c r="A51" s="31" t="s">
         <v>12</v>
       </c>
       <c r="B51" s="22"/>
       <c r="C51" s="22"/>
       <c r="D51" s="22"/>
-      <c r="E51" s="30"/>
+      <c r="E51" s="29"/>
       <c r="F51" s="3"/>
-      <c r="G51" s="58"/>
-      <c r="H51" s="59"/>
+      <c r="G51" s="72"/>
+      <c r="H51" s="73"/>
       <c r="I51" s="22"/>
       <c r="J51" s="22"/>
-      <c r="K51" s="22"/>
-      <c r="L51" s="25"/>
+      <c r="K51" s="27"/>
+      <c r="L51" s="39"/>
     </row>
     <row r="52" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="32" t="s">
+      <c r="A52" s="31" t="s">
         <v>13</v>
       </c>
       <c r="B52" s="22"/>
       <c r="C52" s="22"/>
       <c r="D52" s="22"/>
-      <c r="E52" s="30"/>
+      <c r="E52" s="29"/>
       <c r="F52" s="3"/>
-      <c r="G52" s="58"/>
-      <c r="H52" s="59"/>
+      <c r="G52" s="72"/>
+      <c r="H52" s="73"/>
       <c r="I52" s="22"/>
       <c r="J52" s="22"/>
-      <c r="K52" s="22"/>
-      <c r="L52" s="25"/>
+      <c r="K52" s="27"/>
+      <c r="L52" s="39"/>
     </row>
     <row r="53" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="87" t="s">
+      <c r="A53" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="B53" s="88"/>
-      <c r="C53" s="89"/>
+      <c r="B53" s="79"/>
+      <c r="C53" s="80"/>
       <c r="D53" s="7"/>
       <c r="E53" s="13"/>
       <c r="F53" s="3"/>
-      <c r="G53" s="85"/>
-      <c r="H53" s="86"/>
+      <c r="G53" s="72"/>
+      <c r="H53" s="73"/>
       <c r="I53" s="22"/>
       <c r="J53" s="22"/>
-      <c r="K53" s="22"/>
-      <c r="L53" s="25"/>
+      <c r="K53" s="27"/>
+      <c r="L53" s="39"/>
     </row>
     <row r="54" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="42" t="s">
-        <v>78</v>
-      </c>
-      <c r="B54" s="97" t="s">
-        <v>20</v>
-      </c>
-      <c r="C54" s="98"/>
-      <c r="D54" s="99" t="s">
-        <v>106</v>
-      </c>
-      <c r="E54" s="100"/>
+      <c r="A54" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="B54" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="C54" s="110"/>
+      <c r="D54" s="111" t="s">
+        <v>104</v>
+      </c>
+      <c r="E54" s="112"/>
       <c r="F54" s="3"/>
-      <c r="G54" s="58"/>
-      <c r="H54" s="59"/>
+      <c r="G54" s="72"/>
+      <c r="H54" s="73"/>
       <c r="I54" s="22"/>
       <c r="J54" s="22"/>
-      <c r="K54" s="22"/>
-      <c r="L54" s="25"/>
+      <c r="K54" s="27"/>
+      <c r="L54" s="39"/>
     </row>
     <row r="55" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="43"/>
-      <c r="B55" s="101"/>
-      <c r="C55" s="102"/>
-      <c r="D55" s="101"/>
-      <c r="E55" s="103"/>
+      <c r="A55" s="42"/>
+      <c r="B55" s="69"/>
+      <c r="C55" s="71"/>
+      <c r="D55" s="69"/>
+      <c r="E55" s="70"/>
       <c r="F55" s="3"/>
-      <c r="G55" s="58"/>
-      <c r="H55" s="59"/>
+      <c r="G55" s="72"/>
+      <c r="H55" s="73"/>
       <c r="I55" s="22"/>
       <c r="J55" s="22"/>
-      <c r="K55" s="22"/>
-      <c r="L55" s="25"/>
+      <c r="K55" s="27"/>
+      <c r="L55" s="39"/>
     </row>
     <row r="56" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F56" s="3"/>
-      <c r="G56" s="85"/>
-      <c r="H56" s="86"/>
+      <c r="G56" s="72"/>
+      <c r="H56" s="73"/>
       <c r="I56" s="22"/>
       <c r="J56" s="22"/>
-      <c r="K56" s="22"/>
-      <c r="L56" s="25"/>
+      <c r="K56" s="27"/>
+      <c r="L56" s="39"/>
     </row>
     <row r="57" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A57" s="94" t="s">
-        <v>116</v>
-      </c>
-      <c r="B57" s="95"/>
-      <c r="C57" s="95"/>
-      <c r="D57" s="95"/>
-      <c r="E57" s="96"/>
+      <c r="A57" s="63" t="s">
+        <v>114</v>
+      </c>
+      <c r="B57" s="64"/>
+      <c r="C57" s="64"/>
+      <c r="D57" s="64"/>
+      <c r="E57" s="65"/>
       <c r="F57" s="3"/>
-      <c r="G57" s="58"/>
-      <c r="H57" s="59"/>
+      <c r="G57" s="72"/>
+      <c r="H57" s="73"/>
       <c r="I57" s="22"/>
       <c r="J57" s="22"/>
-      <c r="K57" s="22"/>
-      <c r="L57" s="25"/>
+      <c r="K57" s="27"/>
+      <c r="L57" s="39"/>
     </row>
     <row r="58" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="44" t="s">
+      <c r="A58" s="43" t="s">
         <v>15</v>
       </c>
       <c r="B58" s="11" t="s">
         <v>16</v>
       </c>
       <c r="C58" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="D58" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D58" s="8" t="s">
+      <c r="E58" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="12" t="s">
-        <v>19</v>
-      </c>
       <c r="F58" s="3"/>
-      <c r="G58" s="58"/>
-      <c r="H58" s="59"/>
+      <c r="G58" s="72"/>
+      <c r="H58" s="73"/>
       <c r="I58" s="22"/>
       <c r="J58" s="22"/>
-      <c r="K58" s="22"/>
-      <c r="L58" s="25"/>
+      <c r="K58" s="27"/>
+      <c r="L58" s="39"/>
     </row>
     <row r="59" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="32" t="s">
+      <c r="A59" s="31" t="s">
         <v>9</v>
       </c>
       <c r="B59" s="22"/>
       <c r="C59" s="22"/>
       <c r="D59" s="22"/>
-      <c r="E59" s="30"/>
+      <c r="E59" s="29"/>
       <c r="F59" s="3"/>
-      <c r="G59" s="58"/>
-      <c r="H59" s="59"/>
+      <c r="G59" s="72"/>
+      <c r="H59" s="73"/>
       <c r="I59" s="22"/>
       <c r="J59" s="22"/>
-      <c r="K59" s="22"/>
-      <c r="L59" s="25"/>
+      <c r="K59" s="27"/>
+      <c r="L59" s="39"/>
     </row>
     <row r="60" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="32" t="s">
+      <c r="A60" s="31" t="s">
         <v>10</v>
       </c>
       <c r="B60" s="22"/>
       <c r="C60" s="22"/>
       <c r="D60" s="22"/>
-      <c r="E60" s="30"/>
+      <c r="E60" s="29"/>
       <c r="F60" s="3"/>
-      <c r="G60" s="58"/>
-      <c r="H60" s="59"/>
+      <c r="G60" s="72"/>
+      <c r="H60" s="73"/>
       <c r="I60" s="22"/>
       <c r="J60" s="22"/>
-      <c r="K60" s="22"/>
-      <c r="L60" s="25"/>
+      <c r="K60" s="27"/>
+      <c r="L60" s="39"/>
     </row>
     <row r="61" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="32" t="s">
+      <c r="A61" s="31" t="s">
         <v>11</v>
       </c>
       <c r="B61" s="22"/>
       <c r="C61" s="22"/>
       <c r="D61" s="22"/>
-      <c r="E61" s="30"/>
+      <c r="E61" s="29"/>
       <c r="F61" s="3"/>
-      <c r="G61" s="58"/>
-      <c r="H61" s="59"/>
+      <c r="G61" s="72"/>
+      <c r="H61" s="73"/>
       <c r="I61" s="22"/>
       <c r="J61" s="22"/>
-      <c r="K61" s="22"/>
-      <c r="L61" s="25"/>
+      <c r="K61" s="27"/>
+      <c r="L61" s="39"/>
     </row>
     <row r="62" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="32" t="s">
+      <c r="A62" s="31" t="s">
         <v>12</v>
       </c>
       <c r="B62" s="22"/>
       <c r="C62" s="22"/>
       <c r="D62" s="22"/>
-      <c r="E62" s="30"/>
+      <c r="E62" s="29"/>
       <c r="F62" s="3"/>
-      <c r="G62" s="58"/>
-      <c r="H62" s="59"/>
+      <c r="G62" s="72"/>
+      <c r="H62" s="73"/>
       <c r="I62" s="22"/>
       <c r="J62" s="22"/>
-      <c r="K62" s="22"/>
-      <c r="L62" s="25"/>
+      <c r="K62" s="27"/>
+      <c r="L62" s="39"/>
     </row>
     <row r="63" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="32" t="s">
+      <c r="A63" s="31" t="s">
         <v>13</v>
       </c>
       <c r="B63" s="22"/>
       <c r="C63" s="22"/>
       <c r="D63" s="22"/>
-      <c r="E63" s="30"/>
+      <c r="E63" s="29"/>
       <c r="F63" s="3"/>
-      <c r="G63" s="58"/>
-      <c r="H63" s="59"/>
+      <c r="G63" s="72"/>
+      <c r="H63" s="73"/>
       <c r="I63" s="22"/>
       <c r="J63" s="22"/>
-      <c r="K63" s="22"/>
-      <c r="L63" s="25"/>
+      <c r="K63" s="27"/>
+      <c r="L63" s="39"/>
     </row>
     <row r="64" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="87" t="s">
+      <c r="A64" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="B64" s="88"/>
-      <c r="C64" s="89"/>
+      <c r="B64" s="79"/>
+      <c r="C64" s="80"/>
       <c r="D64" s="7"/>
       <c r="E64" s="13"/>
       <c r="F64" s="3"/>
-      <c r="G64" s="58"/>
-      <c r="H64" s="59"/>
+      <c r="G64" s="72"/>
+      <c r="H64" s="73"/>
       <c r="I64" s="22"/>
       <c r="J64" s="22"/>
-      <c r="K64" s="22"/>
-      <c r="L64" s="25"/>
+      <c r="K64" s="27"/>
+      <c r="L64" s="39"/>
     </row>
     <row r="65" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="42" t="s">
-        <v>78</v>
-      </c>
-      <c r="B65" s="97" t="s">
-        <v>20</v>
-      </c>
-      <c r="C65" s="98"/>
-      <c r="D65" s="99" t="s">
-        <v>106</v>
-      </c>
-      <c r="E65" s="100"/>
+      <c r="A65" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="B65" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="C65" s="110"/>
+      <c r="D65" s="111" t="s">
+        <v>104</v>
+      </c>
+      <c r="E65" s="112"/>
       <c r="F65" s="3"/>
-      <c r="G65" s="58"/>
-      <c r="H65" s="59"/>
+      <c r="G65" s="72"/>
+      <c r="H65" s="73"/>
       <c r="I65" s="22"/>
       <c r="J65" s="22"/>
-      <c r="K65" s="22"/>
-      <c r="L65" s="25"/>
+      <c r="K65" s="27"/>
+      <c r="L65" s="39"/>
     </row>
     <row r="66" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="43"/>
-      <c r="B66" s="101"/>
-      <c r="C66" s="102"/>
-      <c r="D66" s="101"/>
-      <c r="E66" s="103"/>
+      <c r="A66" s="42"/>
+      <c r="B66" s="69"/>
+      <c r="C66" s="71"/>
+      <c r="D66" s="69"/>
+      <c r="E66" s="70"/>
       <c r="F66" s="3"/>
-      <c r="G66" s="58"/>
-      <c r="H66" s="59"/>
+      <c r="G66" s="72"/>
+      <c r="H66" s="73"/>
       <c r="I66" s="22"/>
       <c r="J66" s="22"/>
-      <c r="K66" s="22"/>
-      <c r="L66" s="25"/>
+      <c r="K66" s="27"/>
+      <c r="L66" s="39"/>
     </row>
     <row r="67" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F67" s="3"/>
-      <c r="G67" s="58"/>
-      <c r="H67" s="59"/>
+      <c r="G67" s="72"/>
+      <c r="H67" s="73"/>
       <c r="I67" s="22"/>
       <c r="J67" s="22"/>
-      <c r="K67" s="22"/>
-      <c r="L67" s="25"/>
+      <c r="K67" s="27"/>
+      <c r="L67" s="39"/>
     </row>
     <row r="68" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A68" s="104" t="s">
+      <c r="A68" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="B68" s="105"/>
-      <c r="C68" s="105"/>
-      <c r="D68" s="105"/>
-      <c r="E68" s="106"/>
+      <c r="B68" s="83"/>
+      <c r="C68" s="83"/>
+      <c r="D68" s="83"/>
+      <c r="E68" s="84"/>
       <c r="F68" s="3"/>
-      <c r="G68" s="58"/>
-      <c r="H68" s="59"/>
+      <c r="G68" s="72"/>
+      <c r="H68" s="73"/>
       <c r="I68" s="22"/>
       <c r="J68" s="22"/>
-      <c r="K68" s="22"/>
-      <c r="L68" s="25"/>
+      <c r="K68" s="27"/>
+      <c r="L68" s="39"/>
     </row>
     <row r="69" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="56" t="s">
-        <v>35</v>
-      </c>
-      <c r="B69" s="57"/>
-      <c r="C69" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="D69" s="46" t="s">
-        <v>107</v>
-      </c>
-      <c r="E69" s="45" t="s">
-        <v>44</v>
+      <c r="A69" s="114" t="s">
+        <v>34</v>
+      </c>
+      <c r="B69" s="115"/>
+      <c r="C69" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="D69" s="45" t="s">
+        <v>105</v>
+      </c>
+      <c r="E69" s="44" t="s">
+        <v>42</v>
       </c>
       <c r="F69" s="3"/>
-      <c r="G69" s="58"/>
-      <c r="H69" s="59"/>
+      <c r="G69" s="72"/>
+      <c r="H69" s="73"/>
       <c r="I69" s="22"/>
       <c r="J69" s="22"/>
-      <c r="K69" s="22"/>
-      <c r="L69" s="25"/>
+      <c r="K69" s="27"/>
+      <c r="L69" s="39"/>
     </row>
     <row r="70" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="108"/>
-      <c r="B70" s="109"/>
-      <c r="C70" s="28"/>
+      <c r="A70" s="105"/>
+      <c r="B70" s="106"/>
+      <c r="C70" s="27"/>
       <c r="D70" s="22"/>
-      <c r="E70" s="30"/>
+      <c r="E70" s="29"/>
       <c r="F70" s="3"/>
-      <c r="G70" s="58"/>
-      <c r="H70" s="59"/>
+      <c r="G70" s="72"/>
+      <c r="H70" s="73"/>
       <c r="I70" s="22"/>
       <c r="J70" s="22"/>
-      <c r="K70" s="22"/>
-      <c r="L70" s="25"/>
+      <c r="K70" s="27"/>
+      <c r="L70" s="39"/>
     </row>
     <row r="71" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="83"/>
-      <c r="B71" s="84"/>
+      <c r="A71" s="56"/>
+      <c r="B71" s="57"/>
       <c r="C71" s="22"/>
       <c r="D71" s="22"/>
-      <c r="E71" s="30"/>
+      <c r="E71" s="29"/>
       <c r="F71" s="3"/>
-      <c r="G71" s="58"/>
-      <c r="H71" s="59"/>
+      <c r="G71" s="72"/>
+      <c r="H71" s="73"/>
       <c r="I71" s="22"/>
       <c r="J71" s="22"/>
-      <c r="K71" s="22"/>
-      <c r="L71" s="25"/>
+      <c r="K71" s="27"/>
+      <c r="L71" s="39"/>
     </row>
     <row r="72" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="117"/>
-      <c r="B72" s="118"/>
-      <c r="C72" s="33"/>
-      <c r="D72" s="33"/>
-      <c r="E72" s="34"/>
+      <c r="A72" s="107"/>
+      <c r="B72" s="108"/>
+      <c r="C72" s="32"/>
+      <c r="D72" s="32"/>
+      <c r="E72" s="33"/>
       <c r="F72" s="3"/>
-      <c r="G72" s="58"/>
-      <c r="H72" s="59"/>
+      <c r="G72" s="72"/>
+      <c r="H72" s="73"/>
       <c r="I72" s="22"/>
       <c r="J72" s="22"/>
-      <c r="K72" s="22"/>
-      <c r="L72" s="25"/>
+      <c r="K72" s="27"/>
+      <c r="L72" s="39"/>
     </row>
     <row r="73" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="87" t="s">
-        <v>108</v>
-      </c>
-      <c r="B73" s="88"/>
-      <c r="C73" s="88"/>
-      <c r="D73" s="110"/>
+      <c r="A73" s="78" t="s">
+        <v>106</v>
+      </c>
+      <c r="B73" s="79"/>
+      <c r="C73" s="79"/>
+      <c r="D73" s="81"/>
       <c r="E73" s="14"/>
       <c r="F73" s="3"/>
-      <c r="G73" s="58"/>
-      <c r="H73" s="59"/>
+      <c r="G73" s="72"/>
+      <c r="H73" s="73"/>
       <c r="I73" s="22"/>
       <c r="J73" s="22"/>
-      <c r="K73" s="22"/>
-      <c r="L73" s="25"/>
+      <c r="K73" s="27"/>
+      <c r="L73" s="39"/>
     </row>
     <row r="74" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F74" s="3"/>
-      <c r="G74" s="58"/>
-      <c r="H74" s="59"/>
+      <c r="G74" s="72"/>
+      <c r="H74" s="73"/>
       <c r="I74" s="22"/>
       <c r="J74" s="22"/>
-      <c r="K74" s="22"/>
-      <c r="L74" s="25"/>
+      <c r="K74" s="27"/>
+      <c r="L74" s="39"/>
     </row>
     <row r="75" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A75" s="53" t="s">
-        <v>80</v>
-      </c>
-      <c r="B75" s="54"/>
-      <c r="C75" s="54"/>
-      <c r="D75" s="54"/>
-      <c r="E75" s="55"/>
+      <c r="A75" s="85" t="s">
+        <v>78</v>
+      </c>
+      <c r="B75" s="99"/>
+      <c r="C75" s="99"/>
+      <c r="D75" s="99"/>
+      <c r="E75" s="86"/>
       <c r="F75" s="3"/>
-      <c r="G75" s="58"/>
-      <c r="H75" s="59"/>
-      <c r="I75" s="22"/>
-      <c r="J75" s="22"/>
-      <c r="K75" s="22"/>
-      <c r="L75" s="25"/>
+      <c r="G75" s="76"/>
+      <c r="H75" s="77"/>
+      <c r="I75" s="25"/>
+      <c r="J75" s="25"/>
+      <c r="K75" s="25"/>
+      <c r="L75" s="26"/>
     </row>
     <row r="76" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="73" t="s">
+      <c r="A76" s="66" t="s">
+        <v>48</v>
+      </c>
+      <c r="B76" s="68"/>
+      <c r="C76" s="68"/>
+      <c r="D76" s="67"/>
+      <c r="E76" s="34"/>
+      <c r="F76" s="3"/>
+    </row>
+    <row r="77" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A77" s="66" t="s">
+        <v>49</v>
+      </c>
+      <c r="B77" s="68"/>
+      <c r="C77" s="68"/>
+      <c r="D77" s="67"/>
+      <c r="E77" s="34"/>
+      <c r="F77" s="3"/>
+      <c r="G77" s="85" t="s">
+        <v>8</v>
+      </c>
+      <c r="H77" s="99"/>
+      <c r="I77" s="99"/>
+      <c r="J77" s="99"/>
+      <c r="K77" s="99"/>
+      <c r="L77" s="86"/>
+    </row>
+    <row r="78" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="B76" s="111"/>
-      <c r="C76" s="111"/>
-      <c r="D76" s="74"/>
-      <c r="E76" s="35"/>
-      <c r="F76" s="3"/>
-    </row>
-    <row r="77" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A77" s="73" t="s">
+      <c r="B78" s="68"/>
+      <c r="C78" s="68"/>
+      <c r="D78" s="67"/>
+      <c r="E78" s="34"/>
+      <c r="F78" s="3"/>
+      <c r="G78" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="H78" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="I78" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="J78" s="49" t="s">
+        <v>108</v>
+      </c>
+      <c r="K78" s="49" t="s">
+        <v>47</v>
+      </c>
+      <c r="L78" s="46" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="B77" s="111"/>
-      <c r="C77" s="111"/>
-      <c r="D77" s="74"/>
-      <c r="E77" s="35"/>
-      <c r="F77" s="3"/>
-      <c r="G77" s="53" t="s">
-        <v>8</v>
-      </c>
-      <c r="H77" s="54"/>
-      <c r="I77" s="54"/>
-      <c r="J77" s="54"/>
-      <c r="K77" s="54"/>
-      <c r="L77" s="55"/>
-    </row>
-    <row r="78" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="73" t="s">
-        <v>52</v>
-      </c>
-      <c r="B78" s="111"/>
-      <c r="C78" s="111"/>
-      <c r="D78" s="74"/>
-      <c r="E78" s="35"/>
-      <c r="F78" s="3"/>
-      <c r="G78" s="49" t="s">
-        <v>40</v>
-      </c>
-      <c r="H78" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="I78" s="48" t="s">
-        <v>3</v>
-      </c>
-      <c r="J78" s="50" t="s">
-        <v>110</v>
-      </c>
-      <c r="K78" s="50" t="s">
-        <v>49</v>
-      </c>
-      <c r="L78" s="47" t="s">
+      <c r="B79" s="68"/>
+      <c r="C79" s="68"/>
+      <c r="D79" s="67"/>
+      <c r="E79" s="34"/>
+      <c r="F79" s="3"/>
+      <c r="G79" s="37" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="79" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="73" t="s">
-        <v>53</v>
-      </c>
-      <c r="B79" s="111"/>
-      <c r="C79" s="111"/>
-      <c r="D79" s="74"/>
-      <c r="E79" s="35"/>
-      <c r="F79" s="3"/>
-      <c r="G79" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="H79" s="28"/>
+      <c r="H79" s="27"/>
       <c r="I79" s="22"/>
       <c r="J79" s="22"/>
       <c r="K79" s="22"/>
-      <c r="L79" s="28"/>
+      <c r="L79" s="27"/>
     </row>
     <row r="80" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="90" t="s">
-        <v>54</v>
-      </c>
-      <c r="B80" s="121"/>
-      <c r="C80" s="121"/>
-      <c r="D80" s="91"/>
-      <c r="E80" s="36"/>
+      <c r="A80" s="58" t="s">
+        <v>52</v>
+      </c>
+      <c r="B80" s="59"/>
+      <c r="C80" s="59"/>
+      <c r="D80" s="60"/>
+      <c r="E80" s="35"/>
       <c r="F80" s="3"/>
-      <c r="G80" s="39" t="s">
+      <c r="G80" s="38" t="s">
         <v>1</v>
       </c>
       <c r="H80" s="22"/>
@@ -3653,8 +3711,8 @@
     </row>
     <row r="81" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F81" s="3"/>
-      <c r="G81" s="38" t="s">
-        <v>42</v>
+      <c r="G81" s="37" t="s">
+        <v>40</v>
       </c>
       <c r="H81" s="22"/>
       <c r="I81" s="22"/>
@@ -3663,16 +3721,16 @@
       <c r="L81" s="22"/>
     </row>
     <row r="82" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A82" s="104" t="s">
+      <c r="A82" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="B82" s="105"/>
-      <c r="C82" s="105"/>
-      <c r="D82" s="105"/>
-      <c r="E82" s="106"/>
+      <c r="B82" s="83"/>
+      <c r="C82" s="83"/>
+      <c r="D82" s="83"/>
+      <c r="E82" s="84"/>
       <c r="F82" s="3"/>
-      <c r="G82" s="39" t="s">
-        <v>111</v>
+      <c r="G82" s="38" t="s">
+        <v>109</v>
       </c>
       <c r="H82" s="22"/>
       <c r="I82" s="22"/>
@@ -3681,22 +3739,22 @@
       <c r="L82" s="22"/>
     </row>
     <row r="83" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="107" t="s">
-        <v>35</v>
-      </c>
-      <c r="B83" s="99"/>
-      <c r="C83" s="41" t="s">
+      <c r="A83" s="113" t="s">
         <v>34</v>
       </c>
-      <c r="D83" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="E83" s="47" t="s">
-        <v>37</v>
+      <c r="B83" s="111"/>
+      <c r="C83" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="D83" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="E83" s="46" t="s">
+        <v>36</v>
       </c>
       <c r="F83" s="3"/>
       <c r="G83" s="15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H83" s="16"/>
       <c r="I83" s="16"/>
@@ -3705,425 +3763,425 @@
       <c r="L83" s="17"/>
     </row>
     <row r="84" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="73"/>
-      <c r="B84" s="74"/>
-      <c r="C84" s="28"/>
+      <c r="A84" s="66"/>
+      <c r="B84" s="67"/>
+      <c r="C84" s="27"/>
       <c r="D84" s="22"/>
-      <c r="E84" s="29"/>
+      <c r="E84" s="28"/>
       <c r="F84" s="3"/>
       <c r="G84" s="18" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H84" s="19"/>
-      <c r="I84" s="52"/>
+      <c r="I84" s="51"/>
       <c r="J84" s="20"/>
       <c r="K84" s="20"/>
       <c r="L84" s="20"/>
     </row>
     <row r="85" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="73"/>
-      <c r="B85" s="74"/>
+      <c r="A85" s="66"/>
+      <c r="B85" s="67"/>
       <c r="C85" s="22"/>
       <c r="D85" s="22"/>
-      <c r="E85" s="30"/>
+      <c r="E85" s="29"/>
       <c r="F85" s="3"/>
     </row>
     <row r="86" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A86" s="73"/>
-      <c r="B86" s="74"/>
+      <c r="A86" s="66"/>
+      <c r="B86" s="67"/>
       <c r="C86" s="22"/>
       <c r="D86" s="22"/>
-      <c r="E86" s="30"/>
+      <c r="E86" s="29"/>
       <c r="F86" s="3"/>
-      <c r="G86" s="53" t="s">
-        <v>128</v>
-      </c>
-      <c r="H86" s="55"/>
+      <c r="G86" s="85" t="s">
+        <v>126</v>
+      </c>
+      <c r="H86" s="86"/>
     </row>
     <row r="87" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="73"/>
-      <c r="B87" s="74"/>
+      <c r="A87" s="66"/>
+      <c r="B87" s="67"/>
       <c r="C87" s="22"/>
       <c r="D87" s="22"/>
-      <c r="E87" s="30"/>
+      <c r="E87" s="29"/>
       <c r="F87" s="3"/>
       <c r="G87" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H87" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="88" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="73"/>
-      <c r="B88" s="74"/>
+      <c r="A88" s="66"/>
+      <c r="B88" s="67"/>
       <c r="C88" s="22"/>
       <c r="D88" s="22"/>
-      <c r="E88" s="30"/>
+      <c r="E88" s="29"/>
       <c r="F88" s="3"/>
-      <c r="G88" s="37" t="s">
-        <v>117</v>
-      </c>
-      <c r="H88" s="37"/>
+      <c r="G88" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="H88" s="36"/>
     </row>
     <row r="89" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="73"/>
-      <c r="B89" s="74"/>
+      <c r="A89" s="66"/>
+      <c r="B89" s="67"/>
       <c r="C89" s="22"/>
       <c r="D89" s="22"/>
-      <c r="E89" s="30"/>
+      <c r="E89" s="29"/>
       <c r="F89" s="3"/>
-      <c r="G89" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="H89" s="37"/>
+      <c r="G89" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="H89" s="36"/>
     </row>
     <row r="90" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="73"/>
-      <c r="B90" s="74"/>
+      <c r="A90" s="66"/>
+      <c r="B90" s="67"/>
       <c r="C90" s="22"/>
       <c r="D90" s="22"/>
-      <c r="E90" s="30"/>
+      <c r="E90" s="29"/>
       <c r="F90" s="3"/>
-      <c r="G90" s="37" t="s">
-        <v>119</v>
-      </c>
-      <c r="H90" s="37"/>
+      <c r="G90" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="H90" s="36"/>
     </row>
     <row r="91" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="73"/>
-      <c r="B91" s="74"/>
+      <c r="A91" s="66"/>
+      <c r="B91" s="67"/>
       <c r="C91" s="22"/>
       <c r="D91" s="22"/>
-      <c r="E91" s="30"/>
+      <c r="E91" s="29"/>
       <c r="F91" s="3"/>
-      <c r="G91" s="37" t="s">
-        <v>120</v>
-      </c>
-      <c r="H91" s="37"/>
+      <c r="G91" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="H91" s="36"/>
     </row>
     <row r="92" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="73"/>
-      <c r="B92" s="74"/>
+      <c r="A92" s="66"/>
+      <c r="B92" s="67"/>
       <c r="C92" s="22"/>
       <c r="D92" s="22"/>
-      <c r="E92" s="30"/>
+      <c r="E92" s="29"/>
       <c r="F92" s="3"/>
-      <c r="G92" s="37" t="s">
-        <v>121</v>
-      </c>
-      <c r="H92" s="37"/>
+      <c r="G92" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="H92" s="36"/>
     </row>
     <row r="93" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="73"/>
-      <c r="B93" s="74"/>
+      <c r="A93" s="66"/>
+      <c r="B93" s="67"/>
       <c r="C93" s="22"/>
       <c r="D93" s="22"/>
-      <c r="E93" s="30"/>
+      <c r="E93" s="29"/>
       <c r="F93" s="3"/>
-      <c r="G93" s="37" t="s">
-        <v>122</v>
-      </c>
-      <c r="H93" s="37"/>
+      <c r="G93" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="H93" s="36"/>
     </row>
     <row r="94" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="73"/>
-      <c r="B94" s="74"/>
+      <c r="A94" s="66"/>
+      <c r="B94" s="67"/>
       <c r="C94" s="22"/>
       <c r="D94" s="22"/>
-      <c r="E94" s="30"/>
+      <c r="E94" s="29"/>
       <c r="F94" s="3"/>
-      <c r="G94" s="37" t="s">
-        <v>123</v>
-      </c>
-      <c r="H94" s="37"/>
+      <c r="G94" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="H94" s="36"/>
     </row>
     <row r="95" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="73"/>
-      <c r="B95" s="74"/>
+      <c r="A95" s="66"/>
+      <c r="B95" s="67"/>
       <c r="C95" s="22"/>
       <c r="D95" s="22"/>
-      <c r="E95" s="30"/>
+      <c r="E95" s="29"/>
       <c r="F95" s="3"/>
-      <c r="G95" s="37" t="s">
-        <v>124</v>
-      </c>
-      <c r="H95" s="37"/>
+      <c r="G95" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="H95" s="36"/>
     </row>
     <row r="96" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="73"/>
-      <c r="B96" s="74"/>
+      <c r="A96" s="66"/>
+      <c r="B96" s="67"/>
       <c r="C96" s="22"/>
       <c r="D96" s="22"/>
-      <c r="E96" s="30"/>
+      <c r="E96" s="29"/>
       <c r="F96" s="3"/>
-      <c r="G96" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="H96" s="37"/>
+      <c r="G96" s="36" t="s">
+        <v>123</v>
+      </c>
+      <c r="H96" s="36"/>
     </row>
     <row r="97" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="73"/>
-      <c r="B97" s="74"/>
+      <c r="A97" s="66"/>
+      <c r="B97" s="67"/>
       <c r="C97" s="22"/>
       <c r="D97" s="22"/>
-      <c r="E97" s="30"/>
+      <c r="E97" s="29"/>
       <c r="F97" s="3"/>
     </row>
     <row r="98" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="73"/>
-      <c r="B98" s="74"/>
+      <c r="A98" s="66"/>
+      <c r="B98" s="67"/>
       <c r="C98" s="22"/>
       <c r="D98" s="22"/>
-      <c r="E98" s="30"/>
+      <c r="E98" s="29"/>
       <c r="F98" s="3"/>
-      <c r="G98" s="123" t="s">
-        <v>129</v>
-      </c>
-      <c r="H98" s="124"/>
-      <c r="I98" s="124"/>
-      <c r="J98" s="124"/>
-      <c r="K98" s="124"/>
-      <c r="L98" s="125"/>
+      <c r="G98" s="96" t="s">
+        <v>127</v>
+      </c>
+      <c r="H98" s="97"/>
+      <c r="I98" s="97"/>
+      <c r="J98" s="97"/>
+      <c r="K98" s="97"/>
+      <c r="L98" s="98"/>
     </row>
     <row r="99" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="73"/>
-      <c r="B99" s="74"/>
+      <c r="A99" s="66"/>
+      <c r="B99" s="67"/>
       <c r="C99" s="22"/>
       <c r="D99" s="22"/>
-      <c r="E99" s="30"/>
+      <c r="E99" s="29"/>
       <c r="F99" s="3"/>
-      <c r="G99" s="126"/>
-      <c r="H99" s="127"/>
-      <c r="I99" s="127"/>
-      <c r="J99" s="127"/>
-      <c r="K99" s="127"/>
-      <c r="L99" s="128"/>
+      <c r="G99" s="87"/>
+      <c r="H99" s="88"/>
+      <c r="I99" s="88"/>
+      <c r="J99" s="88"/>
+      <c r="K99" s="88"/>
+      <c r="L99" s="89"/>
     </row>
     <row r="100" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="73"/>
-      <c r="B100" s="74"/>
+      <c r="A100" s="66"/>
+      <c r="B100" s="67"/>
       <c r="C100" s="22"/>
       <c r="D100" s="22"/>
-      <c r="E100" s="30"/>
+      <c r="E100" s="29"/>
       <c r="F100" s="3"/>
-      <c r="G100" s="129"/>
-      <c r="H100" s="130"/>
-      <c r="I100" s="130"/>
-      <c r="J100" s="130"/>
-      <c r="K100" s="130"/>
-      <c r="L100" s="131"/>
+      <c r="G100" s="90"/>
+      <c r="H100" s="91"/>
+      <c r="I100" s="91"/>
+      <c r="J100" s="91"/>
+      <c r="K100" s="91"/>
+      <c r="L100" s="92"/>
     </row>
     <row r="101" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="119"/>
-      <c r="B101" s="120"/>
+      <c r="A101" s="74"/>
+      <c r="B101" s="75"/>
       <c r="C101" s="22"/>
       <c r="D101" s="22"/>
-      <c r="E101" s="30"/>
+      <c r="E101" s="29"/>
       <c r="F101" s="3"/>
-      <c r="G101" s="129"/>
-      <c r="H101" s="130"/>
-      <c r="I101" s="130"/>
-      <c r="J101" s="130"/>
-      <c r="K101" s="130"/>
-      <c r="L101" s="131"/>
+      <c r="G101" s="90"/>
+      <c r="H101" s="91"/>
+      <c r="I101" s="91"/>
+      <c r="J101" s="91"/>
+      <c r="K101" s="91"/>
+      <c r="L101" s="92"/>
     </row>
     <row r="102" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="87" t="s">
+      <c r="A102" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="B102" s="88"/>
-      <c r="C102" s="88"/>
-      <c r="D102" s="110"/>
+      <c r="B102" s="79"/>
+      <c r="C102" s="79"/>
+      <c r="D102" s="81"/>
       <c r="E102" s="14"/>
       <c r="F102" s="3"/>
-      <c r="G102" s="132"/>
-      <c r="H102" s="122"/>
-      <c r="I102" s="122"/>
-      <c r="J102" s="122"/>
-      <c r="K102" s="122"/>
-      <c r="L102" s="133"/>
+      <c r="G102" s="93"/>
+      <c r="H102" s="94"/>
+      <c r="I102" s="94"/>
+      <c r="J102" s="94"/>
+      <c r="K102" s="94"/>
+      <c r="L102" s="95"/>
     </row>
     <row r="103" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F103" s="3"/>
     </row>
     <row r="104" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A104" s="112" t="s">
+      <c r="A104" s="100" t="s">
         <v>7</v>
       </c>
-      <c r="B104" s="113"/>
-      <c r="C104" s="113"/>
-      <c r="D104" s="113"/>
-      <c r="E104" s="114"/>
+      <c r="B104" s="101"/>
+      <c r="C104" s="101"/>
+      <c r="D104" s="101"/>
+      <c r="E104" s="102"/>
       <c r="F104" s="3"/>
     </row>
     <row r="105" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="115" t="s">
-        <v>45</v>
-      </c>
-      <c r="B105" s="116"/>
-      <c r="C105" s="41" t="s">
-        <v>109</v>
-      </c>
-      <c r="D105" s="41" t="s">
+      <c r="A105" s="103" t="s">
+        <v>43</v>
+      </c>
+      <c r="B105" s="104"/>
+      <c r="C105" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="D105" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="E105" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="E105" s="47" t="s">
-        <v>48</v>
-      </c>
       <c r="F105" s="3"/>
     </row>
     <row r="106" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="108"/>
-      <c r="B106" s="109"/>
-      <c r="C106" s="28"/>
-      <c r="D106" s="28"/>
-      <c r="E106" s="29"/>
+      <c r="A106" s="105"/>
+      <c r="B106" s="106"/>
+      <c r="C106" s="27"/>
+      <c r="D106" s="27"/>
+      <c r="E106" s="28"/>
       <c r="F106" s="3"/>
     </row>
     <row r="107" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="83"/>
-      <c r="B107" s="84"/>
+      <c r="A107" s="56"/>
+      <c r="B107" s="57"/>
       <c r="C107" s="22"/>
       <c r="D107" s="22"/>
-      <c r="E107" s="30"/>
+      <c r="E107" s="29"/>
       <c r="F107" s="3"/>
     </row>
     <row r="108" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="83"/>
-      <c r="B108" s="84"/>
-      <c r="C108" s="28"/>
-      <c r="D108" s="28"/>
-      <c r="E108" s="29"/>
+      <c r="A108" s="56"/>
+      <c r="B108" s="57"/>
+      <c r="C108" s="27"/>
+      <c r="D108" s="27"/>
+      <c r="E108" s="28"/>
       <c r="F108" s="3"/>
     </row>
     <row r="109" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="83"/>
-      <c r="B109" s="84"/>
+      <c r="A109" s="56"/>
+      <c r="B109" s="57"/>
       <c r="C109" s="22"/>
       <c r="D109" s="22"/>
-      <c r="E109" s="30"/>
+      <c r="E109" s="29"/>
       <c r="F109" s="3"/>
     </row>
     <row r="110" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="83"/>
-      <c r="B110" s="84"/>
-      <c r="C110" s="28"/>
-      <c r="D110" s="28"/>
-      <c r="E110" s="29"/>
+      <c r="A110" s="56"/>
+      <c r="B110" s="57"/>
+      <c r="C110" s="27"/>
+      <c r="D110" s="27"/>
+      <c r="E110" s="28"/>
       <c r="F110" s="3"/>
     </row>
     <row r="111" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="83"/>
-      <c r="B111" s="84"/>
+      <c r="A111" s="56"/>
+      <c r="B111" s="57"/>
       <c r="C111" s="22"/>
       <c r="D111" s="22"/>
-      <c r="E111" s="30"/>
+      <c r="E111" s="29"/>
       <c r="F111" s="3"/>
     </row>
     <row r="112" spans="1:12" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="83"/>
-      <c r="B112" s="84"/>
-      <c r="C112" s="28"/>
-      <c r="D112" s="28"/>
-      <c r="E112" s="29"/>
+      <c r="A112" s="56"/>
+      <c r="B112" s="57"/>
+      <c r="C112" s="27"/>
+      <c r="D112" s="27"/>
+      <c r="E112" s="28"/>
       <c r="F112" s="3"/>
     </row>
     <row r="113" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="83"/>
-      <c r="B113" s="84"/>
+      <c r="A113" s="56"/>
+      <c r="B113" s="57"/>
       <c r="C113" s="22"/>
       <c r="D113" s="22"/>
-      <c r="E113" s="30"/>
+      <c r="E113" s="29"/>
       <c r="F113" s="3"/>
     </row>
     <row r="114" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="83"/>
-      <c r="B114" s="84"/>
+      <c r="A114" s="56"/>
+      <c r="B114" s="57"/>
       <c r="C114" s="22"/>
       <c r="D114" s="22"/>
-      <c r="E114" s="29"/>
+      <c r="E114" s="28"/>
       <c r="F114" s="3"/>
     </row>
     <row r="115" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="83"/>
-      <c r="B115" s="84"/>
+      <c r="A115" s="56"/>
+      <c r="B115" s="57"/>
       <c r="C115" s="22"/>
       <c r="D115" s="22"/>
-      <c r="E115" s="30"/>
+      <c r="E115" s="29"/>
       <c r="F115" s="3"/>
     </row>
     <row r="116" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="83"/>
-      <c r="B116" s="84"/>
+      <c r="A116" s="56"/>
+      <c r="B116" s="57"/>
       <c r="C116" s="22"/>
       <c r="D116" s="22"/>
-      <c r="E116" s="29"/>
+      <c r="E116" s="28"/>
       <c r="F116" s="3"/>
     </row>
     <row r="117" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="83"/>
-      <c r="B117" s="84"/>
+      <c r="A117" s="56"/>
+      <c r="B117" s="57"/>
       <c r="C117" s="22"/>
       <c r="D117" s="22"/>
-      <c r="E117" s="30"/>
+      <c r="E117" s="29"/>
       <c r="F117" s="3"/>
     </row>
     <row r="118" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="83"/>
-      <c r="B118" s="84"/>
+      <c r="A118" s="56"/>
+      <c r="B118" s="57"/>
       <c r="C118" s="22"/>
       <c r="D118" s="22"/>
-      <c r="E118" s="29"/>
+      <c r="E118" s="28"/>
       <c r="F118" s="3"/>
     </row>
     <row r="119" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="83"/>
-      <c r="B119" s="84"/>
+      <c r="A119" s="56"/>
+      <c r="B119" s="57"/>
       <c r="C119" s="22"/>
       <c r="D119" s="22"/>
-      <c r="E119" s="30"/>
+      <c r="E119" s="29"/>
       <c r="F119" s="3"/>
     </row>
     <row r="120" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="83"/>
-      <c r="B120" s="84"/>
+      <c r="A120" s="56"/>
+      <c r="B120" s="57"/>
       <c r="C120" s="22"/>
       <c r="D120" s="22"/>
-      <c r="E120" s="30"/>
+      <c r="E120" s="29"/>
       <c r="F120" s="3"/>
     </row>
     <row r="121" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="83"/>
-      <c r="B121" s="84"/>
+      <c r="A121" s="56"/>
+      <c r="B121" s="57"/>
       <c r="C121" s="22"/>
       <c r="D121" s="22"/>
-      <c r="E121" s="30"/>
+      <c r="E121" s="29"/>
       <c r="F121" s="3"/>
     </row>
     <row r="122" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="83"/>
-      <c r="B122" s="84"/>
+      <c r="A122" s="56"/>
+      <c r="B122" s="57"/>
       <c r="C122" s="22"/>
       <c r="D122" s="22"/>
-      <c r="E122" s="30"/>
+      <c r="E122" s="29"/>
       <c r="F122" s="3"/>
     </row>
     <row r="123" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A123" s="83"/>
-      <c r="B123" s="84"/>
+      <c r="A123" s="56"/>
+      <c r="B123" s="57"/>
       <c r="C123" s="22"/>
       <c r="D123" s="22"/>
-      <c r="E123" s="30"/>
+      <c r="E123" s="29"/>
       <c r="F123" s="3"/>
     </row>
     <row r="124" spans="1:6" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A124" s="87" t="s">
-        <v>114</v>
-      </c>
-      <c r="B124" s="88"/>
-      <c r="C124" s="88"/>
-      <c r="D124" s="110"/>
+      <c r="A124" s="78" t="s">
+        <v>112</v>
+      </c>
+      <c r="B124" s="79"/>
+      <c r="C124" s="79"/>
+      <c r="D124" s="81"/>
       <c r="E124" s="14"/>
       <c r="F124" s="3"/>
     </row>
@@ -4699,53 +4757,109 @@
       <c r="E219" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="187">
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A116:B116"/>
-    <mergeCell ref="A117:B117"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="A80:D80"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="A57:E57"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A77:D77"/>
-    <mergeCell ref="A78:D78"/>
-    <mergeCell ref="A79:D79"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="A114:B114"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="G59:H59"/>
-    <mergeCell ref="G60:H60"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="G71:H71"/>
-    <mergeCell ref="G72:H72"/>
-    <mergeCell ref="G73:H73"/>
-    <mergeCell ref="G74:H74"/>
-    <mergeCell ref="G75:H75"/>
-    <mergeCell ref="A64:C64"/>
-    <mergeCell ref="G66:H66"/>
-    <mergeCell ref="G67:H67"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="G69:H69"/>
-    <mergeCell ref="A102:D102"/>
-    <mergeCell ref="A68:E68"/>
-    <mergeCell ref="G86:H86"/>
-    <mergeCell ref="G99:L102"/>
-    <mergeCell ref="G98:L98"/>
+  <mergeCells count="170">
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G41:L41"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="G63:H63"/>
+    <mergeCell ref="G64:H64"/>
+    <mergeCell ref="G65:H65"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="G1:L1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="A53:C53"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="A46:E46"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="A82:E82"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="A73:D73"/>
+    <mergeCell ref="G61:H61"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="G70:H70"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="G49:H49"/>
     <mergeCell ref="G54:H54"/>
     <mergeCell ref="A97:B97"/>
     <mergeCell ref="A124:D124"/>
@@ -4770,123 +4884,50 @@
     <mergeCell ref="B65:C65"/>
     <mergeCell ref="D65:E65"/>
     <mergeCell ref="A94:B94"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="A73:D73"/>
-    <mergeCell ref="G61:H61"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="G52:H52"/>
-    <mergeCell ref="G70:H70"/>
-    <mergeCell ref="G53:H53"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="A53:C53"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="G57:H57"/>
-    <mergeCell ref="A46:E46"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="A82:E82"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="G59:H59"/>
+    <mergeCell ref="G60:H60"/>
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="G71:H71"/>
+    <mergeCell ref="G72:H72"/>
+    <mergeCell ref="G73:H73"/>
+    <mergeCell ref="G74:H74"/>
+    <mergeCell ref="G75:H75"/>
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="G67:H67"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="G69:H69"/>
+    <mergeCell ref="A102:D102"/>
+    <mergeCell ref="A68:E68"/>
+    <mergeCell ref="G86:H86"/>
+    <mergeCell ref="G99:L102"/>
+    <mergeCell ref="G98:L98"/>
     <mergeCell ref="G77:L77"/>
-    <mergeCell ref="G41:L41"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="G63:H63"/>
-    <mergeCell ref="G64:H64"/>
-    <mergeCell ref="G65:H65"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="G1:L1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A116:B116"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="A80:D80"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A57:E57"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A77:D77"/>
+    <mergeCell ref="A78:D78"/>
+    <mergeCell ref="A79:D79"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="A114:B114"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>